<commit_message>
updated source file path for zl
</commit_message>
<xml_diff>
--- a/data/Phenotypes Variable List.xlsx
+++ b/data/Phenotypes Variable List.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10211"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{0AF53CB1-23E0-45A0-9003-9470A819876D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5361779F-7B5A-654E-B4E8-ADF7E5C9719D}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{0AF53CB1-23E0-45A0-9003-9470A819876D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CFACD291-CF87-4A4F-AC32-E92B33A41309}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="29340" windowHeight="17180" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="29340" windowHeight="17180" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Harmonized" sheetId="2" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1828" uniqueCount="984">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1829" uniqueCount="985">
   <si>
     <t>harmonized</t>
   </si>
@@ -3384,6 +3384,9 @@
   </si>
   <si>
     <t>whtsup</t>
+  </si>
+  <si>
+    <t>chma</t>
   </si>
 </sst>
 </file>
@@ -3686,6 +3689,10 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -4294,10 +4301,10 @@
   <dimension ref="A1:D163"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A40" sqref="A40"/>
+      <selection pane="bottomRight" activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8703,13 +8710,13 @@
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A1:B38"/>
+  <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="170" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B7" sqref="B7"/>
+      <selection pane="bottomRight" activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8718,15 +8725,18 @@
     <col min="2" max="2" width="14.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>124</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D1" t="s">
+        <v>984</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -8735,7 +8745,7 @@
         <v>id</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -8744,7 +8754,7 @@
         <v>study_id</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>51</v>
       </c>
@@ -8753,7 +8763,7 @@
         <v>dmduration</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>52</v>
       </c>
@@ -8762,7 +8772,7 @@
         <v>dmagediag</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -8771,7 +8781,7 @@
         <v>age</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>64</v>
       </c>
@@ -8780,7 +8790,7 @@
         <v>female</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>67</v>
       </c>
@@ -8789,7 +8799,7 @@
         <v>race</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>68</v>
       </c>
@@ -8798,7 +8808,7 @@
         <v>ethnicity</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>53</v>
       </c>
@@ -8807,7 +8817,7 @@
         <v>alcohol</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>54</v>
       </c>
@@ -8816,7 +8826,7 @@
         <v>smoking</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>55</v>
       </c>
@@ -8825,7 +8835,7 @@
         <v>dmfamilyhistory</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -8834,7 +8844,7 @@
         <v>height</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -8843,7 +8853,7 @@
         <v>weight</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>11</v>
       </c>
@@ -8852,7 +8862,7 @@
         <v>bmi</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>48</v>
       </c>
@@ -9111,8 +9121,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{824997C4-ECFA-43DC-9501-1C6C5C097BCA}">
   <dimension ref="A1:U90"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C30" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="E30" sqref="E30"/>
@@ -10346,7 +10356,7 @@
   <dimension ref="A1:V87"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="E30" sqref="E30"/>
       <selection pane="topRight" activeCell="E30" sqref="E30"/>
       <selection pane="bottomLeft" activeCell="E30" sqref="E30"/>
@@ -11520,11 +11530,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55874760-86AA-41EB-A2D6-050D3575AF4D}">
   <dimension ref="A1:X47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A5" sqref="A5:XFD5"/>
+      <selection pane="bottomRight" activeCell="A10" sqref="A10:XFD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -12322,7 +12332,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C46" sqref="C46"/>
+      <selection pane="bottomRight" activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
ARIC data extract file updated
</commit_message>
<xml_diff>
--- a/data/Phenotypes Variable List.xlsx
+++ b/data/Phenotypes Variable List.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10211"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="889" documentId="13_ncr:1_{0AF53CB1-23E0-45A0-9003-9470A819876D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3B447FB5-E9FC-9541-9916-3E1D364061FB}"/>
+  <xr:revisionPtr revIDLastSave="891" documentId="13_ncr:1_{0AF53CB1-23E0-45A0-9003-9470A819876D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A55A2EA9-1F1A-E745-87F6-ACAF7C80B15D}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17740" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20" yWindow="760" windowWidth="22920" windowHeight="17740" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Harmonized" sheetId="2" r:id="rId1"/>
@@ -10258,16 +10258,16 @@
   <dimension ref="A1:BE157"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="170" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="AR2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="AE22" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AV58" sqref="AV58"/>
+      <selection pane="bottomRight" activeCell="A32" sqref="A32:XFD32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="28.6640625" customWidth="1"/>
-    <col min="2" max="2" width="19.83203125" customWidth="1"/>
+    <col min="1" max="1" width="22.83203125" customWidth="1"/>
+    <col min="2" max="2" width="15" customWidth="1"/>
     <col min="3" max="3" width="2.5" style="8" customWidth="1"/>
     <col min="4" max="4" width="9" customWidth="1"/>
     <col min="5" max="6" width="9.83203125" customWidth="1"/>

</xml_diff>

<commit_message>
analysis updates-RF and NMF
</commit_message>
<xml_diff>
--- a/data/Phenotypes Variable List.xlsx
+++ b/data/Phenotypes Variable List.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10414"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="2205" documentId="13_ncr:1_{0AF53CB1-23E0-45A0-9003-9470A819876D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AFF5340A-4DBB-BE4C-9D73-6906A8833AD3}"/>
+  <xr:revisionPtr revIDLastSave="2217" documentId="13_ncr:1_{0AF53CB1-23E0-45A0-9003-9470A819876D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D812EE87-D0FD-734C-B189-F25E376AE60A}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17680" firstSheet="1" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1700" yWindow="760" windowWidth="30240" windowHeight="17680" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Harmonized" sheetId="2" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3412" uniqueCount="2247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3418" uniqueCount="2250">
   <si>
     <t>harmonized</t>
   </si>
@@ -7164,6 +7164,15 @@
   </si>
   <si>
     <t>mesaexam2dm_drepos_20220301</t>
+  </si>
+  <si>
+    <t>ULAB</t>
+  </si>
+  <si>
+    <t>UCRE</t>
+  </si>
+  <si>
+    <t>CHOLESTEROL</t>
   </si>
 </sst>
 </file>
@@ -7397,6 +7406,9 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -7406,7 +7418,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -8203,9 +8214,9 @@
   </sheetPr>
   <dimension ref="A1:M76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="207" workbookViewId="0">
+    <sheetView topLeftCell="A20" zoomScale="207" workbookViewId="0">
       <pane xSplit="2" topLeftCell="I1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A44" sqref="A44"/>
+      <selection pane="topRight" activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -8243,7 +8254,7 @@
       <c r="F1" t="s">
         <v>2077</v>
       </c>
-      <c r="G1" s="30" t="s">
+      <c r="G1" t="s">
         <v>2246</v>
       </c>
       <c r="H1" s="23" t="s">
@@ -13006,7 +13017,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="G14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" sqref="A1:B38"/>
+      <selection pane="bottomRight" activeCell="G43" sqref="G43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -13103,15 +13114,15 @@
       <c r="L3" t="s">
         <v>125</v>
       </c>
-      <c r="O3" s="27" t="s">
+      <c r="O3" s="28" t="s">
         <v>310</v>
       </c>
-      <c r="P3" s="27"/>
-      <c r="Q3" s="27"/>
-      <c r="R3" s="27"/>
-      <c r="S3" s="27"/>
-      <c r="T3" s="27"/>
-      <c r="U3" s="27"/>
+      <c r="P3" s="28"/>
+      <c r="Q3" s="28"/>
+      <c r="R3" s="28"/>
+      <c r="S3" s="28"/>
+      <c r="T3" s="28"/>
+      <c r="U3" s="28"/>
     </row>
     <row r="4" spans="1:21">
       <c r="A4" t="s">
@@ -13124,13 +13135,13 @@
       <c r="C4" t="s">
         <v>338</v>
       </c>
-      <c r="O4" s="27"/>
-      <c r="P4" s="27"/>
-      <c r="Q4" s="27"/>
-      <c r="R4" s="27"/>
-      <c r="S4" s="27"/>
-      <c r="T4" s="27"/>
-      <c r="U4" s="27"/>
+      <c r="O4" s="28"/>
+      <c r="P4" s="28"/>
+      <c r="Q4" s="28"/>
+      <c r="R4" s="28"/>
+      <c r="S4" s="28"/>
+      <c r="T4" s="28"/>
+      <c r="U4" s="28"/>
     </row>
     <row r="5" spans="1:21">
       <c r="A5" t="s">
@@ -13140,13 +13151,13 @@
         <f>INDEX(Harmonized!B:B,MATCH(A5,Harmonized!A:A,0))</f>
         <v>dmagediag</v>
       </c>
-      <c r="O5" s="27"/>
-      <c r="P5" s="27"/>
-      <c r="Q5" s="27"/>
-      <c r="R5" s="27"/>
-      <c r="S5" s="27"/>
-      <c r="T5" s="27"/>
-      <c r="U5" s="27"/>
+      <c r="O5" s="28"/>
+      <c r="P5" s="28"/>
+      <c r="Q5" s="28"/>
+      <c r="R5" s="28"/>
+      <c r="S5" s="28"/>
+      <c r="T5" s="28"/>
+      <c r="U5" s="28"/>
     </row>
     <row r="6" spans="1:21">
       <c r="A6" t="s">
@@ -13156,13 +13167,13 @@
         <f>INDEX(Harmonized!B:B,MATCH(A6,Harmonized!A:A,0))</f>
         <v>age</v>
       </c>
-      <c r="O6" s="27"/>
-      <c r="P6" s="27"/>
-      <c r="Q6" s="27"/>
-      <c r="R6" s="27"/>
-      <c r="S6" s="27"/>
-      <c r="T6" s="27"/>
-      <c r="U6" s="27"/>
+      <c r="O6" s="28"/>
+      <c r="P6" s="28"/>
+      <c r="Q6" s="28"/>
+      <c r="R6" s="28"/>
+      <c r="S6" s="28"/>
+      <c r="T6" s="28"/>
+      <c r="U6" s="28"/>
     </row>
     <row r="7" spans="1:21">
       <c r="A7" t="s">
@@ -13175,13 +13186,13 @@
       <c r="G7" t="s">
         <v>65</v>
       </c>
-      <c r="O7" s="27"/>
-      <c r="P7" s="27"/>
-      <c r="Q7" s="27"/>
-      <c r="R7" s="27"/>
-      <c r="S7" s="27"/>
-      <c r="T7" s="27"/>
-      <c r="U7" s="27"/>
+      <c r="O7" s="28"/>
+      <c r="P7" s="28"/>
+      <c r="Q7" s="28"/>
+      <c r="R7" s="28"/>
+      <c r="S7" s="28"/>
+      <c r="T7" s="28"/>
+      <c r="U7" s="28"/>
     </row>
     <row r="8" spans="1:21">
       <c r="A8" t="s">
@@ -13191,13 +13202,13 @@
         <f>INDEX(Harmonized!B:B,MATCH(A8,Harmonized!A:A,0))</f>
         <v>race</v>
       </c>
-      <c r="O8" s="27"/>
-      <c r="P8" s="27"/>
-      <c r="Q8" s="27"/>
-      <c r="R8" s="27"/>
-      <c r="S8" s="27"/>
-      <c r="T8" s="27"/>
-      <c r="U8" s="27"/>
+      <c r="O8" s="28"/>
+      <c r="P8" s="28"/>
+      <c r="Q8" s="28"/>
+      <c r="R8" s="28"/>
+      <c r="S8" s="28"/>
+      <c r="T8" s="28"/>
+      <c r="U8" s="28"/>
     </row>
     <row r="9" spans="1:21">
       <c r="A9" t="s">
@@ -13207,13 +13218,13 @@
         <f>INDEX(Harmonized!B:B,MATCH(A9,Harmonized!A:A,0))</f>
         <v>ethnicity</v>
       </c>
-      <c r="O9" s="27"/>
-      <c r="P9" s="27"/>
-      <c r="Q9" s="27"/>
-      <c r="R9" s="27"/>
-      <c r="S9" s="27"/>
-      <c r="T9" s="27"/>
-      <c r="U9" s="27"/>
+      <c r="O9" s="28"/>
+      <c r="P9" s="28"/>
+      <c r="Q9" s="28"/>
+      <c r="R9" s="28"/>
+      <c r="S9" s="28"/>
+      <c r="T9" s="28"/>
+      <c r="U9" s="28"/>
     </row>
     <row r="10" spans="1:21">
       <c r="A10" t="s">
@@ -13226,13 +13237,13 @@
       <c r="C10" t="s">
         <v>57</v>
       </c>
-      <c r="O10" s="27"/>
-      <c r="P10" s="27"/>
-      <c r="Q10" s="27"/>
-      <c r="R10" s="27"/>
-      <c r="S10" s="27"/>
-      <c r="T10" s="27"/>
-      <c r="U10" s="27"/>
+      <c r="O10" s="28"/>
+      <c r="P10" s="28"/>
+      <c r="Q10" s="28"/>
+      <c r="R10" s="28"/>
+      <c r="S10" s="28"/>
+      <c r="T10" s="28"/>
+      <c r="U10" s="28"/>
     </row>
     <row r="11" spans="1:21">
       <c r="A11" t="s">
@@ -13245,13 +13256,13 @@
       <c r="C11" s="3" t="s">
         <v>339</v>
       </c>
-      <c r="O11" s="27"/>
-      <c r="P11" s="27"/>
-      <c r="Q11" s="27"/>
-      <c r="R11" s="27"/>
-      <c r="S11" s="27"/>
-      <c r="T11" s="27"/>
-      <c r="U11" s="27"/>
+      <c r="O11" s="28"/>
+      <c r="P11" s="28"/>
+      <c r="Q11" s="28"/>
+      <c r="R11" s="28"/>
+      <c r="S11" s="28"/>
+      <c r="T11" s="28"/>
+      <c r="U11" s="28"/>
     </row>
     <row r="12" spans="1:21">
       <c r="A12" t="s">
@@ -13261,13 +13272,13 @@
         <f>INDEX(Harmonized!B:B,MATCH(A12,Harmonized!A:A,0))</f>
         <v>dmfamilyhistory</v>
       </c>
-      <c r="O12" s="27"/>
-      <c r="P12" s="27"/>
-      <c r="Q12" s="27"/>
-      <c r="R12" s="27"/>
-      <c r="S12" s="27"/>
-      <c r="T12" s="27"/>
-      <c r="U12" s="27"/>
+      <c r="O12" s="28"/>
+      <c r="P12" s="28"/>
+      <c r="Q12" s="28"/>
+      <c r="R12" s="28"/>
+      <c r="S12" s="28"/>
+      <c r="T12" s="28"/>
+      <c r="U12" s="28"/>
     </row>
     <row r="13" spans="1:21">
       <c r="A13" t="s">
@@ -13280,13 +13291,13 @@
       <c r="C13" t="s">
         <v>340</v>
       </c>
-      <c r="O13" s="27"/>
-      <c r="P13" s="27"/>
-      <c r="Q13" s="27"/>
-      <c r="R13" s="27"/>
-      <c r="S13" s="27"/>
-      <c r="T13" s="27"/>
-      <c r="U13" s="27"/>
+      <c r="O13" s="28"/>
+      <c r="P13" s="28"/>
+      <c r="Q13" s="28"/>
+      <c r="R13" s="28"/>
+      <c r="S13" s="28"/>
+      <c r="T13" s="28"/>
+      <c r="U13" s="28"/>
     </row>
     <row r="14" spans="1:21">
       <c r="A14" t="s">
@@ -13299,13 +13310,13 @@
       <c r="C14" t="s">
         <v>341</v>
       </c>
-      <c r="O14" s="27"/>
-      <c r="P14" s="27"/>
-      <c r="Q14" s="27"/>
-      <c r="R14" s="27"/>
-      <c r="S14" s="27"/>
-      <c r="T14" s="27"/>
-      <c r="U14" s="27"/>
+      <c r="O14" s="28"/>
+      <c r="P14" s="28"/>
+      <c r="Q14" s="28"/>
+      <c r="R14" s="28"/>
+      <c r="S14" s="28"/>
+      <c r="T14" s="28"/>
+      <c r="U14" s="28"/>
     </row>
     <row r="15" spans="1:21">
       <c r="A15" t="s">
@@ -13315,13 +13326,13 @@
         <f>INDEX(Harmonized!B:B,MATCH(A15,Harmonized!A:A,0))</f>
         <v>bmi</v>
       </c>
-      <c r="O15" s="27"/>
-      <c r="P15" s="27"/>
-      <c r="Q15" s="27"/>
-      <c r="R15" s="27"/>
-      <c r="S15" s="27"/>
-      <c r="T15" s="27"/>
-      <c r="U15" s="27"/>
+      <c r="O15" s="28"/>
+      <c r="P15" s="28"/>
+      <c r="Q15" s="28"/>
+      <c r="R15" s="28"/>
+      <c r="S15" s="28"/>
+      <c r="T15" s="28"/>
+      <c r="U15" s="28"/>
     </row>
     <row r="16" spans="1:21">
       <c r="A16" t="s">
@@ -13337,13 +13348,13 @@
       <c r="H16" t="s">
         <v>59</v>
       </c>
-      <c r="O16" s="27"/>
-      <c r="P16" s="27"/>
-      <c r="Q16" s="27"/>
-      <c r="R16" s="27"/>
-      <c r="S16" s="27"/>
-      <c r="T16" s="27"/>
-      <c r="U16" s="27"/>
+      <c r="O16" s="28"/>
+      <c r="P16" s="28"/>
+      <c r="Q16" s="28"/>
+      <c r="R16" s="28"/>
+      <c r="S16" s="28"/>
+      <c r="T16" s="28"/>
+      <c r="U16" s="28"/>
     </row>
     <row r="17" spans="1:21">
       <c r="A17" t="s">
@@ -13359,13 +13370,13 @@
       <c r="H17" t="s">
         <v>60</v>
       </c>
-      <c r="O17" s="27"/>
-      <c r="P17" s="27"/>
-      <c r="Q17" s="27"/>
-      <c r="R17" s="27"/>
-      <c r="S17" s="27"/>
-      <c r="T17" s="27"/>
-      <c r="U17" s="27"/>
+      <c r="O17" s="28"/>
+      <c r="P17" s="28"/>
+      <c r="Q17" s="28"/>
+      <c r="R17" s="28"/>
+      <c r="S17" s="28"/>
+      <c r="T17" s="28"/>
+      <c r="U17" s="28"/>
     </row>
     <row r="18" spans="1:21">
       <c r="A18" t="s">
@@ -13378,13 +13389,13 @@
       <c r="C18" t="s">
         <v>342</v>
       </c>
-      <c r="O18" s="27"/>
-      <c r="P18" s="27"/>
-      <c r="Q18" s="27"/>
-      <c r="R18" s="27"/>
-      <c r="S18" s="27"/>
-      <c r="T18" s="27"/>
-      <c r="U18" s="27"/>
+      <c r="O18" s="28"/>
+      <c r="P18" s="28"/>
+      <c r="Q18" s="28"/>
+      <c r="R18" s="28"/>
+      <c r="S18" s="28"/>
+      <c r="T18" s="28"/>
+      <c r="U18" s="28"/>
     </row>
     <row r="19" spans="1:21">
       <c r="A19" t="s">
@@ -13397,13 +13408,13 @@
       <c r="J19" t="s">
         <v>34</v>
       </c>
-      <c r="O19" s="27"/>
-      <c r="P19" s="27"/>
-      <c r="Q19" s="27"/>
-      <c r="R19" s="27"/>
-      <c r="S19" s="27"/>
-      <c r="T19" s="27"/>
-      <c r="U19" s="27"/>
+      <c r="O19" s="28"/>
+      <c r="P19" s="28"/>
+      <c r="Q19" s="28"/>
+      <c r="R19" s="28"/>
+      <c r="S19" s="28"/>
+      <c r="T19" s="28"/>
+      <c r="U19" s="28"/>
     </row>
     <row r="20" spans="1:21">
       <c r="A20" t="s">
@@ -13413,13 +13424,13 @@
         <f>INDEX(Harmonized!B:B,MATCH(A20,Harmonized!A:A,0))</f>
         <v>insulinf</v>
       </c>
-      <c r="O20" s="27"/>
-      <c r="P20" s="27"/>
-      <c r="Q20" s="27"/>
-      <c r="R20" s="27"/>
-      <c r="S20" s="27"/>
-      <c r="T20" s="27"/>
-      <c r="U20" s="27"/>
+      <c r="O20" s="28"/>
+      <c r="P20" s="28"/>
+      <c r="Q20" s="28"/>
+      <c r="R20" s="28"/>
+      <c r="S20" s="28"/>
+      <c r="T20" s="28"/>
+      <c r="U20" s="28"/>
     </row>
     <row r="21" spans="1:21">
       <c r="A21" t="s">
@@ -13429,13 +13440,13 @@
         <f>INDEX(Harmonized!B:B,MATCH(A21,Harmonized!A:A,0))</f>
         <v>cpeptidef</v>
       </c>
-      <c r="O21" s="27"/>
-      <c r="P21" s="27"/>
-      <c r="Q21" s="27"/>
-      <c r="R21" s="27"/>
-      <c r="S21" s="27"/>
-      <c r="T21" s="27"/>
-      <c r="U21" s="27"/>
+      <c r="O21" s="28"/>
+      <c r="P21" s="28"/>
+      <c r="Q21" s="28"/>
+      <c r="R21" s="28"/>
+      <c r="S21" s="28"/>
+      <c r="T21" s="28"/>
+      <c r="U21" s="28"/>
     </row>
     <row r="22" spans="1:21">
       <c r="A22" t="s">
@@ -13448,13 +13459,13 @@
       <c r="L22" t="s">
         <v>321</v>
       </c>
-      <c r="O22" s="27"/>
-      <c r="P22" s="27"/>
-      <c r="Q22" s="27"/>
-      <c r="R22" s="27"/>
-      <c r="S22" s="27"/>
-      <c r="T22" s="27"/>
-      <c r="U22" s="27"/>
+      <c r="O22" s="28"/>
+      <c r="P22" s="28"/>
+      <c r="Q22" s="28"/>
+      <c r="R22" s="28"/>
+      <c r="S22" s="28"/>
+      <c r="T22" s="28"/>
+      <c r="U22" s="28"/>
     </row>
     <row r="23" spans="1:21">
       <c r="A23" t="s">
@@ -13792,10 +13803,10 @@
   <dimension ref="A1:BE165"/>
   <sheetViews>
     <sheetView zoomScale="125" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C79" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="AM17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A105" sqref="A105"/>
+      <selection pane="bottomRight" activeCell="A33" sqref="A33:XFD33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -20245,13 +20256,13 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{824997C4-ECFA-43DC-9501-1C6C5C097BCA}">
-  <dimension ref="A1:U90"/>
+  <dimension ref="A1:U91"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C33" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C18" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H69" sqref="H69"/>
+      <selection pane="bottomRight" activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -20295,18 +20306,18 @@
         <f>INDEX(Harmonized!B:B,MATCH(A2,Harmonized!A:A,0))</f>
         <v>id</v>
       </c>
-      <c r="L2" s="28" t="s">
+      <c r="L2" s="29" t="s">
         <v>136</v>
       </c>
-      <c r="M2" s="28"/>
-      <c r="N2" s="28"/>
-      <c r="O2" s="28"/>
-      <c r="P2" s="28"/>
-      <c r="Q2" s="28"/>
-      <c r="R2" s="28"/>
-      <c r="S2" s="28"/>
-      <c r="T2" s="28"/>
-      <c r="U2" s="28"/>
+      <c r="M2" s="29"/>
+      <c r="N2" s="29"/>
+      <c r="O2" s="29"/>
+      <c r="P2" s="29"/>
+      <c r="Q2" s="29"/>
+      <c r="R2" s="29"/>
+      <c r="S2" s="29"/>
+      <c r="T2" s="29"/>
+      <c r="U2" s="29"/>
     </row>
     <row r="3" spans="1:21">
       <c r="A3" t="s">
@@ -20334,16 +20345,16 @@
       <c r="H3" t="s">
         <v>138</v>
       </c>
-      <c r="L3" s="28"/>
-      <c r="M3" s="28"/>
-      <c r="N3" s="28"/>
-      <c r="O3" s="28"/>
-      <c r="P3" s="28"/>
-      <c r="Q3" s="28"/>
-      <c r="R3" s="28"/>
-      <c r="S3" s="28"/>
-      <c r="T3" s="28"/>
-      <c r="U3" s="28"/>
+      <c r="L3" s="29"/>
+      <c r="M3" s="29"/>
+      <c r="N3" s="29"/>
+      <c r="O3" s="29"/>
+      <c r="P3" s="29"/>
+      <c r="Q3" s="29"/>
+      <c r="R3" s="29"/>
+      <c r="S3" s="29"/>
+      <c r="T3" s="29"/>
+      <c r="U3" s="29"/>
     </row>
     <row r="4" spans="1:21">
       <c r="A4" t="s">
@@ -20353,16 +20364,16 @@
         <f>INDEX(Harmonized!B:B,MATCH(A4,Harmonized!A:A,0))</f>
         <v>dmduration</v>
       </c>
-      <c r="L4" s="28"/>
-      <c r="M4" s="28"/>
-      <c r="N4" s="28"/>
-      <c r="O4" s="28"/>
-      <c r="P4" s="28"/>
-      <c r="Q4" s="28"/>
-      <c r="R4" s="28"/>
-      <c r="S4" s="28"/>
-      <c r="T4" s="28"/>
-      <c r="U4" s="28"/>
+      <c r="L4" s="29"/>
+      <c r="M4" s="29"/>
+      <c r="N4" s="29"/>
+      <c r="O4" s="29"/>
+      <c r="P4" s="29"/>
+      <c r="Q4" s="29"/>
+      <c r="R4" s="29"/>
+      <c r="S4" s="29"/>
+      <c r="T4" s="29"/>
+      <c r="U4" s="29"/>
     </row>
     <row r="5" spans="1:21">
       <c r="A5" t="s">
@@ -20373,16 +20384,16 @@
         <v>dmagediag</v>
       </c>
       <c r="G5" s="3"/>
-      <c r="L5" s="28"/>
-      <c r="M5" s="28"/>
-      <c r="N5" s="28"/>
-      <c r="O5" s="28"/>
-      <c r="P5" s="28"/>
-      <c r="Q5" s="28"/>
-      <c r="R5" s="28"/>
-      <c r="S5" s="28"/>
-      <c r="T5" s="28"/>
-      <c r="U5" s="28"/>
+      <c r="L5" s="29"/>
+      <c r="M5" s="29"/>
+      <c r="N5" s="29"/>
+      <c r="O5" s="29"/>
+      <c r="P5" s="29"/>
+      <c r="Q5" s="29"/>
+      <c r="R5" s="29"/>
+      <c r="S5" s="29"/>
+      <c r="T5" s="29"/>
+      <c r="U5" s="29"/>
     </row>
     <row r="6" spans="1:21">
       <c r="A6" t="s">
@@ -20392,16 +20403,16 @@
         <f>INDEX(Harmonized!B:B,MATCH(A6,Harmonized!A:A,0))</f>
         <v>age</v>
       </c>
-      <c r="L6" s="28"/>
-      <c r="M6" s="28"/>
-      <c r="N6" s="28"/>
-      <c r="O6" s="28"/>
-      <c r="P6" s="28"/>
-      <c r="Q6" s="28"/>
-      <c r="R6" s="28"/>
-      <c r="S6" s="28"/>
-      <c r="T6" s="28"/>
-      <c r="U6" s="28"/>
+      <c r="L6" s="29"/>
+      <c r="M6" s="29"/>
+      <c r="N6" s="29"/>
+      <c r="O6" s="29"/>
+      <c r="P6" s="29"/>
+      <c r="Q6" s="29"/>
+      <c r="R6" s="29"/>
+      <c r="S6" s="29"/>
+      <c r="T6" s="29"/>
+      <c r="U6" s="29"/>
     </row>
     <row r="7" spans="1:21">
       <c r="A7" t="s">
@@ -20411,16 +20422,16 @@
         <f>INDEX(Harmonized!B:B,MATCH(A7,Harmonized!A:A,0))</f>
         <v>female</v>
       </c>
-      <c r="L7" s="28"/>
-      <c r="M7" s="28"/>
-      <c r="N7" s="28"/>
-      <c r="O7" s="28"/>
-      <c r="P7" s="28"/>
-      <c r="Q7" s="28"/>
-      <c r="R7" s="28"/>
-      <c r="S7" s="28"/>
-      <c r="T7" s="28"/>
-      <c r="U7" s="28"/>
+      <c r="L7" s="29"/>
+      <c r="M7" s="29"/>
+      <c r="N7" s="29"/>
+      <c r="O7" s="29"/>
+      <c r="P7" s="29"/>
+      <c r="Q7" s="29"/>
+      <c r="R7" s="29"/>
+      <c r="S7" s="29"/>
+      <c r="T7" s="29"/>
+      <c r="U7" s="29"/>
     </row>
     <row r="8" spans="1:21">
       <c r="A8" t="s">
@@ -20430,16 +20441,16 @@
         <f>INDEX(Harmonized!B:B,MATCH(A8,Harmonized!A:A,0))</f>
         <v>race</v>
       </c>
-      <c r="L8" s="28"/>
-      <c r="M8" s="28"/>
-      <c r="N8" s="28"/>
-      <c r="O8" s="28"/>
-      <c r="P8" s="28"/>
-      <c r="Q8" s="28"/>
-      <c r="R8" s="28"/>
-      <c r="S8" s="28"/>
-      <c r="T8" s="28"/>
-      <c r="U8" s="28"/>
+      <c r="L8" s="29"/>
+      <c r="M8" s="29"/>
+      <c r="N8" s="29"/>
+      <c r="O8" s="29"/>
+      <c r="P8" s="29"/>
+      <c r="Q8" s="29"/>
+      <c r="R8" s="29"/>
+      <c r="S8" s="29"/>
+      <c r="T8" s="29"/>
+      <c r="U8" s="29"/>
     </row>
     <row r="9" spans="1:21">
       <c r="A9" t="s">
@@ -20449,16 +20460,16 @@
         <f>INDEX(Harmonized!B:B,MATCH(A9,Harmonized!A:A,0))</f>
         <v>ethnicity</v>
       </c>
-      <c r="L9" s="28"/>
-      <c r="M9" s="28"/>
-      <c r="N9" s="28"/>
-      <c r="O9" s="28"/>
-      <c r="P9" s="28"/>
-      <c r="Q9" s="28"/>
-      <c r="R9" s="28"/>
-      <c r="S9" s="28"/>
-      <c r="T9" s="28"/>
-      <c r="U9" s="28"/>
+      <c r="L9" s="29"/>
+      <c r="M9" s="29"/>
+      <c r="N9" s="29"/>
+      <c r="O9" s="29"/>
+      <c r="P9" s="29"/>
+      <c r="Q9" s="29"/>
+      <c r="R9" s="29"/>
+      <c r="S9" s="29"/>
+      <c r="T9" s="29"/>
+      <c r="U9" s="29"/>
     </row>
     <row r="10" spans="1:21">
       <c r="A10" t="s">
@@ -20468,16 +20479,16 @@
         <f>INDEX(Harmonized!B:B,MATCH(A10,Harmonized!A:A,0))</f>
         <v>alcohol</v>
       </c>
-      <c r="L10" s="28"/>
-      <c r="M10" s="28"/>
-      <c r="N10" s="28"/>
-      <c r="O10" s="28"/>
-      <c r="P10" s="28"/>
-      <c r="Q10" s="28"/>
-      <c r="R10" s="28"/>
-      <c r="S10" s="28"/>
-      <c r="T10" s="28"/>
-      <c r="U10" s="28"/>
+      <c r="L10" s="29"/>
+      <c r="M10" s="29"/>
+      <c r="N10" s="29"/>
+      <c r="O10" s="29"/>
+      <c r="P10" s="29"/>
+      <c r="Q10" s="29"/>
+      <c r="R10" s="29"/>
+      <c r="S10" s="29"/>
+      <c r="T10" s="29"/>
+      <c r="U10" s="29"/>
     </row>
     <row r="11" spans="1:21">
       <c r="A11" t="s">
@@ -20487,16 +20498,16 @@
         <f>INDEX(Harmonized!B:B,MATCH(A11,Harmonized!A:A,0))</f>
         <v>smoking</v>
       </c>
-      <c r="L11" s="28"/>
-      <c r="M11" s="28"/>
-      <c r="N11" s="28"/>
-      <c r="O11" s="28"/>
-      <c r="P11" s="28"/>
-      <c r="Q11" s="28"/>
-      <c r="R11" s="28"/>
-      <c r="S11" s="28"/>
-      <c r="T11" s="28"/>
-      <c r="U11" s="28"/>
+      <c r="L11" s="29"/>
+      <c r="M11" s="29"/>
+      <c r="N11" s="29"/>
+      <c r="O11" s="29"/>
+      <c r="P11" s="29"/>
+      <c r="Q11" s="29"/>
+      <c r="R11" s="29"/>
+      <c r="S11" s="29"/>
+      <c r="T11" s="29"/>
+      <c r="U11" s="29"/>
     </row>
     <row r="12" spans="1:21">
       <c r="A12" t="s">
@@ -20506,16 +20517,16 @@
         <f>INDEX(Harmonized!B:B,MATCH(A12,Harmonized!A:A,0))</f>
         <v>dmfamilyhistory</v>
       </c>
-      <c r="L12" s="28"/>
-      <c r="M12" s="28"/>
-      <c r="N12" s="28"/>
-      <c r="O12" s="28"/>
-      <c r="P12" s="28"/>
-      <c r="Q12" s="28"/>
-      <c r="R12" s="28"/>
-      <c r="S12" s="28"/>
-      <c r="T12" s="28"/>
-      <c r="U12" s="28"/>
+      <c r="L12" s="29"/>
+      <c r="M12" s="29"/>
+      <c r="N12" s="29"/>
+      <c r="O12" s="29"/>
+      <c r="P12" s="29"/>
+      <c r="Q12" s="29"/>
+      <c r="R12" s="29"/>
+      <c r="S12" s="29"/>
+      <c r="T12" s="29"/>
+      <c r="U12" s="29"/>
     </row>
     <row r="13" spans="1:21">
       <c r="A13" t="s">
@@ -20525,16 +20536,16 @@
         <f>INDEX(Harmonized!B:B,MATCH(A13,Harmonized!A:A,0))</f>
         <v>height</v>
       </c>
-      <c r="L13" s="28"/>
-      <c r="M13" s="28"/>
-      <c r="N13" s="28"/>
-      <c r="O13" s="28"/>
-      <c r="P13" s="28"/>
-      <c r="Q13" s="28"/>
-      <c r="R13" s="28"/>
-      <c r="S13" s="28"/>
-      <c r="T13" s="28"/>
-      <c r="U13" s="28"/>
+      <c r="L13" s="29"/>
+      <c r="M13" s="29"/>
+      <c r="N13" s="29"/>
+      <c r="O13" s="29"/>
+      <c r="P13" s="29"/>
+      <c r="Q13" s="29"/>
+      <c r="R13" s="29"/>
+      <c r="S13" s="29"/>
+      <c r="T13" s="29"/>
+      <c r="U13" s="29"/>
     </row>
     <row r="14" spans="1:21">
       <c r="A14" t="s">
@@ -20544,16 +20555,16 @@
         <f>INDEX(Harmonized!B:B,MATCH(A14,Harmonized!A:A,0))</f>
         <v>weight</v>
       </c>
-      <c r="L14" s="28"/>
-      <c r="M14" s="28"/>
-      <c r="N14" s="28"/>
-      <c r="O14" s="28"/>
-      <c r="P14" s="28"/>
-      <c r="Q14" s="28"/>
-      <c r="R14" s="28"/>
-      <c r="S14" s="28"/>
-      <c r="T14" s="28"/>
-      <c r="U14" s="28"/>
+      <c r="L14" s="29"/>
+      <c r="M14" s="29"/>
+      <c r="N14" s="29"/>
+      <c r="O14" s="29"/>
+      <c r="P14" s="29"/>
+      <c r="Q14" s="29"/>
+      <c r="R14" s="29"/>
+      <c r="S14" s="29"/>
+      <c r="T14" s="29"/>
+      <c r="U14" s="29"/>
     </row>
     <row r="15" spans="1:21">
       <c r="A15" t="s">
@@ -20563,16 +20574,16 @@
         <f>INDEX(Harmonized!B:B,MATCH(A15,Harmonized!A:A,0))</f>
         <v>bmi</v>
       </c>
-      <c r="L15" s="28"/>
-      <c r="M15" s="28"/>
-      <c r="N15" s="28"/>
-      <c r="O15" s="28"/>
-      <c r="P15" s="28"/>
-      <c r="Q15" s="28"/>
-      <c r="R15" s="28"/>
-      <c r="S15" s="28"/>
-      <c r="T15" s="28"/>
-      <c r="U15" s="28"/>
+      <c r="L15" s="29"/>
+      <c r="M15" s="29"/>
+      <c r="N15" s="29"/>
+      <c r="O15" s="29"/>
+      <c r="P15" s="29"/>
+      <c r="Q15" s="29"/>
+      <c r="R15" s="29"/>
+      <c r="S15" s="29"/>
+      <c r="T15" s="29"/>
+      <c r="U15" s="29"/>
     </row>
     <row r="16" spans="1:21">
       <c r="A16" t="s">
@@ -20582,16 +20593,16 @@
         <f>INDEX(Harmonized!B:B,MATCH(A16,Harmonized!A:A,0))</f>
         <v>sbp</v>
       </c>
-      <c r="L16" s="28"/>
-      <c r="M16" s="28"/>
-      <c r="N16" s="28"/>
-      <c r="O16" s="28"/>
-      <c r="P16" s="28"/>
-      <c r="Q16" s="28"/>
-      <c r="R16" s="28"/>
-      <c r="S16" s="28"/>
-      <c r="T16" s="28"/>
-      <c r="U16" s="28"/>
+      <c r="L16" s="29"/>
+      <c r="M16" s="29"/>
+      <c r="N16" s="29"/>
+      <c r="O16" s="29"/>
+      <c r="P16" s="29"/>
+      <c r="Q16" s="29"/>
+      <c r="R16" s="29"/>
+      <c r="S16" s="29"/>
+      <c r="T16" s="29"/>
+      <c r="U16" s="29"/>
     </row>
     <row r="17" spans="1:21">
       <c r="A17" t="s">
@@ -20601,16 +20612,16 @@
         <f>INDEX(Harmonized!B:B,MATCH(A17,Harmonized!A:A,0))</f>
         <v>dbp</v>
       </c>
-      <c r="L17" s="28"/>
-      <c r="M17" s="28"/>
-      <c r="N17" s="28"/>
-      <c r="O17" s="28"/>
-      <c r="P17" s="28"/>
-      <c r="Q17" s="28"/>
-      <c r="R17" s="28"/>
-      <c r="S17" s="28"/>
-      <c r="T17" s="28"/>
-      <c r="U17" s="28"/>
+      <c r="L17" s="29"/>
+      <c r="M17" s="29"/>
+      <c r="N17" s="29"/>
+      <c r="O17" s="29"/>
+      <c r="P17" s="29"/>
+      <c r="Q17" s="29"/>
+      <c r="R17" s="29"/>
+      <c r="S17" s="29"/>
+      <c r="T17" s="29"/>
+      <c r="U17" s="29"/>
     </row>
     <row r="18" spans="1:21">
       <c r="A18" t="s">
@@ -20620,16 +20631,16 @@
         <f>INDEX(Harmonized!B:B,MATCH(A18,Harmonized!A:A,0))</f>
         <v>wc</v>
       </c>
-      <c r="L18" s="28"/>
-      <c r="M18" s="28"/>
-      <c r="N18" s="28"/>
-      <c r="O18" s="28"/>
-      <c r="P18" s="28"/>
-      <c r="Q18" s="28"/>
-      <c r="R18" s="28"/>
-      <c r="S18" s="28"/>
-      <c r="T18" s="28"/>
-      <c r="U18" s="28"/>
+      <c r="L18" s="29"/>
+      <c r="M18" s="29"/>
+      <c r="N18" s="29"/>
+      <c r="O18" s="29"/>
+      <c r="P18" s="29"/>
+      <c r="Q18" s="29"/>
+      <c r="R18" s="29"/>
+      <c r="S18" s="29"/>
+      <c r="T18" s="29"/>
+      <c r="U18" s="29"/>
     </row>
     <row r="19" spans="1:21">
       <c r="A19" t="s">
@@ -20642,16 +20653,16 @@
       <c r="E19" t="s">
         <v>141</v>
       </c>
-      <c r="L19" s="28"/>
-      <c r="M19" s="28"/>
-      <c r="N19" s="28"/>
-      <c r="O19" s="28"/>
-      <c r="P19" s="28"/>
-      <c r="Q19" s="28"/>
-      <c r="R19" s="28"/>
-      <c r="S19" s="28"/>
-      <c r="T19" s="28"/>
-      <c r="U19" s="28"/>
+      <c r="L19" s="29"/>
+      <c r="M19" s="29"/>
+      <c r="N19" s="29"/>
+      <c r="O19" s="29"/>
+      <c r="P19" s="29"/>
+      <c r="Q19" s="29"/>
+      <c r="R19" s="29"/>
+      <c r="S19" s="29"/>
+      <c r="T19" s="29"/>
+      <c r="U19" s="29"/>
     </row>
     <row r="20" spans="1:21">
       <c r="A20" t="s">
@@ -20664,16 +20675,16 @@
       <c r="E20" t="s">
         <v>148</v>
       </c>
-      <c r="L20" s="28"/>
-      <c r="M20" s="28"/>
-      <c r="N20" s="28"/>
-      <c r="O20" s="28"/>
-      <c r="P20" s="28"/>
-      <c r="Q20" s="28"/>
-      <c r="R20" s="28"/>
-      <c r="S20" s="28"/>
-      <c r="T20" s="28"/>
-      <c r="U20" s="28"/>
+      <c r="L20" s="29"/>
+      <c r="M20" s="29"/>
+      <c r="N20" s="29"/>
+      <c r="O20" s="29"/>
+      <c r="P20" s="29"/>
+      <c r="Q20" s="29"/>
+      <c r="R20" s="29"/>
+      <c r="S20" s="29"/>
+      <c r="T20" s="29"/>
+      <c r="U20" s="29"/>
     </row>
     <row r="21" spans="1:21">
       <c r="A21" t="s">
@@ -20683,16 +20694,16 @@
         <f>INDEX(Harmonized!B:B,MATCH(A21,Harmonized!A:A,0))</f>
         <v>cpeptidef</v>
       </c>
-      <c r="L21" s="28"/>
-      <c r="M21" s="28"/>
-      <c r="N21" s="28"/>
-      <c r="O21" s="28"/>
-      <c r="P21" s="28"/>
-      <c r="Q21" s="28"/>
-      <c r="R21" s="28"/>
-      <c r="S21" s="28"/>
-      <c r="T21" s="28"/>
-      <c r="U21" s="28"/>
+      <c r="L21" s="29"/>
+      <c r="M21" s="29"/>
+      <c r="N21" s="29"/>
+      <c r="O21" s="29"/>
+      <c r="P21" s="29"/>
+      <c r="Q21" s="29"/>
+      <c r="R21" s="29"/>
+      <c r="S21" s="29"/>
+      <c r="T21" s="29"/>
+      <c r="U21" s="29"/>
     </row>
     <row r="22" spans="1:21">
       <c r="A22" t="s">
@@ -20705,16 +20716,16 @@
       <c r="E22" t="s">
         <v>146</v>
       </c>
-      <c r="L22" s="28"/>
-      <c r="M22" s="28"/>
-      <c r="N22" s="28"/>
-      <c r="O22" s="28"/>
-      <c r="P22" s="28"/>
-      <c r="Q22" s="28"/>
-      <c r="R22" s="28"/>
-      <c r="S22" s="28"/>
-      <c r="T22" s="28"/>
-      <c r="U22" s="28"/>
+      <c r="L22" s="29"/>
+      <c r="M22" s="29"/>
+      <c r="N22" s="29"/>
+      <c r="O22" s="29"/>
+      <c r="P22" s="29"/>
+      <c r="Q22" s="29"/>
+      <c r="R22" s="29"/>
+      <c r="S22" s="29"/>
+      <c r="T22" s="29"/>
+      <c r="U22" s="29"/>
     </row>
     <row r="23" spans="1:21">
       <c r="A23" t="s">
@@ -20724,16 +20735,16 @@
         <f>INDEX(Harmonized!B:B,MATCH(A23,Harmonized!A:A,0))</f>
         <v>glucoser</v>
       </c>
-      <c r="L23" s="28"/>
-      <c r="M23" s="28"/>
-      <c r="N23" s="28"/>
-      <c r="O23" s="28"/>
-      <c r="P23" s="28"/>
-      <c r="Q23" s="28"/>
-      <c r="R23" s="28"/>
-      <c r="S23" s="28"/>
-      <c r="T23" s="28"/>
-      <c r="U23" s="28"/>
+      <c r="L23" s="29"/>
+      <c r="M23" s="29"/>
+      <c r="N23" s="29"/>
+      <c r="O23" s="29"/>
+      <c r="P23" s="29"/>
+      <c r="Q23" s="29"/>
+      <c r="R23" s="29"/>
+      <c r="S23" s="29"/>
+      <c r="T23" s="29"/>
+      <c r="U23" s="29"/>
     </row>
     <row r="24" spans="1:21">
       <c r="A24" t="s">
@@ -20746,16 +20757,16 @@
       <c r="E24" t="s">
         <v>147</v>
       </c>
-      <c r="L24" s="28"/>
-      <c r="M24" s="28"/>
-      <c r="N24" s="28"/>
-      <c r="O24" s="28"/>
-      <c r="P24" s="28"/>
-      <c r="Q24" s="28"/>
-      <c r="R24" s="28"/>
-      <c r="S24" s="28"/>
-      <c r="T24" s="28"/>
-      <c r="U24" s="28"/>
+      <c r="L24" s="29"/>
+      <c r="M24" s="29"/>
+      <c r="N24" s="29"/>
+      <c r="O24" s="29"/>
+      <c r="P24" s="29"/>
+      <c r="Q24" s="29"/>
+      <c r="R24" s="29"/>
+      <c r="S24" s="29"/>
+      <c r="T24" s="29"/>
+      <c r="U24" s="29"/>
     </row>
     <row r="25" spans="1:21">
       <c r="A25" t="s">
@@ -20765,16 +20776,16 @@
         <f>INDEX(Harmonized!B:B,MATCH(A25,Harmonized!A:A,0))</f>
         <v>homab</v>
       </c>
-      <c r="L25" s="28"/>
-      <c r="M25" s="28"/>
-      <c r="N25" s="28"/>
-      <c r="O25" s="28"/>
-      <c r="P25" s="28"/>
-      <c r="Q25" s="28"/>
-      <c r="R25" s="28"/>
-      <c r="S25" s="28"/>
-      <c r="T25" s="28"/>
-      <c r="U25" s="28"/>
+      <c r="L25" s="29"/>
+      <c r="M25" s="29"/>
+      <c r="N25" s="29"/>
+      <c r="O25" s="29"/>
+      <c r="P25" s="29"/>
+      <c r="Q25" s="29"/>
+      <c r="R25" s="29"/>
+      <c r="S25" s="29"/>
+      <c r="T25" s="29"/>
+      <c r="U25" s="29"/>
     </row>
     <row r="26" spans="1:21">
       <c r="A26" t="s">
@@ -20784,688 +20795,734 @@
         <f>INDEX(Harmonized!B:B,MATCH(A26,Harmonized!A:A,0))</f>
         <v>homair</v>
       </c>
-      <c r="L26" s="28"/>
-      <c r="M26" s="28"/>
-      <c r="N26" s="28"/>
-      <c r="O26" s="28"/>
-      <c r="P26" s="28"/>
-      <c r="Q26" s="28"/>
-      <c r="R26" s="28"/>
-      <c r="S26" s="28"/>
-      <c r="T26" s="28"/>
-      <c r="U26" s="28"/>
+      <c r="L26" s="29"/>
+      <c r="M26" s="29"/>
+      <c r="N26" s="29"/>
+      <c r="O26" s="29"/>
+      <c r="P26" s="29"/>
+      <c r="Q26" s="29"/>
+      <c r="R26" s="29"/>
+      <c r="S26" s="29"/>
+      <c r="T26" s="29"/>
+      <c r="U26" s="29"/>
     </row>
     <row r="27" spans="1:21">
       <c r="A27" t="s">
-        <v>20</v>
+        <v>142</v>
       </c>
       <c r="B27" t="str">
         <f>INDEX(Harmonized!B:B,MATCH(A27,Harmonized!A:A,0))</f>
-        <v>ldlc</v>
+        <v>totalc</v>
       </c>
       <c r="E27" t="s">
-        <v>300</v>
-      </c>
+        <v>2249</v>
+      </c>
+      <c r="L27" s="27"/>
+      <c r="M27" s="27"/>
+      <c r="N27" s="27"/>
+      <c r="O27" s="27"/>
+      <c r="P27" s="27"/>
+      <c r="Q27" s="27"/>
+      <c r="R27" s="27"/>
+      <c r="S27" s="27"/>
+      <c r="T27" s="27"/>
+      <c r="U27" s="27"/>
     </row>
     <row r="28" spans="1:21">
       <c r="A28" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B28" t="str">
         <f>INDEX(Harmonized!B:B,MATCH(A28,Harmonized!A:A,0))</f>
-        <v>hdlc</v>
+        <v>ldlc</v>
       </c>
       <c r="E28" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="29" spans="1:21">
       <c r="A29" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B29" t="str">
         <f>INDEX(Harmonized!B:B,MATCH(A29,Harmonized!A:A,0))</f>
-        <v>vldlc</v>
+        <v>hdlc</v>
       </c>
       <c r="E29" t="s">
-        <v>81</v>
+        <v>301</v>
       </c>
     </row>
     <row r="30" spans="1:21">
       <c r="A30" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B30" t="str">
         <f>INDEX(Harmonized!B:B,MATCH(A30,Harmonized!A:A,0))</f>
-        <v>tgl</v>
+        <v>vldlc</v>
       </c>
       <c r="E30" t="s">
-        <v>145</v>
+        <v>81</v>
       </c>
     </row>
     <row r="31" spans="1:21">
       <c r="A31" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B31" t="str">
         <f>INDEX(Harmonized!B:B,MATCH(A31,Harmonized!A:A,0))</f>
-        <v>serumcreatinine</v>
+        <v>tgl</v>
       </c>
       <c r="E31" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
     </row>
     <row r="32" spans="1:21">
       <c r="A32" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B32" t="str">
         <f>INDEX(Harmonized!B:B,MATCH(A32,Harmonized!A:A,0))</f>
-        <v>urinealbumin</v>
+        <v>serumcreatinine</v>
+      </c>
+      <c r="E32" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="33" spans="1:8">
       <c r="A33" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B33" t="str">
         <f>INDEX(Harmonized!B:B,MATCH(A33,Harmonized!A:A,0))</f>
-        <v>urinecreatinine</v>
+        <v>urinealbumin</v>
       </c>
       <c r="E33" t="s">
-        <v>183</v>
+        <v>2247</v>
       </c>
     </row>
     <row r="34" spans="1:8">
       <c r="A34" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B34" t="str">
         <f>INDEX(Harmonized!B:B,MATCH(A34,Harmonized!A:A,0))</f>
-        <v>uacr</v>
+        <v>urinecreatinine</v>
       </c>
       <c r="E34" t="s">
-        <v>184</v>
+        <v>2248</v>
       </c>
     </row>
     <row r="35" spans="1:8">
       <c r="A35" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B35" t="str">
         <f>INDEX(Harmonized!B:B,MATCH(A35,Harmonized!A:A,0))</f>
+        <v>uacr</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8">
+      <c r="A36" t="s">
+        <v>28</v>
+      </c>
+      <c r="B36" t="str">
+        <f>INDEX(Harmonized!B:B,MATCH(A36,Harmonized!A:A,0))</f>
         <v>egfr</v>
       </c>
     </row>
-    <row r="42" spans="1:8">
-      <c r="A42" s="2" t="s">
+    <row r="37" spans="1:8">
+      <c r="A37" t="s">
+        <v>179</v>
+      </c>
+      <c r="B37" t="str">
+        <f>INDEX(Harmonized!B:B,MATCH(A37,Harmonized!A:A,0))</f>
+        <v>ast</v>
+      </c>
+      <c r="E37" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8">
+      <c r="A38" t="s">
+        <v>180</v>
+      </c>
+      <c r="B38" t="str">
+        <f>INDEX(Harmonized!B:B,MATCH(A38,Harmonized!A:A,0))</f>
+        <v>alt</v>
+      </c>
+      <c r="E38" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8">
+      <c r="A43" s="2" t="s">
         <v>88</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8">
-      <c r="A43" t="s">
-        <v>89</v>
-      </c>
-      <c r="B43" t="s">
-        <v>90</v>
-      </c>
-      <c r="C43" t="s">
-        <v>137</v>
-      </c>
-      <c r="D43" t="s">
-        <v>137</v>
-      </c>
-      <c r="E43" t="s">
-        <v>137</v>
-      </c>
-      <c r="H43" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="44" spans="1:8">
       <c r="A44" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B44" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C44" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D44" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E44" t="s">
-        <v>139</v>
+        <v>137</v>
+      </c>
+      <c r="H44" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="45" spans="1:8">
       <c r="A45" t="s">
-        <v>167</v>
+        <v>91</v>
       </c>
       <c r="B45" t="s">
-        <v>171</v>
-      </c>
-      <c r="F45" s="3" t="s">
-        <v>149</v>
+        <v>92</v>
+      </c>
+      <c r="C45" t="s">
+        <v>139</v>
+      </c>
+      <c r="D45" t="s">
+        <v>139</v>
+      </c>
+      <c r="E45" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="46" spans="1:8">
       <c r="A46" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B46" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="47" spans="1:8">
       <c r="A47" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B47" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="48" spans="1:8">
       <c r="A48" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="B48" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="F48" s="3" t="s">
-        <v>174</v>
+        <v>150</v>
       </c>
     </row>
     <row r="49" spans="1:7">
       <c r="A49" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B49" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="50" spans="1:7">
       <c r="A50" t="s">
-        <v>153</v>
+        <v>178</v>
       </c>
       <c r="B50" t="s">
-        <v>155</v>
-      </c>
-      <c r="G50" t="s">
-        <v>154</v>
+        <v>173</v>
+      </c>
+      <c r="F50" s="3" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="51" spans="1:7">
       <c r="A51" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="B51" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="G51" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
     </row>
     <row r="52" spans="1:7">
       <c r="A52" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B52" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G52" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="53" spans="1:7">
       <c r="A53" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B53" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G53" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="54" spans="1:7">
       <c r="A54" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B54" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G54" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="55" spans="1:7">
       <c r="A55" t="s">
-        <v>190</v>
+        <v>159</v>
       </c>
       <c r="B55" t="s">
-        <v>205</v>
-      </c>
-      <c r="C55" t="s">
-        <v>199</v>
-      </c>
-      <c r="D55" t="s">
-        <v>212</v>
+        <v>166</v>
+      </c>
+      <c r="G55" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="56" spans="1:7">
       <c r="A56" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B56" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C56" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D56" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="57" spans="1:7">
       <c r="A57" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B57" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C57" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="D57" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="58" spans="1:7">
       <c r="A58" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B58" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C58" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D58" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="59" spans="1:7">
       <c r="A59" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B59" t="s">
-        <v>284</v>
+        <v>208</v>
       </c>
       <c r="C59" t="s">
-        <v>268</v>
+        <v>198</v>
       </c>
       <c r="D59" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
     </row>
     <row r="60" spans="1:7">
       <c r="A60" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B60" t="s">
-        <v>209</v>
+        <v>284</v>
       </c>
       <c r="C60" t="s">
-        <v>201</v>
+        <v>268</v>
       </c>
       <c r="D60" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
     </row>
     <row r="61" spans="1:7">
       <c r="A61" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B61" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C61" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D61" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="62" spans="1:7">
       <c r="A62" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="B62" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C62" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D62" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="63" spans="1:7">
       <c r="A63" t="s">
-        <v>220</v>
+        <v>203</v>
       </c>
       <c r="B63" t="s">
-        <v>221</v>
+        <v>211</v>
+      </c>
+      <c r="C63" t="s">
+        <v>204</v>
       </c>
       <c r="D63" t="s">
-        <v>226</v>
+        <v>218</v>
       </c>
     </row>
     <row r="64" spans="1:7">
       <c r="A64" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B64" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="D64" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="65" spans="1:4">
       <c r="A65" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B65" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D65" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="66" spans="1:4">
       <c r="A66" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="B66" t="s">
-        <v>235</v>
+        <v>225</v>
       </c>
       <c r="D66" t="s">
-        <v>250</v>
+        <v>228</v>
       </c>
     </row>
     <row r="67" spans="1:4">
       <c r="A67" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B67" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D67" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="68" spans="1:4">
       <c r="A68" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B68" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D68" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="69" spans="1:4">
       <c r="A69" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B69" t="s">
-        <v>269</v>
+        <v>237</v>
       </c>
       <c r="D69" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="70" spans="1:4">
       <c r="A70" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B70" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D70" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="71" spans="1:4">
       <c r="A71" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B71" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D71" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="72" spans="1:4">
       <c r="A72" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="B72" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D72" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="73" spans="1:4">
       <c r="A73" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B73" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D73" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="74" spans="1:4">
       <c r="A74" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B74" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D74" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="75" spans="1:4">
       <c r="A75" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B75" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D75" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="76" spans="1:4">
       <c r="A76" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B76" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D76" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="77" spans="1:4">
       <c r="A77" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B77" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D77" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="78" spans="1:4">
       <c r="A78" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B78" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D78" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="79" spans="1:4">
       <c r="A79" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B79" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D79" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="80" spans="1:4">
       <c r="A80" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B80" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D80" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="81" spans="1:8">
       <c r="A81" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B81" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D81" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="82" spans="1:8">
       <c r="A82" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B82" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D82" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="83" spans="1:8">
       <c r="A83" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B83" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D83" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="84" spans="1:8">
       <c r="A84" t="s">
-        <v>286</v>
+        <v>249</v>
       </c>
       <c r="B84" t="s">
-        <v>295</v>
-      </c>
-      <c r="H84" t="s">
-        <v>289</v>
+        <v>283</v>
+      </c>
+      <c r="D84" t="s">
+        <v>267</v>
       </c>
     </row>
     <row r="85" spans="1:8">
       <c r="A85" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B85" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="H85" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="86" spans="1:8">
       <c r="A86" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B86" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="H86" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="87" spans="1:8">
       <c r="A87" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="B87" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="H87" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="88" spans="1:8">
       <c r="A88" t="s">
-        <v>305</v>
+        <v>293</v>
       </c>
       <c r="B88" t="s">
-        <v>307</v>
-      </c>
-      <c r="F88" t="s">
-        <v>302</v>
+        <v>294</v>
+      </c>
+      <c r="H88" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="89" spans="1:8">
       <c r="A89" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="B89" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="F89" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="90" spans="1:8">
       <c r="A90" t="s">
+        <v>304</v>
+      </c>
+      <c r="B90" t="s">
+        <v>308</v>
+      </c>
+      <c r="F90" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8">
+      <c r="A91" t="s">
         <v>306</v>
       </c>
-      <c r="B90" t="s">
+      <c r="B91" t="s">
         <v>309</v>
       </c>
-      <c r="F90" t="s">
+      <c r="F91" t="s">
         <v>11</v>
       </c>
     </row>
@@ -21481,12 +21538,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72BEC307-7012-42C0-8F8D-AEA3F585C15F}">
   <dimension ref="A1:V87"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="150" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C12" activePane="bottomRight" state="frozen"/>
       <selection activeCell="E30" sqref="E30"/>
       <selection pane="topRight" activeCell="E30" sqref="E30"/>
       <selection pane="bottomLeft" activeCell="E30" sqref="E30"/>
-      <selection pane="bottomRight" activeCell="A22" sqref="A22:XFD22"/>
+      <selection pane="bottomRight" activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -21530,19 +21587,19 @@
         <f>INDEX(Harmonized!B:B,MATCH(A2,Harmonized!A:A,0))</f>
         <v>id</v>
       </c>
-      <c r="L2" s="28" t="s">
+      <c r="L2" s="29" t="s">
         <v>135</v>
       </c>
-      <c r="M2" s="28"/>
-      <c r="N2" s="28"/>
-      <c r="O2" s="28"/>
-      <c r="P2" s="28"/>
-      <c r="Q2" s="28"/>
-      <c r="R2" s="28"/>
-      <c r="S2" s="28"/>
-      <c r="T2" s="28"/>
-      <c r="U2" s="28"/>
-      <c r="V2" s="28"/>
+      <c r="M2" s="29"/>
+      <c r="N2" s="29"/>
+      <c r="O2" s="29"/>
+      <c r="P2" s="29"/>
+      <c r="Q2" s="29"/>
+      <c r="R2" s="29"/>
+      <c r="S2" s="29"/>
+      <c r="T2" s="29"/>
+      <c r="U2" s="29"/>
+      <c r="V2" s="29"/>
     </row>
     <row r="3" spans="1:22">
       <c r="A3" t="s">
@@ -21570,17 +21627,17 @@
       <c r="H3" t="s">
         <v>138</v>
       </c>
-      <c r="L3" s="28"/>
-      <c r="M3" s="28"/>
-      <c r="N3" s="28"/>
-      <c r="O3" s="28"/>
-      <c r="P3" s="28"/>
-      <c r="Q3" s="28"/>
-      <c r="R3" s="28"/>
-      <c r="S3" s="28"/>
-      <c r="T3" s="28"/>
-      <c r="U3" s="28"/>
-      <c r="V3" s="28"/>
+      <c r="L3" s="29"/>
+      <c r="M3" s="29"/>
+      <c r="N3" s="29"/>
+      <c r="O3" s="29"/>
+      <c r="P3" s="29"/>
+      <c r="Q3" s="29"/>
+      <c r="R3" s="29"/>
+      <c r="S3" s="29"/>
+      <c r="T3" s="29"/>
+      <c r="U3" s="29"/>
+      <c r="V3" s="29"/>
     </row>
     <row r="4" spans="1:22">
       <c r="A4" t="s">
@@ -21590,17 +21647,17 @@
         <f>INDEX(Harmonized!B:B,MATCH(A4,Harmonized!A:A,0))</f>
         <v>dmduration</v>
       </c>
-      <c r="L4" s="28"/>
-      <c r="M4" s="28"/>
-      <c r="N4" s="28"/>
-      <c r="O4" s="28"/>
-      <c r="P4" s="28"/>
-      <c r="Q4" s="28"/>
-      <c r="R4" s="28"/>
-      <c r="S4" s="28"/>
-      <c r="T4" s="28"/>
-      <c r="U4" s="28"/>
-      <c r="V4" s="28"/>
+      <c r="L4" s="29"/>
+      <c r="M4" s="29"/>
+      <c r="N4" s="29"/>
+      <c r="O4" s="29"/>
+      <c r="P4" s="29"/>
+      <c r="Q4" s="29"/>
+      <c r="R4" s="29"/>
+      <c r="S4" s="29"/>
+      <c r="T4" s="29"/>
+      <c r="U4" s="29"/>
+      <c r="V4" s="29"/>
     </row>
     <row r="5" spans="1:22">
       <c r="A5" t="s">
@@ -21611,17 +21668,17 @@
         <v>dmagediag</v>
       </c>
       <c r="G5" s="3"/>
-      <c r="L5" s="28"/>
-      <c r="M5" s="28"/>
-      <c r="N5" s="28"/>
-      <c r="O5" s="28"/>
-      <c r="P5" s="28"/>
-      <c r="Q5" s="28"/>
-      <c r="R5" s="28"/>
-      <c r="S5" s="28"/>
-      <c r="T5" s="28"/>
-      <c r="U5" s="28"/>
-      <c r="V5" s="28"/>
+      <c r="L5" s="29"/>
+      <c r="M5" s="29"/>
+      <c r="N5" s="29"/>
+      <c r="O5" s="29"/>
+      <c r="P5" s="29"/>
+      <c r="Q5" s="29"/>
+      <c r="R5" s="29"/>
+      <c r="S5" s="29"/>
+      <c r="T5" s="29"/>
+      <c r="U5" s="29"/>
+      <c r="V5" s="29"/>
     </row>
     <row r="6" spans="1:22">
       <c r="A6" t="s">
@@ -21631,17 +21688,17 @@
         <f>INDEX(Harmonized!B:B,MATCH(A6,Harmonized!A:A,0))</f>
         <v>age</v>
       </c>
-      <c r="L6" s="28"/>
-      <c r="M6" s="28"/>
-      <c r="N6" s="28"/>
-      <c r="O6" s="28"/>
-      <c r="P6" s="28"/>
-      <c r="Q6" s="28"/>
-      <c r="R6" s="28"/>
-      <c r="S6" s="28"/>
-      <c r="T6" s="28"/>
-      <c r="U6" s="28"/>
-      <c r="V6" s="28"/>
+      <c r="L6" s="29"/>
+      <c r="M6" s="29"/>
+      <c r="N6" s="29"/>
+      <c r="O6" s="29"/>
+      <c r="P6" s="29"/>
+      <c r="Q6" s="29"/>
+      <c r="R6" s="29"/>
+      <c r="S6" s="29"/>
+      <c r="T6" s="29"/>
+      <c r="U6" s="29"/>
+      <c r="V6" s="29"/>
     </row>
     <row r="7" spans="1:22">
       <c r="A7" t="s">
@@ -21651,17 +21708,17 @@
         <f>INDEX(Harmonized!B:B,MATCH(A7,Harmonized!A:A,0))</f>
         <v>female</v>
       </c>
-      <c r="L7" s="28"/>
-      <c r="M7" s="28"/>
-      <c r="N7" s="28"/>
-      <c r="O7" s="28"/>
-      <c r="P7" s="28"/>
-      <c r="Q7" s="28"/>
-      <c r="R7" s="28"/>
-      <c r="S7" s="28"/>
-      <c r="T7" s="28"/>
-      <c r="U7" s="28"/>
-      <c r="V7" s="28"/>
+      <c r="L7" s="29"/>
+      <c r="M7" s="29"/>
+      <c r="N7" s="29"/>
+      <c r="O7" s="29"/>
+      <c r="P7" s="29"/>
+      <c r="Q7" s="29"/>
+      <c r="R7" s="29"/>
+      <c r="S7" s="29"/>
+      <c r="T7" s="29"/>
+      <c r="U7" s="29"/>
+      <c r="V7" s="29"/>
     </row>
     <row r="8" spans="1:22">
       <c r="A8" t="s">
@@ -21671,17 +21728,17 @@
         <f>INDEX(Harmonized!B:B,MATCH(A8,Harmonized!A:A,0))</f>
         <v>race</v>
       </c>
-      <c r="L8" s="28"/>
-      <c r="M8" s="28"/>
-      <c r="N8" s="28"/>
-      <c r="O8" s="28"/>
-      <c r="P8" s="28"/>
-      <c r="Q8" s="28"/>
-      <c r="R8" s="28"/>
-      <c r="S8" s="28"/>
-      <c r="T8" s="28"/>
-      <c r="U8" s="28"/>
-      <c r="V8" s="28"/>
+      <c r="L8" s="29"/>
+      <c r="M8" s="29"/>
+      <c r="N8" s="29"/>
+      <c r="O8" s="29"/>
+      <c r="P8" s="29"/>
+      <c r="Q8" s="29"/>
+      <c r="R8" s="29"/>
+      <c r="S8" s="29"/>
+      <c r="T8" s="29"/>
+      <c r="U8" s="29"/>
+      <c r="V8" s="29"/>
     </row>
     <row r="9" spans="1:22">
       <c r="A9" t="s">
@@ -21691,17 +21748,17 @@
         <f>INDEX(Harmonized!B:B,MATCH(A9,Harmonized!A:A,0))</f>
         <v>ethnicity</v>
       </c>
-      <c r="L9" s="28"/>
-      <c r="M9" s="28"/>
-      <c r="N9" s="28"/>
-      <c r="O9" s="28"/>
-      <c r="P9" s="28"/>
-      <c r="Q9" s="28"/>
-      <c r="R9" s="28"/>
-      <c r="S9" s="28"/>
-      <c r="T9" s="28"/>
-      <c r="U9" s="28"/>
-      <c r="V9" s="28"/>
+      <c r="L9" s="29"/>
+      <c r="M9" s="29"/>
+      <c r="N9" s="29"/>
+      <c r="O9" s="29"/>
+      <c r="P9" s="29"/>
+      <c r="Q9" s="29"/>
+      <c r="R9" s="29"/>
+      <c r="S9" s="29"/>
+      <c r="T9" s="29"/>
+      <c r="U9" s="29"/>
+      <c r="V9" s="29"/>
     </row>
     <row r="10" spans="1:22">
       <c r="A10" t="s">
@@ -21711,17 +21768,17 @@
         <f>INDEX(Harmonized!B:B,MATCH(A10,Harmonized!A:A,0))</f>
         <v>alcohol</v>
       </c>
-      <c r="L10" s="28"/>
-      <c r="M10" s="28"/>
-      <c r="N10" s="28"/>
-      <c r="O10" s="28"/>
-      <c r="P10" s="28"/>
-      <c r="Q10" s="28"/>
-      <c r="R10" s="28"/>
-      <c r="S10" s="28"/>
-      <c r="T10" s="28"/>
-      <c r="U10" s="28"/>
-      <c r="V10" s="28"/>
+      <c r="L10" s="29"/>
+      <c r="M10" s="29"/>
+      <c r="N10" s="29"/>
+      <c r="O10" s="29"/>
+      <c r="P10" s="29"/>
+      <c r="Q10" s="29"/>
+      <c r="R10" s="29"/>
+      <c r="S10" s="29"/>
+      <c r="T10" s="29"/>
+      <c r="U10" s="29"/>
+      <c r="V10" s="29"/>
     </row>
     <row r="11" spans="1:22">
       <c r="A11" t="s">
@@ -21731,17 +21788,17 @@
         <f>INDEX(Harmonized!B:B,MATCH(A11,Harmonized!A:A,0))</f>
         <v>smoking</v>
       </c>
-      <c r="L11" s="28"/>
-      <c r="M11" s="28"/>
-      <c r="N11" s="28"/>
-      <c r="O11" s="28"/>
-      <c r="P11" s="28"/>
-      <c r="Q11" s="28"/>
-      <c r="R11" s="28"/>
-      <c r="S11" s="28"/>
-      <c r="T11" s="28"/>
-      <c r="U11" s="28"/>
-      <c r="V11" s="28"/>
+      <c r="L11" s="29"/>
+      <c r="M11" s="29"/>
+      <c r="N11" s="29"/>
+      <c r="O11" s="29"/>
+      <c r="P11" s="29"/>
+      <c r="Q11" s="29"/>
+      <c r="R11" s="29"/>
+      <c r="S11" s="29"/>
+      <c r="T11" s="29"/>
+      <c r="U11" s="29"/>
+      <c r="V11" s="29"/>
     </row>
     <row r="12" spans="1:22">
       <c r="A12" t="s">
@@ -21751,17 +21808,17 @@
         <f>INDEX(Harmonized!B:B,MATCH(A12,Harmonized!A:A,0))</f>
         <v>dmfamilyhistory</v>
       </c>
-      <c r="L12" s="28"/>
-      <c r="M12" s="28"/>
-      <c r="N12" s="28"/>
-      <c r="O12" s="28"/>
-      <c r="P12" s="28"/>
-      <c r="Q12" s="28"/>
-      <c r="R12" s="28"/>
-      <c r="S12" s="28"/>
-      <c r="T12" s="28"/>
-      <c r="U12" s="28"/>
-      <c r="V12" s="28"/>
+      <c r="L12" s="29"/>
+      <c r="M12" s="29"/>
+      <c r="N12" s="29"/>
+      <c r="O12" s="29"/>
+      <c r="P12" s="29"/>
+      <c r="Q12" s="29"/>
+      <c r="R12" s="29"/>
+      <c r="S12" s="29"/>
+      <c r="T12" s="29"/>
+      <c r="U12" s="29"/>
+      <c r="V12" s="29"/>
     </row>
     <row r="13" spans="1:22">
       <c r="A13" t="s">
@@ -21771,17 +21828,17 @@
         <f>INDEX(Harmonized!B:B,MATCH(A13,Harmonized!A:A,0))</f>
         <v>height</v>
       </c>
-      <c r="L13" s="28"/>
-      <c r="M13" s="28"/>
-      <c r="N13" s="28"/>
-      <c r="O13" s="28"/>
-      <c r="P13" s="28"/>
-      <c r="Q13" s="28"/>
-      <c r="R13" s="28"/>
-      <c r="S13" s="28"/>
-      <c r="T13" s="28"/>
-      <c r="U13" s="28"/>
-      <c r="V13" s="28"/>
+      <c r="L13" s="29"/>
+      <c r="M13" s="29"/>
+      <c r="N13" s="29"/>
+      <c r="O13" s="29"/>
+      <c r="P13" s="29"/>
+      <c r="Q13" s="29"/>
+      <c r="R13" s="29"/>
+      <c r="S13" s="29"/>
+      <c r="T13" s="29"/>
+      <c r="U13" s="29"/>
+      <c r="V13" s="29"/>
     </row>
     <row r="14" spans="1:22">
       <c r="A14" t="s">
@@ -21791,17 +21848,17 @@
         <f>INDEX(Harmonized!B:B,MATCH(A14,Harmonized!A:A,0))</f>
         <v>weight</v>
       </c>
-      <c r="L14" s="28"/>
-      <c r="M14" s="28"/>
-      <c r="N14" s="28"/>
-      <c r="O14" s="28"/>
-      <c r="P14" s="28"/>
-      <c r="Q14" s="28"/>
-      <c r="R14" s="28"/>
-      <c r="S14" s="28"/>
-      <c r="T14" s="28"/>
-      <c r="U14" s="28"/>
-      <c r="V14" s="28"/>
+      <c r="L14" s="29"/>
+      <c r="M14" s="29"/>
+      <c r="N14" s="29"/>
+      <c r="O14" s="29"/>
+      <c r="P14" s="29"/>
+      <c r="Q14" s="29"/>
+      <c r="R14" s="29"/>
+      <c r="S14" s="29"/>
+      <c r="T14" s="29"/>
+      <c r="U14" s="29"/>
+      <c r="V14" s="29"/>
     </row>
     <row r="15" spans="1:22">
       <c r="A15" t="s">
@@ -21811,17 +21868,17 @@
         <f>INDEX(Harmonized!B:B,MATCH(A15,Harmonized!A:A,0))</f>
         <v>bmi</v>
       </c>
-      <c r="L15" s="28"/>
-      <c r="M15" s="28"/>
-      <c r="N15" s="28"/>
-      <c r="O15" s="28"/>
-      <c r="P15" s="28"/>
-      <c r="Q15" s="28"/>
-      <c r="R15" s="28"/>
-      <c r="S15" s="28"/>
-      <c r="T15" s="28"/>
-      <c r="U15" s="28"/>
-      <c r="V15" s="28"/>
+      <c r="L15" s="29"/>
+      <c r="M15" s="29"/>
+      <c r="N15" s="29"/>
+      <c r="O15" s="29"/>
+      <c r="P15" s="29"/>
+      <c r="Q15" s="29"/>
+      <c r="R15" s="29"/>
+      <c r="S15" s="29"/>
+      <c r="T15" s="29"/>
+      <c r="U15" s="29"/>
+      <c r="V15" s="29"/>
     </row>
     <row r="16" spans="1:22">
       <c r="A16" t="s">
@@ -21831,17 +21888,17 @@
         <f>INDEX(Harmonized!B:B,MATCH(A16,Harmonized!A:A,0))</f>
         <v>sbp</v>
       </c>
-      <c r="L16" s="28"/>
-      <c r="M16" s="28"/>
-      <c r="N16" s="28"/>
-      <c r="O16" s="28"/>
-      <c r="P16" s="28"/>
-      <c r="Q16" s="28"/>
-      <c r="R16" s="28"/>
-      <c r="S16" s="28"/>
-      <c r="T16" s="28"/>
-      <c r="U16" s="28"/>
-      <c r="V16" s="28"/>
+      <c r="L16" s="29"/>
+      <c r="M16" s="29"/>
+      <c r="N16" s="29"/>
+      <c r="O16" s="29"/>
+      <c r="P16" s="29"/>
+      <c r="Q16" s="29"/>
+      <c r="R16" s="29"/>
+      <c r="S16" s="29"/>
+      <c r="T16" s="29"/>
+      <c r="U16" s="29"/>
+      <c r="V16" s="29"/>
     </row>
     <row r="17" spans="1:22">
       <c r="A17" t="s">
@@ -21851,17 +21908,17 @@
         <f>INDEX(Harmonized!B:B,MATCH(A17,Harmonized!A:A,0))</f>
         <v>dbp</v>
       </c>
-      <c r="L17" s="28"/>
-      <c r="M17" s="28"/>
-      <c r="N17" s="28"/>
-      <c r="O17" s="28"/>
-      <c r="P17" s="28"/>
-      <c r="Q17" s="28"/>
-      <c r="R17" s="28"/>
-      <c r="S17" s="28"/>
-      <c r="T17" s="28"/>
-      <c r="U17" s="28"/>
-      <c r="V17" s="28"/>
+      <c r="L17" s="29"/>
+      <c r="M17" s="29"/>
+      <c r="N17" s="29"/>
+      <c r="O17" s="29"/>
+      <c r="P17" s="29"/>
+      <c r="Q17" s="29"/>
+      <c r="R17" s="29"/>
+      <c r="S17" s="29"/>
+      <c r="T17" s="29"/>
+      <c r="U17" s="29"/>
+      <c r="V17" s="29"/>
     </row>
     <row r="18" spans="1:22">
       <c r="A18" t="s">
@@ -21871,17 +21928,17 @@
         <f>INDEX(Harmonized!B:B,MATCH(A18,Harmonized!A:A,0))</f>
         <v>wc</v>
       </c>
-      <c r="L18" s="28"/>
-      <c r="M18" s="28"/>
-      <c r="N18" s="28"/>
-      <c r="O18" s="28"/>
-      <c r="P18" s="28"/>
-      <c r="Q18" s="28"/>
-      <c r="R18" s="28"/>
-      <c r="S18" s="28"/>
-      <c r="T18" s="28"/>
-      <c r="U18" s="28"/>
-      <c r="V18" s="28"/>
+      <c r="L18" s="29"/>
+      <c r="M18" s="29"/>
+      <c r="N18" s="29"/>
+      <c r="O18" s="29"/>
+      <c r="P18" s="29"/>
+      <c r="Q18" s="29"/>
+      <c r="R18" s="29"/>
+      <c r="S18" s="29"/>
+      <c r="T18" s="29"/>
+      <c r="U18" s="29"/>
+      <c r="V18" s="29"/>
     </row>
     <row r="19" spans="1:22">
       <c r="A19" t="s">
@@ -21894,17 +21951,17 @@
       <c r="E19" t="s">
         <v>141</v>
       </c>
-      <c r="L19" s="28"/>
-      <c r="M19" s="28"/>
-      <c r="N19" s="28"/>
-      <c r="O19" s="28"/>
-      <c r="P19" s="28"/>
-      <c r="Q19" s="28"/>
-      <c r="R19" s="28"/>
-      <c r="S19" s="28"/>
-      <c r="T19" s="28"/>
-      <c r="U19" s="28"/>
-      <c r="V19" s="28"/>
+      <c r="L19" s="29"/>
+      <c r="M19" s="29"/>
+      <c r="N19" s="29"/>
+      <c r="O19" s="29"/>
+      <c r="P19" s="29"/>
+      <c r="Q19" s="29"/>
+      <c r="R19" s="29"/>
+      <c r="S19" s="29"/>
+      <c r="T19" s="29"/>
+      <c r="U19" s="29"/>
+      <c r="V19" s="29"/>
     </row>
     <row r="20" spans="1:22">
       <c r="A20" t="s">
@@ -21917,30 +21974,30 @@
       <c r="E20" t="s">
         <v>148</v>
       </c>
-      <c r="L20" s="28"/>
-      <c r="M20" s="28"/>
-      <c r="N20" s="28"/>
-      <c r="O20" s="28"/>
-      <c r="P20" s="28"/>
-      <c r="Q20" s="28"/>
-      <c r="R20" s="28"/>
-      <c r="S20" s="28"/>
-      <c r="T20" s="28"/>
-      <c r="U20" s="28"/>
-      <c r="V20" s="28"/>
+      <c r="L20" s="29"/>
+      <c r="M20" s="29"/>
+      <c r="N20" s="29"/>
+      <c r="O20" s="29"/>
+      <c r="P20" s="29"/>
+      <c r="Q20" s="29"/>
+      <c r="R20" s="29"/>
+      <c r="S20" s="29"/>
+      <c r="T20" s="29"/>
+      <c r="U20" s="29"/>
+      <c r="V20" s="29"/>
     </row>
     <row r="21" spans="1:22">
-      <c r="L21" s="28"/>
-      <c r="M21" s="28"/>
-      <c r="N21" s="28"/>
-      <c r="O21" s="28"/>
-      <c r="P21" s="28"/>
-      <c r="Q21" s="28"/>
-      <c r="R21" s="28"/>
-      <c r="S21" s="28"/>
-      <c r="T21" s="28"/>
-      <c r="U21" s="28"/>
-      <c r="V21" s="28"/>
+      <c r="L21" s="29"/>
+      <c r="M21" s="29"/>
+      <c r="N21" s="29"/>
+      <c r="O21" s="29"/>
+      <c r="P21" s="29"/>
+      <c r="Q21" s="29"/>
+      <c r="R21" s="29"/>
+      <c r="S21" s="29"/>
+      <c r="T21" s="29"/>
+      <c r="U21" s="29"/>
+      <c r="V21" s="29"/>
     </row>
     <row r="22" spans="1:22">
       <c r="A22" t="s">
@@ -21953,30 +22010,30 @@
       <c r="E22" t="s">
         <v>146</v>
       </c>
-      <c r="L22" s="28"/>
-      <c r="M22" s="28"/>
-      <c r="N22" s="28"/>
-      <c r="O22" s="28"/>
-      <c r="P22" s="28"/>
-      <c r="Q22" s="28"/>
-      <c r="R22" s="28"/>
-      <c r="S22" s="28"/>
-      <c r="T22" s="28"/>
-      <c r="U22" s="28"/>
-      <c r="V22" s="28"/>
+      <c r="L22" s="29"/>
+      <c r="M22" s="29"/>
+      <c r="N22" s="29"/>
+      <c r="O22" s="29"/>
+      <c r="P22" s="29"/>
+      <c r="Q22" s="29"/>
+      <c r="R22" s="29"/>
+      <c r="S22" s="29"/>
+      <c r="T22" s="29"/>
+      <c r="U22" s="29"/>
+      <c r="V22" s="29"/>
     </row>
     <row r="23" spans="1:22">
-      <c r="L23" s="28"/>
-      <c r="M23" s="28"/>
-      <c r="N23" s="28"/>
-      <c r="O23" s="28"/>
-      <c r="P23" s="28"/>
-      <c r="Q23" s="28"/>
-      <c r="R23" s="28"/>
-      <c r="S23" s="28"/>
-      <c r="T23" s="28"/>
-      <c r="U23" s="28"/>
-      <c r="V23" s="28"/>
+      <c r="L23" s="29"/>
+      <c r="M23" s="29"/>
+      <c r="N23" s="29"/>
+      <c r="O23" s="29"/>
+      <c r="P23" s="29"/>
+      <c r="Q23" s="29"/>
+      <c r="R23" s="29"/>
+      <c r="S23" s="29"/>
+      <c r="T23" s="29"/>
+      <c r="U23" s="29"/>
+      <c r="V23" s="29"/>
     </row>
     <row r="24" spans="1:22">
       <c r="A24" t="s">
@@ -22656,11 +22713,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55874760-86AA-41EB-A2D6-050D3575AF4D}">
   <dimension ref="A1:X47"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="150" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C22" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A10" sqref="A10:XFD10"/>
+      <selection pane="bottomRight" activeCell="D34" sqref="D34:H34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -22811,18 +22868,18 @@
         <f>INDEX(Harmonized!B:B,MATCH(A9,Harmonized!A:A,0))</f>
         <v>ethnicity</v>
       </c>
-      <c r="O9" s="29" t="s">
+      <c r="O9" s="30" t="s">
         <v>406</v>
       </c>
-      <c r="P9" s="29"/>
-      <c r="Q9" s="29"/>
-      <c r="R9" s="29"/>
-      <c r="S9" s="29"/>
-      <c r="T9" s="29"/>
-      <c r="U9" s="29"/>
-      <c r="V9" s="29"/>
-      <c r="W9" s="29"/>
-      <c r="X9" s="29"/>
+      <c r="P9" s="30"/>
+      <c r="Q9" s="30"/>
+      <c r="R9" s="30"/>
+      <c r="S9" s="30"/>
+      <c r="T9" s="30"/>
+      <c r="U9" s="30"/>
+      <c r="V9" s="30"/>
+      <c r="W9" s="30"/>
+      <c r="X9" s="30"/>
     </row>
     <row r="10" spans="1:24">
       <c r="A10" t="s">
@@ -22835,16 +22892,16 @@
       <c r="D10" t="s">
         <v>370</v>
       </c>
-      <c r="O10" s="29"/>
-      <c r="P10" s="29"/>
-      <c r="Q10" s="29"/>
-      <c r="R10" s="29"/>
-      <c r="S10" s="29"/>
-      <c r="T10" s="29"/>
-      <c r="U10" s="29"/>
-      <c r="V10" s="29"/>
-      <c r="W10" s="29"/>
-      <c r="X10" s="29"/>
+      <c r="O10" s="30"/>
+      <c r="P10" s="30"/>
+      <c r="Q10" s="30"/>
+      <c r="R10" s="30"/>
+      <c r="S10" s="30"/>
+      <c r="T10" s="30"/>
+      <c r="U10" s="30"/>
+      <c r="V10" s="30"/>
+      <c r="W10" s="30"/>
+      <c r="X10" s="30"/>
     </row>
     <row r="11" spans="1:24">
       <c r="A11" t="s">
@@ -22857,16 +22914,16 @@
       <c r="D11" t="s">
         <v>369</v>
       </c>
-      <c r="O11" s="29"/>
-      <c r="P11" s="29"/>
-      <c r="Q11" s="29"/>
-      <c r="R11" s="29"/>
-      <c r="S11" s="29"/>
-      <c r="T11" s="29"/>
-      <c r="U11" s="29"/>
-      <c r="V11" s="29"/>
-      <c r="W11" s="29"/>
-      <c r="X11" s="29"/>
+      <c r="O11" s="30"/>
+      <c r="P11" s="30"/>
+      <c r="Q11" s="30"/>
+      <c r="R11" s="30"/>
+      <c r="S11" s="30"/>
+      <c r="T11" s="30"/>
+      <c r="U11" s="30"/>
+      <c r="V11" s="30"/>
+      <c r="W11" s="30"/>
+      <c r="X11" s="30"/>
     </row>
     <row r="12" spans="1:24">
       <c r="A12" t="s">
@@ -22876,16 +22933,16 @@
         <f>INDEX(Harmonized!B:B,MATCH(A12,Harmonized!A:A,0))</f>
         <v>dmfamilyhistory</v>
       </c>
-      <c r="O12" s="29"/>
-      <c r="P12" s="29"/>
-      <c r="Q12" s="29"/>
-      <c r="R12" s="29"/>
-      <c r="S12" s="29"/>
-      <c r="T12" s="29"/>
-      <c r="U12" s="29"/>
-      <c r="V12" s="29"/>
-      <c r="W12" s="29"/>
-      <c r="X12" s="29"/>
+      <c r="O12" s="30"/>
+      <c r="P12" s="30"/>
+      <c r="Q12" s="30"/>
+      <c r="R12" s="30"/>
+      <c r="S12" s="30"/>
+      <c r="T12" s="30"/>
+      <c r="U12" s="30"/>
+      <c r="V12" s="30"/>
+      <c r="W12" s="30"/>
+      <c r="X12" s="30"/>
     </row>
     <row r="13" spans="1:24">
       <c r="A13" t="s">
@@ -22904,16 +22961,16 @@
       <c r="H13" t="s">
         <v>367</v>
       </c>
-      <c r="O13" s="29"/>
-      <c r="P13" s="29"/>
-      <c r="Q13" s="29"/>
-      <c r="R13" s="29"/>
-      <c r="S13" s="29"/>
-      <c r="T13" s="29"/>
-      <c r="U13" s="29"/>
-      <c r="V13" s="29"/>
-      <c r="W13" s="29"/>
-      <c r="X13" s="29"/>
+      <c r="O13" s="30"/>
+      <c r="P13" s="30"/>
+      <c r="Q13" s="30"/>
+      <c r="R13" s="30"/>
+      <c r="S13" s="30"/>
+      <c r="T13" s="30"/>
+      <c r="U13" s="30"/>
+      <c r="V13" s="30"/>
+      <c r="W13" s="30"/>
+      <c r="X13" s="30"/>
     </row>
     <row r="14" spans="1:24">
       <c r="A14" t="s">
@@ -22932,16 +22989,16 @@
       <c r="H14" t="s">
         <v>303</v>
       </c>
-      <c r="O14" s="29"/>
-      <c r="P14" s="29"/>
-      <c r="Q14" s="29"/>
-      <c r="R14" s="29"/>
-      <c r="S14" s="29"/>
-      <c r="T14" s="29"/>
-      <c r="U14" s="29"/>
-      <c r="V14" s="29"/>
-      <c r="W14" s="29"/>
-      <c r="X14" s="29"/>
+      <c r="O14" s="30"/>
+      <c r="P14" s="30"/>
+      <c r="Q14" s="30"/>
+      <c r="R14" s="30"/>
+      <c r="S14" s="30"/>
+      <c r="T14" s="30"/>
+      <c r="U14" s="30"/>
+      <c r="V14" s="30"/>
+      <c r="W14" s="30"/>
+      <c r="X14" s="30"/>
     </row>
     <row r="15" spans="1:24">
       <c r="A15" t="s">
@@ -22960,16 +23017,16 @@
       <c r="H15" t="s">
         <v>11</v>
       </c>
-      <c r="O15" s="29"/>
-      <c r="P15" s="29"/>
-      <c r="Q15" s="29"/>
-      <c r="R15" s="29"/>
-      <c r="S15" s="29"/>
-      <c r="T15" s="29"/>
-      <c r="U15" s="29"/>
-      <c r="V15" s="29"/>
-      <c r="W15" s="29"/>
-      <c r="X15" s="29"/>
+      <c r="O15" s="30"/>
+      <c r="P15" s="30"/>
+      <c r="Q15" s="30"/>
+      <c r="R15" s="30"/>
+      <c r="S15" s="30"/>
+      <c r="T15" s="30"/>
+      <c r="U15" s="30"/>
+      <c r="V15" s="30"/>
+      <c r="W15" s="30"/>
+      <c r="X15" s="30"/>
     </row>
     <row r="16" spans="1:24">
       <c r="A16" t="s">
@@ -22988,16 +23045,16 @@
       <c r="H16" t="s">
         <v>48</v>
       </c>
-      <c r="O16" s="29"/>
-      <c r="P16" s="29"/>
-      <c r="Q16" s="29"/>
-      <c r="R16" s="29"/>
-      <c r="S16" s="29"/>
-      <c r="T16" s="29"/>
-      <c r="U16" s="29"/>
-      <c r="V16" s="29"/>
-      <c r="W16" s="29"/>
-      <c r="X16" s="29"/>
+      <c r="O16" s="30"/>
+      <c r="P16" s="30"/>
+      <c r="Q16" s="30"/>
+      <c r="R16" s="30"/>
+      <c r="S16" s="30"/>
+      <c r="T16" s="30"/>
+      <c r="U16" s="30"/>
+      <c r="V16" s="30"/>
+      <c r="W16" s="30"/>
+      <c r="X16" s="30"/>
     </row>
     <row r="17" spans="1:24">
       <c r="A17" t="s">
@@ -23016,16 +23073,16 @@
       <c r="H17" t="s">
         <v>49</v>
       </c>
-      <c r="O17" s="29"/>
-      <c r="P17" s="29"/>
-      <c r="Q17" s="29"/>
-      <c r="R17" s="29"/>
-      <c r="S17" s="29"/>
-      <c r="T17" s="29"/>
-      <c r="U17" s="29"/>
-      <c r="V17" s="29"/>
-      <c r="W17" s="29"/>
-      <c r="X17" s="29"/>
+      <c r="O17" s="30"/>
+      <c r="P17" s="30"/>
+      <c r="Q17" s="30"/>
+      <c r="R17" s="30"/>
+      <c r="S17" s="30"/>
+      <c r="T17" s="30"/>
+      <c r="U17" s="30"/>
+      <c r="V17" s="30"/>
+      <c r="W17" s="30"/>
+      <c r="X17" s="30"/>
     </row>
     <row r="18" spans="1:24">
       <c r="A18" t="s">
@@ -23044,16 +23101,16 @@
       <c r="H18" t="s">
         <v>368</v>
       </c>
-      <c r="O18" s="29"/>
-      <c r="P18" s="29"/>
-      <c r="Q18" s="29"/>
-      <c r="R18" s="29"/>
-      <c r="S18" s="29"/>
-      <c r="T18" s="29"/>
-      <c r="U18" s="29"/>
-      <c r="V18" s="29"/>
-      <c r="W18" s="29"/>
-      <c r="X18" s="29"/>
+      <c r="O18" s="30"/>
+      <c r="P18" s="30"/>
+      <c r="Q18" s="30"/>
+      <c r="R18" s="30"/>
+      <c r="S18" s="30"/>
+      <c r="T18" s="30"/>
+      <c r="U18" s="30"/>
+      <c r="V18" s="30"/>
+      <c r="W18" s="30"/>
+      <c r="X18" s="30"/>
     </row>
     <row r="19" spans="1:24">
       <c r="A19" t="s">
@@ -23072,16 +23129,16 @@
       <c r="H19" t="s">
         <v>381</v>
       </c>
-      <c r="O19" s="29"/>
-      <c r="P19" s="29"/>
-      <c r="Q19" s="29"/>
-      <c r="R19" s="29"/>
-      <c r="S19" s="29"/>
-      <c r="T19" s="29"/>
-      <c r="U19" s="29"/>
-      <c r="V19" s="29"/>
-      <c r="W19" s="29"/>
-      <c r="X19" s="29"/>
+      <c r="O19" s="30"/>
+      <c r="P19" s="30"/>
+      <c r="Q19" s="30"/>
+      <c r="R19" s="30"/>
+      <c r="S19" s="30"/>
+      <c r="T19" s="30"/>
+      <c r="U19" s="30"/>
+      <c r="V19" s="30"/>
+      <c r="W19" s="30"/>
+      <c r="X19" s="30"/>
     </row>
     <row r="20" spans="1:24">
       <c r="A20" t="s">
@@ -23097,16 +23154,16 @@
       <c r="H20" t="s">
         <v>382</v>
       </c>
-      <c r="O20" s="29"/>
-      <c r="P20" s="29"/>
-      <c r="Q20" s="29"/>
-      <c r="R20" s="29"/>
-      <c r="S20" s="29"/>
-      <c r="T20" s="29"/>
-      <c r="U20" s="29"/>
-      <c r="V20" s="29"/>
-      <c r="W20" s="29"/>
-      <c r="X20" s="29"/>
+      <c r="O20" s="30"/>
+      <c r="P20" s="30"/>
+      <c r="Q20" s="30"/>
+      <c r="R20" s="30"/>
+      <c r="S20" s="30"/>
+      <c r="T20" s="30"/>
+      <c r="U20" s="30"/>
+      <c r="V20" s="30"/>
+      <c r="W20" s="30"/>
+      <c r="X20" s="30"/>
     </row>
     <row r="21" spans="1:24">
       <c r="A21" t="s">
@@ -23285,13 +23342,13 @@
         <v>urinealbumin</v>
       </c>
       <c r="D33" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="F33" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="H33" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row r="34" spans="1:8">
@@ -23303,13 +23360,13 @@
         <v>urinecreatinine</v>
       </c>
       <c r="D34" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="F34" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="H34" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="35" spans="1:8">
@@ -23455,10 +23512,10 @@
   <dimension ref="A1:T58"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A21" sqref="A21:XFD21"/>
+      <selection pane="bottomRight" activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -23512,17 +23569,17 @@
       <c r="E3" t="s">
         <v>125</v>
       </c>
-      <c r="L3" s="28" t="s">
+      <c r="L3" s="29" t="s">
         <v>123</v>
       </c>
-      <c r="M3" s="28"/>
-      <c r="N3" s="28"/>
-      <c r="O3" s="28"/>
-      <c r="P3" s="28"/>
-      <c r="Q3" s="28"/>
-      <c r="R3" s="28"/>
-      <c r="S3" s="28"/>
-      <c r="T3" s="28"/>
+      <c r="M3" s="29"/>
+      <c r="N3" s="29"/>
+      <c r="O3" s="29"/>
+      <c r="P3" s="29"/>
+      <c r="Q3" s="29"/>
+      <c r="R3" s="29"/>
+      <c r="S3" s="29"/>
+      <c r="T3" s="29"/>
     </row>
     <row r="4" spans="1:20">
       <c r="A4" t="s">
@@ -23535,15 +23592,15 @@
       <c r="C4" t="s">
         <v>66</v>
       </c>
-      <c r="L4" s="28"/>
-      <c r="M4" s="28"/>
-      <c r="N4" s="28"/>
-      <c r="O4" s="28"/>
-      <c r="P4" s="28"/>
-      <c r="Q4" s="28"/>
-      <c r="R4" s="28"/>
-      <c r="S4" s="28"/>
-      <c r="T4" s="28"/>
+      <c r="L4" s="29"/>
+      <c r="M4" s="29"/>
+      <c r="N4" s="29"/>
+      <c r="O4" s="29"/>
+      <c r="P4" s="29"/>
+      <c r="Q4" s="29"/>
+      <c r="R4" s="29"/>
+      <c r="S4" s="29"/>
+      <c r="T4" s="29"/>
     </row>
     <row r="5" spans="1:20">
       <c r="A5" t="s">
@@ -23553,15 +23610,15 @@
         <f>INDEX(Harmonized!B:B,MATCH(A5,Harmonized!A:A,0))</f>
         <v>dmagediag</v>
       </c>
-      <c r="L5" s="28"/>
-      <c r="M5" s="28"/>
-      <c r="N5" s="28"/>
-      <c r="O5" s="28"/>
-      <c r="P5" s="28"/>
-      <c r="Q5" s="28"/>
-      <c r="R5" s="28"/>
-      <c r="S5" s="28"/>
-      <c r="T5" s="28"/>
+      <c r="L5" s="29"/>
+      <c r="M5" s="29"/>
+      <c r="N5" s="29"/>
+      <c r="O5" s="29"/>
+      <c r="P5" s="29"/>
+      <c r="Q5" s="29"/>
+      <c r="R5" s="29"/>
+      <c r="S5" s="29"/>
+      <c r="T5" s="29"/>
     </row>
     <row r="6" spans="1:20">
       <c r="A6" t="s">
@@ -23574,15 +23631,15 @@
       <c r="C6" t="s">
         <v>8</v>
       </c>
-      <c r="L6" s="28"/>
-      <c r="M6" s="28"/>
-      <c r="N6" s="28"/>
-      <c r="O6" s="28"/>
-      <c r="P6" s="28"/>
-      <c r="Q6" s="28"/>
-      <c r="R6" s="28"/>
-      <c r="S6" s="28"/>
-      <c r="T6" s="28"/>
+      <c r="L6" s="29"/>
+      <c r="M6" s="29"/>
+      <c r="N6" s="29"/>
+      <c r="O6" s="29"/>
+      <c r="P6" s="29"/>
+      <c r="Q6" s="29"/>
+      <c r="R6" s="29"/>
+      <c r="S6" s="29"/>
+      <c r="T6" s="29"/>
     </row>
     <row r="7" spans="1:20">
       <c r="A7" t="s">
@@ -23595,15 +23652,15 @@
       <c r="C7" t="s">
         <v>64</v>
       </c>
-      <c r="L7" s="28"/>
-      <c r="M7" s="28"/>
-      <c r="N7" s="28"/>
-      <c r="O7" s="28"/>
-      <c r="P7" s="28"/>
-      <c r="Q7" s="28"/>
-      <c r="R7" s="28"/>
-      <c r="S7" s="28"/>
-      <c r="T7" s="28"/>
+      <c r="L7" s="29"/>
+      <c r="M7" s="29"/>
+      <c r="N7" s="29"/>
+      <c r="O7" s="29"/>
+      <c r="P7" s="29"/>
+      <c r="Q7" s="29"/>
+      <c r="R7" s="29"/>
+      <c r="S7" s="29"/>
+      <c r="T7" s="29"/>
     </row>
     <row r="8" spans="1:20">
       <c r="A8" t="s">
@@ -23616,15 +23673,15 @@
       <c r="C8" t="s">
         <v>69</v>
       </c>
-      <c r="L8" s="28"/>
-      <c r="M8" s="28"/>
-      <c r="N8" s="28"/>
-      <c r="O8" s="28"/>
-      <c r="P8" s="28"/>
-      <c r="Q8" s="28"/>
-      <c r="R8" s="28"/>
-      <c r="S8" s="28"/>
-      <c r="T8" s="28"/>
+      <c r="L8" s="29"/>
+      <c r="M8" s="29"/>
+      <c r="N8" s="29"/>
+      <c r="O8" s="29"/>
+      <c r="P8" s="29"/>
+      <c r="Q8" s="29"/>
+      <c r="R8" s="29"/>
+      <c r="S8" s="29"/>
+      <c r="T8" s="29"/>
     </row>
     <row r="9" spans="1:20">
       <c r="A9" t="s">
@@ -23637,15 +23694,15 @@
       <c r="C9" t="s">
         <v>70</v>
       </c>
-      <c r="L9" s="28"/>
-      <c r="M9" s="28"/>
-      <c r="N9" s="28"/>
-      <c r="O9" s="28"/>
-      <c r="P9" s="28"/>
-      <c r="Q9" s="28"/>
-      <c r="R9" s="28"/>
-      <c r="S9" s="28"/>
-      <c r="T9" s="28"/>
+      <c r="L9" s="29"/>
+      <c r="M9" s="29"/>
+      <c r="N9" s="29"/>
+      <c r="O9" s="29"/>
+      <c r="P9" s="29"/>
+      <c r="Q9" s="29"/>
+      <c r="R9" s="29"/>
+      <c r="S9" s="29"/>
+      <c r="T9" s="29"/>
     </row>
     <row r="10" spans="1:20">
       <c r="A10" t="s">
@@ -23658,15 +23715,15 @@
       <c r="C10" t="s">
         <v>73</v>
       </c>
-      <c r="L10" s="28"/>
-      <c r="M10" s="28"/>
-      <c r="N10" s="28"/>
-      <c r="O10" s="28"/>
-      <c r="P10" s="28"/>
-      <c r="Q10" s="28"/>
-      <c r="R10" s="28"/>
-      <c r="S10" s="28"/>
-      <c r="T10" s="28"/>
+      <c r="L10" s="29"/>
+      <c r="M10" s="29"/>
+      <c r="N10" s="29"/>
+      <c r="O10" s="29"/>
+      <c r="P10" s="29"/>
+      <c r="Q10" s="29"/>
+      <c r="R10" s="29"/>
+      <c r="S10" s="29"/>
+      <c r="T10" s="29"/>
     </row>
     <row r="11" spans="1:20">
       <c r="A11" t="s">
@@ -23679,15 +23736,15 @@
       <c r="C11" t="s">
         <v>54</v>
       </c>
-      <c r="L11" s="28"/>
-      <c r="M11" s="28"/>
-      <c r="N11" s="28"/>
-      <c r="O11" s="28"/>
-      <c r="P11" s="28"/>
-      <c r="Q11" s="28"/>
-      <c r="R11" s="28"/>
-      <c r="S11" s="28"/>
-      <c r="T11" s="28"/>
+      <c r="L11" s="29"/>
+      <c r="M11" s="29"/>
+      <c r="N11" s="29"/>
+      <c r="O11" s="29"/>
+      <c r="P11" s="29"/>
+      <c r="Q11" s="29"/>
+      <c r="R11" s="29"/>
+      <c r="S11" s="29"/>
+      <c r="T11" s="29"/>
     </row>
     <row r="12" spans="1:20">
       <c r="A12" t="s">
@@ -23700,15 +23757,15 @@
       <c r="C12" t="s">
         <v>74</v>
       </c>
-      <c r="L12" s="28"/>
-      <c r="M12" s="28"/>
-      <c r="N12" s="28"/>
-      <c r="O12" s="28"/>
-      <c r="P12" s="28"/>
-      <c r="Q12" s="28"/>
-      <c r="R12" s="28"/>
-      <c r="S12" s="28"/>
-      <c r="T12" s="28"/>
+      <c r="L12" s="29"/>
+      <c r="M12" s="29"/>
+      <c r="N12" s="29"/>
+      <c r="O12" s="29"/>
+      <c r="P12" s="29"/>
+      <c r="Q12" s="29"/>
+      <c r="R12" s="29"/>
+      <c r="S12" s="29"/>
+      <c r="T12" s="29"/>
     </row>
     <row r="13" spans="1:20">
       <c r="A13" t="s">
@@ -23719,15 +23776,15 @@
         <v>height</v>
       </c>
       <c r="E13" s="1"/>
-      <c r="L13" s="28"/>
-      <c r="M13" s="28"/>
-      <c r="N13" s="28"/>
-      <c r="O13" s="28"/>
-      <c r="P13" s="28"/>
-      <c r="Q13" s="28"/>
-      <c r="R13" s="28"/>
-      <c r="S13" s="28"/>
-      <c r="T13" s="28"/>
+      <c r="L13" s="29"/>
+      <c r="M13" s="29"/>
+      <c r="N13" s="29"/>
+      <c r="O13" s="29"/>
+      <c r="P13" s="29"/>
+      <c r="Q13" s="29"/>
+      <c r="R13" s="29"/>
+      <c r="S13" s="29"/>
+      <c r="T13" s="29"/>
     </row>
     <row r="14" spans="1:20">
       <c r="A14" t="s">
@@ -23738,15 +23795,15 @@
         <v>weight</v>
       </c>
       <c r="E14" s="1"/>
-      <c r="L14" s="28"/>
-      <c r="M14" s="28"/>
-      <c r="N14" s="28"/>
-      <c r="O14" s="28"/>
-      <c r="P14" s="28"/>
-      <c r="Q14" s="28"/>
-      <c r="R14" s="28"/>
-      <c r="S14" s="28"/>
-      <c r="T14" s="28"/>
+      <c r="L14" s="29"/>
+      <c r="M14" s="29"/>
+      <c r="N14" s="29"/>
+      <c r="O14" s="29"/>
+      <c r="P14" s="29"/>
+      <c r="Q14" s="29"/>
+      <c r="R14" s="29"/>
+      <c r="S14" s="29"/>
+      <c r="T14" s="29"/>
     </row>
     <row r="15" spans="1:20">
       <c r="A15" t="s">
@@ -23759,15 +23816,15 @@
       <c r="E15" t="s">
         <v>76</v>
       </c>
-      <c r="L15" s="28"/>
-      <c r="M15" s="28"/>
-      <c r="N15" s="28"/>
-      <c r="O15" s="28"/>
-      <c r="P15" s="28"/>
-      <c r="Q15" s="28"/>
-      <c r="R15" s="28"/>
-      <c r="S15" s="28"/>
-      <c r="T15" s="28"/>
+      <c r="L15" s="29"/>
+      <c r="M15" s="29"/>
+      <c r="N15" s="29"/>
+      <c r="O15" s="29"/>
+      <c r="P15" s="29"/>
+      <c r="Q15" s="29"/>
+      <c r="R15" s="29"/>
+      <c r="S15" s="29"/>
+      <c r="T15" s="29"/>
     </row>
     <row r="16" spans="1:20">
       <c r="A16" t="s">

</xml_diff>

<commit_message>
extracted gender and race variables
</commit_message>
<xml_diff>
--- a/data/Phenotypes Variable List.xlsx
+++ b/data/Phenotypes Variable List.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10609"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="2217" documentId="13_ncr:1_{0AF53CB1-23E0-45A0-9003-9470A819876D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D812EE87-D0FD-734C-B189-F25E376AE60A}"/>
+  <xr:revisionPtr revIDLastSave="2222" documentId="13_ncr:1_{0AF53CB1-23E0-45A0-9003-9470A819876D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A5552DD7-E038-CF43-B4AF-58FD49FFAD91}"/>
   <bookViews>
-    <workbookView xWindow="1700" yWindow="760" windowWidth="30240" windowHeight="17680" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17680" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Harmonized" sheetId="2" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3418" uniqueCount="2250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3422" uniqueCount="2249">
   <si>
     <t>harmonized</t>
   </si>
@@ -5283,9 +5283,6 @@
   </si>
   <si>
     <t>AGE AT EXAM 1 (VERIFIED AT EXAM 2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RACE </t>
   </si>
   <si>
     <t>baf07</t>
@@ -8243,37 +8240,37 @@
         <v>0</v>
       </c>
       <c r="C1" s="23" t="s">
+        <v>2021</v>
+      </c>
+      <c r="D1" t="s">
         <v>2022</v>
       </c>
-      <c r="D1" t="s">
-        <v>2023</v>
-      </c>
       <c r="E1" s="23" t="s">
-        <v>2074</v>
+        <v>2073</v>
       </c>
       <c r="F1" t="s">
-        <v>2077</v>
+        <v>2076</v>
       </c>
       <c r="G1" t="s">
-        <v>2246</v>
+        <v>2245</v>
       </c>
       <c r="H1" s="23" t="s">
+        <v>2103</v>
+      </c>
+      <c r="I1" t="s">
         <v>2104</v>
       </c>
-      <c r="I1" t="s">
-        <v>2105</v>
-      </c>
       <c r="J1" s="23" t="s">
+        <v>2124</v>
+      </c>
+      <c r="K1" t="s">
         <v>2125</v>
       </c>
-      <c r="K1" t="s">
-        <v>2126</v>
-      </c>
       <c r="L1" s="23" t="s">
-        <v>2182</v>
+        <v>2181</v>
       </c>
       <c r="M1" t="s">
-        <v>2220</v>
+        <v>2219</v>
       </c>
     </row>
     <row r="2" spans="1:13">
@@ -8294,22 +8291,22 @@
         <v>study_id</v>
       </c>
       <c r="D3" t="s">
-        <v>2026</v>
+        <v>2025</v>
       </c>
       <c r="F3" t="s">
-        <v>2075</v>
+        <v>2074</v>
       </c>
       <c r="G3" t="s">
-        <v>2026</v>
+        <v>2025</v>
       </c>
       <c r="I3" t="s">
-        <v>2075</v>
+        <v>2074</v>
       </c>
       <c r="K3" t="s">
-        <v>2075</v>
+        <v>2074</v>
       </c>
       <c r="M3" t="s">
-        <v>2026</v>
+        <v>2025</v>
       </c>
     </row>
     <row r="4" spans="1:13">
@@ -8340,19 +8337,19 @@
         <v>age</v>
       </c>
       <c r="D6" t="s">
-        <v>2025</v>
+        <v>2024</v>
       </c>
       <c r="F6" t="s">
-        <v>2076</v>
+        <v>2075</v>
       </c>
       <c r="I6" t="s">
-        <v>2106</v>
+        <v>2105</v>
       </c>
       <c r="K6" t="s">
-        <v>2127</v>
+        <v>2126</v>
       </c>
       <c r="M6" t="s">
-        <v>2183</v>
+        <v>2182</v>
       </c>
     </row>
     <row r="7" spans="1:13">
@@ -8364,19 +8361,19 @@
         <v>female</v>
       </c>
       <c r="D7" t="s">
-        <v>2024</v>
+        <v>2023</v>
       </c>
       <c r="F7" t="s">
-        <v>2024</v>
+        <v>2023</v>
       </c>
       <c r="I7" t="s">
-        <v>2024</v>
+        <v>2023</v>
       </c>
       <c r="K7" t="s">
-        <v>2024</v>
+        <v>2023</v>
       </c>
       <c r="M7" t="s">
-        <v>2184</v>
+        <v>2183</v>
       </c>
     </row>
     <row r="8" spans="1:13">
@@ -8388,19 +8385,19 @@
         <v>race</v>
       </c>
       <c r="D8" t="s">
-        <v>2027</v>
+        <v>2026</v>
       </c>
       <c r="F8" t="s">
-        <v>2027</v>
+        <v>2026</v>
       </c>
       <c r="I8" t="s">
-        <v>2027</v>
+        <v>2026</v>
       </c>
       <c r="K8" t="s">
-        <v>2027</v>
+        <v>2026</v>
       </c>
       <c r="M8" t="s">
-        <v>2185</v>
+        <v>2184</v>
       </c>
     </row>
     <row r="9" spans="1:13">
@@ -8412,19 +8409,19 @@
         <v>ethnicity</v>
       </c>
       <c r="D9" t="s">
-        <v>2128</v>
+        <v>2127</v>
       </c>
       <c r="F9" t="s">
-        <v>2128</v>
+        <v>2127</v>
       </c>
       <c r="I9" t="s">
-        <v>2128</v>
+        <v>2127</v>
       </c>
       <c r="K9" t="s">
-        <v>2128</v>
+        <v>2127</v>
       </c>
       <c r="M9" t="s">
-        <v>2186</v>
+        <v>2185</v>
       </c>
     </row>
     <row r="10" spans="1:13">
@@ -8454,7 +8451,7 @@
         <v>dmfamilyhistory</v>
       </c>
       <c r="G12" t="s">
-        <v>2084</v>
+        <v>2083</v>
       </c>
     </row>
     <row r="13" spans="1:13">
@@ -8466,19 +8463,19 @@
         <v>height</v>
       </c>
       <c r="D13" t="s">
-        <v>2055</v>
+        <v>2054</v>
       </c>
       <c r="F13" t="s">
-        <v>2091</v>
+        <v>2090</v>
       </c>
       <c r="I13" t="s">
-        <v>2111</v>
+        <v>2110</v>
       </c>
       <c r="K13" t="s">
-        <v>2133</v>
+        <v>2132</v>
       </c>
       <c r="M13" t="s">
-        <v>2197</v>
+        <v>2196</v>
       </c>
     </row>
     <row r="14" spans="1:13">
@@ -8490,19 +8487,19 @@
         <v>weight</v>
       </c>
       <c r="D14" t="s">
-        <v>2056</v>
+        <v>2055</v>
       </c>
       <c r="F14" t="s">
-        <v>2092</v>
+        <v>2091</v>
       </c>
       <c r="I14" t="s">
-        <v>2112</v>
+        <v>2111</v>
       </c>
       <c r="K14" t="s">
-        <v>2134</v>
+        <v>2133</v>
       </c>
       <c r="M14" t="s">
-        <v>2198</v>
+        <v>2197</v>
       </c>
     </row>
     <row r="15" spans="1:13">
@@ -8514,19 +8511,19 @@
         <v>bmi</v>
       </c>
       <c r="D15" t="s">
-        <v>2057</v>
+        <v>2056</v>
       </c>
       <c r="F15" t="s">
-        <v>2093</v>
+        <v>2092</v>
       </c>
       <c r="I15" t="s">
-        <v>2113</v>
+        <v>2112</v>
       </c>
       <c r="K15" t="s">
-        <v>2135</v>
+        <v>2134</v>
       </c>
       <c r="M15" t="s">
-        <v>2199</v>
+        <v>2198</v>
       </c>
     </row>
     <row r="16" spans="1:13">
@@ -8558,19 +8555,19 @@
         <v>wc</v>
       </c>
       <c r="D18" t="s">
-        <v>2058</v>
+        <v>2057</v>
       </c>
       <c r="F18" t="s">
-        <v>2094</v>
+        <v>2093</v>
       </c>
       <c r="I18" t="s">
+        <v>2147</v>
+      </c>
+      <c r="K18" t="s">
         <v>2148</v>
       </c>
-      <c r="K18" t="s">
-        <v>2149</v>
-      </c>
       <c r="M18" t="s">
-        <v>2200</v>
+        <v>2199</v>
       </c>
     </row>
     <row r="19" spans="1:13">
@@ -8609,16 +8606,16 @@
         <v>glucosef</v>
       </c>
       <c r="F22" t="s">
-        <v>2096</v>
+        <v>2095</v>
       </c>
       <c r="I22" t="s">
-        <v>2114</v>
+        <v>2113</v>
       </c>
       <c r="K22" t="s">
-        <v>2153</v>
+        <v>2152</v>
       </c>
       <c r="M22" t="s">
-        <v>2202</v>
+        <v>2201</v>
       </c>
     </row>
     <row r="23" spans="1:13">
@@ -8648,20 +8645,20 @@
         <v>totalc</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>2065</v>
+        <v>2064</v>
       </c>
       <c r="F25" s="6" t="s">
-        <v>2097</v>
+        <v>2096</v>
       </c>
       <c r="G25" s="6"/>
       <c r="I25" s="6" t="s">
-        <v>2115</v>
+        <v>2114</v>
       </c>
       <c r="K25" t="s">
-        <v>2154</v>
+        <v>2153</v>
       </c>
       <c r="M25" t="s">
-        <v>2203</v>
+        <v>2202</v>
       </c>
     </row>
     <row r="26" spans="1:13">
@@ -8673,20 +8670,20 @@
         <v>ldlc</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>2066</v>
+        <v>2065</v>
       </c>
       <c r="F26" s="6" t="s">
-        <v>2098</v>
+        <v>2097</v>
       </c>
       <c r="G26" s="6"/>
       <c r="I26" s="6" t="s">
-        <v>2116</v>
+        <v>2115</v>
       </c>
       <c r="K26" s="6" t="s">
-        <v>2155</v>
+        <v>2154</v>
       </c>
       <c r="M26" t="s">
-        <v>2204</v>
+        <v>2203</v>
       </c>
     </row>
     <row r="27" spans="1:13">
@@ -8698,20 +8695,20 @@
         <v>hdlc</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>2067</v>
+        <v>2066</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>2099</v>
+        <v>2098</v>
       </c>
       <c r="G27" s="6"/>
       <c r="I27" s="6" t="s">
-        <v>2117</v>
+        <v>2116</v>
       </c>
       <c r="K27" s="6" t="s">
-        <v>2156</v>
+        <v>2155</v>
       </c>
       <c r="M27" t="s">
-        <v>2205</v>
+        <v>2204</v>
       </c>
     </row>
     <row r="28" spans="1:13">
@@ -8732,20 +8729,20 @@
         <v>tgl</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>2068</v>
+        <v>2067</v>
       </c>
       <c r="F29" s="6" t="s">
-        <v>2100</v>
+        <v>2099</v>
       </c>
       <c r="G29" s="6"/>
       <c r="I29" s="6" t="s">
-        <v>2118</v>
+        <v>2117</v>
       </c>
       <c r="K29" s="6" t="s">
-        <v>2157</v>
+        <v>2156</v>
       </c>
       <c r="M29" s="6" t="s">
-        <v>2206</v>
+        <v>2205</v>
       </c>
     </row>
     <row r="30" spans="1:13">
@@ -8757,16 +8754,16 @@
         <v>serumcreatinine</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>2072</v>
+        <v>2071</v>
       </c>
       <c r="I30" s="6" t="s">
-        <v>2122</v>
+        <v>2121</v>
       </c>
       <c r="K30" s="6" t="s">
-        <v>2158</v>
+        <v>2157</v>
       </c>
       <c r="M30" t="s">
-        <v>2207</v>
+        <v>2206</v>
       </c>
     </row>
     <row r="31" spans="1:13">
@@ -8778,17 +8775,17 @@
         <v>urinealbumin</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>2073</v>
+        <v>2072</v>
       </c>
       <c r="F31" s="6" t="s">
-        <v>2103</v>
+        <v>2102</v>
       </c>
       <c r="G31" s="6"/>
       <c r="I31" s="6" t="s">
-        <v>2120</v>
+        <v>2119</v>
       </c>
       <c r="M31" t="s">
-        <v>2210</v>
+        <v>2209</v>
       </c>
     </row>
     <row r="32" spans="1:13">
@@ -8800,16 +8797,16 @@
         <v>urinecreatinine</v>
       </c>
       <c r="D32" t="s">
-        <v>2071</v>
+        <v>2070</v>
       </c>
       <c r="F32" t="s">
-        <v>2102</v>
+        <v>2101</v>
       </c>
       <c r="I32" t="s">
-        <v>2119</v>
+        <v>2118</v>
       </c>
       <c r="M32" t="s">
-        <v>2209</v>
+        <v>2208</v>
       </c>
     </row>
     <row r="33" spans="1:13">
@@ -8821,16 +8818,16 @@
         <v>uacr</v>
       </c>
       <c r="D33" t="s">
-        <v>2070</v>
+        <v>2069</v>
       </c>
       <c r="F33" t="s">
-        <v>2101</v>
+        <v>2100</v>
       </c>
       <c r="I33" s="6" t="s">
-        <v>2121</v>
+        <v>2120</v>
       </c>
       <c r="M33" t="s">
-        <v>2208</v>
+        <v>2207</v>
       </c>
     </row>
     <row r="34" spans="1:13">
@@ -8842,15 +8839,15 @@
         <v>egfr</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>2069</v>
+        <v>2068</v>
       </c>
       <c r="F34" s="6"/>
       <c r="G34" s="6"/>
       <c r="K34" s="6" t="s">
-        <v>2150</v>
+        <v>2149</v>
       </c>
       <c r="M34" t="s">
-        <v>2221</v>
+        <v>2220</v>
       </c>
     </row>
     <row r="35" spans="1:13">
@@ -8878,507 +8875,507 @@
     </row>
     <row r="39" spans="1:13">
       <c r="A39" s="6" t="s">
-        <v>2079</v>
+        <v>2078</v>
       </c>
       <c r="B39" t="s">
-        <v>2222</v>
+        <v>2221</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>2028</v>
+        <v>2027</v>
       </c>
       <c r="F39" t="s">
-        <v>2078</v>
+        <v>2077</v>
       </c>
       <c r="I39" t="s">
-        <v>2107</v>
+        <v>2106</v>
       </c>
       <c r="K39" t="s">
-        <v>2129</v>
+        <v>2128</v>
       </c>
       <c r="M39" t="s">
-        <v>2187</v>
+        <v>2186</v>
       </c>
     </row>
     <row r="40" spans="1:13">
       <c r="A40" s="6" t="s">
+        <v>2028</v>
+      </c>
+      <c r="B40" t="s">
+        <v>2222</v>
+      </c>
+      <c r="D40" s="6" t="s">
         <v>2029</v>
-      </c>
-      <c r="B40" t="s">
-        <v>2223</v>
-      </c>
-      <c r="D40" s="6" t="s">
-        <v>2030</v>
       </c>
     </row>
     <row r="41" spans="1:13">
       <c r="A41" s="6" t="s">
-        <v>2031</v>
+        <v>2030</v>
       </c>
       <c r="B41" t="s">
-        <v>2224</v>
+        <v>2223</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>2035</v>
+        <v>2034</v>
       </c>
     </row>
     <row r="42" spans="1:13">
       <c r="A42" s="6" t="s">
-        <v>2032</v>
+        <v>2031</v>
       </c>
       <c r="B42" t="s">
-        <v>2225</v>
+        <v>2224</v>
       </c>
       <c r="D42" s="6" t="s">
-        <v>2036</v>
+        <v>2035</v>
       </c>
       <c r="M42" t="s">
-        <v>2192</v>
+        <v>2191</v>
       </c>
     </row>
     <row r="43" spans="1:13">
       <c r="A43" s="6" t="s">
-        <v>2189</v>
+        <v>2188</v>
       </c>
       <c r="B43" t="s">
-        <v>2226</v>
+        <v>2225</v>
       </c>
       <c r="D43" s="6"/>
       <c r="M43" t="s">
-        <v>2188</v>
+        <v>2187</v>
       </c>
     </row>
     <row r="44" spans="1:13">
       <c r="A44" s="6" t="s">
-        <v>2190</v>
+        <v>2189</v>
       </c>
       <c r="B44" t="s">
-        <v>2227</v>
+        <v>2226</v>
       </c>
       <c r="D44" s="6"/>
       <c r="M44" s="6" t="s">
-        <v>2191</v>
+        <v>2190</v>
       </c>
     </row>
     <row r="45" spans="1:13">
       <c r="A45" s="6" t="s">
-        <v>2033</v>
+        <v>2032</v>
       </c>
       <c r="B45" t="s">
-        <v>2229</v>
+        <v>2228</v>
       </c>
       <c r="D45" s="6" t="s">
-        <v>2037</v>
+        <v>2036</v>
       </c>
     </row>
     <row r="46" spans="1:13">
       <c r="A46" s="6" t="s">
-        <v>2034</v>
+        <v>2033</v>
       </c>
       <c r="B46" t="s">
-        <v>2228</v>
+        <v>2227</v>
       </c>
       <c r="D46" s="6" t="s">
-        <v>2038</v>
+        <v>2037</v>
       </c>
     </row>
     <row r="47" spans="1:13">
       <c r="A47" s="6" t="s">
+        <v>2038</v>
+      </c>
+      <c r="B47" t="s">
+        <v>2231</v>
+      </c>
+      <c r="D47" s="6" t="s">
         <v>2039</v>
-      </c>
-      <c r="B47" t="s">
-        <v>2232</v>
-      </c>
-      <c r="D47" s="6" t="s">
-        <v>2040</v>
       </c>
     </row>
     <row r="48" spans="1:13">
       <c r="A48" s="6" t="s">
+        <v>2050</v>
+      </c>
+      <c r="B48" t="s">
+        <v>2230</v>
+      </c>
+      <c r="D48" s="6" t="s">
         <v>2051</v>
       </c>
-      <c r="B48" t="s">
-        <v>2231</v>
-      </c>
-      <c r="D48" s="6" t="s">
-        <v>2052</v>
-      </c>
       <c r="F48" t="s">
-        <v>2082</v>
+        <v>2081</v>
       </c>
       <c r="I48" t="s">
-        <v>2108</v>
+        <v>2107</v>
       </c>
       <c r="K48" t="s">
-        <v>2130</v>
+        <v>2129</v>
       </c>
       <c r="M48" t="s">
-        <v>2195</v>
+        <v>2194</v>
       </c>
     </row>
     <row r="49" spans="1:13">
       <c r="A49" s="6" t="s">
+        <v>2052</v>
+      </c>
+      <c r="B49" t="s">
+        <v>2232</v>
+      </c>
+      <c r="D49" s="6" t="s">
         <v>2053</v>
       </c>
-      <c r="B49" t="s">
-        <v>2233</v>
-      </c>
-      <c r="D49" s="6" t="s">
-        <v>2054</v>
-      </c>
       <c r="F49" t="s">
-        <v>2083</v>
+        <v>2082</v>
       </c>
       <c r="I49" t="s">
-        <v>2109</v>
+        <v>2108</v>
       </c>
       <c r="K49" t="s">
-        <v>2131</v>
+        <v>2130</v>
       </c>
       <c r="M49" t="s">
-        <v>2193</v>
+        <v>2192</v>
       </c>
     </row>
     <row r="50" spans="1:13">
       <c r="A50" s="6" t="s">
+        <v>2060</v>
+      </c>
+      <c r="B50" t="s">
+        <v>2229</v>
+      </c>
+      <c r="D50" s="6" t="s">
         <v>2061</v>
       </c>
-      <c r="B50" t="s">
-        <v>2230</v>
-      </c>
-      <c r="D50" s="6" t="s">
-        <v>2062</v>
-      </c>
       <c r="F50" t="s">
-        <v>2245</v>
+        <v>2244</v>
       </c>
       <c r="I50" s="6" t="s">
-        <v>2110</v>
+        <v>2109</v>
       </c>
       <c r="K50" s="6" t="s">
-        <v>2132</v>
+        <v>2131</v>
       </c>
       <c r="M50" t="s">
-        <v>2196</v>
+        <v>2195</v>
       </c>
     </row>
     <row r="51" spans="1:13">
       <c r="A51" s="6" t="s">
+        <v>2079</v>
+      </c>
+      <c r="B51" t="s">
+        <v>2233</v>
+      </c>
+      <c r="F51" s="6" t="s">
         <v>2080</v>
-      </c>
-      <c r="B51" t="s">
-        <v>2234</v>
-      </c>
-      <c r="F51" s="6" t="s">
-        <v>2081</v>
       </c>
       <c r="G51" s="6"/>
     </row>
     <row r="54" spans="1:13">
       <c r="A54" s="6" t="s">
+        <v>2058</v>
+      </c>
+      <c r="B54" t="s">
+        <v>2234</v>
+      </c>
+      <c r="D54" s="6" t="s">
         <v>2059</v>
       </c>
-      <c r="B54" t="s">
-        <v>2235</v>
-      </c>
-      <c r="D54" s="6" t="s">
-        <v>2060</v>
-      </c>
       <c r="M54" t="s">
-        <v>2194</v>
+        <v>2193</v>
       </c>
     </row>
     <row r="56" spans="1:13">
       <c r="A56" s="6" t="s">
+        <v>2062</v>
+      </c>
+      <c r="B56" t="s">
+        <v>2235</v>
+      </c>
+      <c r="D56" s="6" t="s">
         <v>2063</v>
-      </c>
-      <c r="B56" t="s">
-        <v>2236</v>
-      </c>
-      <c r="D56" s="6" t="s">
-        <v>2064</v>
       </c>
     </row>
     <row r="58" spans="1:13">
       <c r="A58" s="6" t="s">
-        <v>2095</v>
+        <v>2094</v>
       </c>
       <c r="B58" t="s">
-        <v>2237</v>
+        <v>2236</v>
       </c>
       <c r="F58" t="s">
         <v>34</v>
       </c>
       <c r="M58" t="s">
-        <v>2201</v>
+        <v>2200</v>
       </c>
     </row>
     <row r="60" spans="1:13">
       <c r="A60" s="6" t="s">
+        <v>2040</v>
+      </c>
+      <c r="B60" t="s">
+        <v>2237</v>
+      </c>
+      <c r="D60" s="6" t="s">
         <v>2041</v>
-      </c>
-      <c r="B60" t="s">
-        <v>2238</v>
-      </c>
-      <c r="D60" s="6" t="s">
-        <v>2042</v>
       </c>
     </row>
     <row r="61" spans="1:13">
       <c r="A61" s="6" t="s">
+        <v>2042</v>
+      </c>
+      <c r="B61" t="s">
+        <v>2238</v>
+      </c>
+      <c r="D61" s="6" t="s">
         <v>2043</v>
-      </c>
-      <c r="B61" t="s">
-        <v>2239</v>
-      </c>
-      <c r="D61" s="6" t="s">
-        <v>2044</v>
       </c>
     </row>
     <row r="62" spans="1:13">
       <c r="A62" s="6" t="s">
+        <v>2044</v>
+      </c>
+      <c r="B62" t="s">
+        <v>2239</v>
+      </c>
+      <c r="D62" s="6" t="s">
         <v>2045</v>
-      </c>
-      <c r="B62" t="s">
-        <v>2240</v>
-      </c>
-      <c r="D62" s="6" t="s">
-        <v>2046</v>
       </c>
     </row>
     <row r="63" spans="1:13">
       <c r="A63" s="6" t="s">
+        <v>2046</v>
+      </c>
+      <c r="B63" t="s">
+        <v>2240</v>
+      </c>
+      <c r="D63" s="6" t="s">
         <v>2047</v>
-      </c>
-      <c r="B63" t="s">
-        <v>2241</v>
-      </c>
-      <c r="D63" s="6" t="s">
-        <v>2048</v>
       </c>
     </row>
     <row r="64" spans="1:13">
       <c r="A64" s="6" t="s">
+        <v>2048</v>
+      </c>
+      <c r="B64" t="s">
+        <v>2241</v>
+      </c>
+      <c r="D64" s="6" t="s">
         <v>2049</v>
-      </c>
-      <c r="B64" t="s">
-        <v>2242</v>
-      </c>
-      <c r="D64" s="6" t="s">
-        <v>2050</v>
       </c>
     </row>
     <row r="66" spans="1:13">
       <c r="A66" s="6" t="s">
+        <v>2084</v>
+      </c>
+      <c r="B66" t="s">
+        <v>2242</v>
+      </c>
+      <c r="D66" s="6" t="s">
         <v>2085</v>
       </c>
-      <c r="B66" t="s">
-        <v>2243</v>
-      </c>
-      <c r="D66" s="6" t="s">
-        <v>2086</v>
-      </c>
       <c r="F66" t="s">
-        <v>2089</v>
+        <v>2088</v>
       </c>
       <c r="I66" t="s">
-        <v>2124</v>
+        <v>2123</v>
       </c>
       <c r="K66" t="s">
-        <v>2160</v>
+        <v>2159</v>
       </c>
       <c r="M66" t="s">
-        <v>2211</v>
+        <v>2210</v>
       </c>
     </row>
     <row r="67" spans="1:13">
       <c r="A67" s="6" t="s">
+        <v>2086</v>
+      </c>
+      <c r="B67" t="s">
+        <v>2243</v>
+      </c>
+      <c r="D67" s="6" t="s">
         <v>2087</v>
       </c>
-      <c r="B67" t="s">
-        <v>2244</v>
-      </c>
-      <c r="D67" s="6" t="s">
-        <v>2088</v>
-      </c>
       <c r="F67" t="s">
-        <v>2090</v>
+        <v>2089</v>
       </c>
       <c r="I67" t="s">
-        <v>2123</v>
+        <v>2122</v>
       </c>
       <c r="K67" t="s">
-        <v>2159</v>
+        <v>2158</v>
       </c>
       <c r="M67" t="s">
-        <v>2212</v>
+        <v>2211</v>
       </c>
     </row>
     <row r="69" spans="1:13">
       <c r="A69" s="6" t="s">
-        <v>2136</v>
+        <v>2135</v>
       </c>
       <c r="B69" t="s">
         <v>205</v>
       </c>
       <c r="D69" s="6" t="s">
-        <v>2175</v>
+        <v>2174</v>
       </c>
       <c r="F69" s="6" t="s">
-        <v>2168</v>
+        <v>2167</v>
       </c>
       <c r="G69" s="6"/>
       <c r="I69" s="6" t="s">
-        <v>2161</v>
+        <v>2160</v>
       </c>
       <c r="K69" s="6" t="s">
-        <v>2146</v>
+        <v>2145</v>
       </c>
       <c r="M69" s="6" t="s">
-        <v>2213</v>
+        <v>2212</v>
       </c>
     </row>
     <row r="70" spans="1:13">
       <c r="A70" s="6" t="s">
-        <v>2137</v>
+        <v>2136</v>
       </c>
       <c r="B70" t="s">
         <v>207</v>
       </c>
       <c r="D70" s="6" t="s">
-        <v>2176</v>
+        <v>2175</v>
       </c>
       <c r="F70" s="6" t="s">
-        <v>2169</v>
+        <v>2168</v>
       </c>
       <c r="G70" s="6"/>
       <c r="I70" s="6" t="s">
-        <v>2162</v>
+        <v>2161</v>
       </c>
       <c r="K70" s="6" t="s">
-        <v>2147</v>
+        <v>2146</v>
       </c>
       <c r="M70" s="6" t="s">
-        <v>2214</v>
+        <v>2213</v>
       </c>
     </row>
     <row r="71" spans="1:13">
       <c r="A71" s="6" t="s">
-        <v>2138</v>
+        <v>2137</v>
       </c>
       <c r="B71" t="s">
         <v>206</v>
       </c>
       <c r="D71" s="6" t="s">
-        <v>2177</v>
+        <v>2176</v>
       </c>
       <c r="F71" s="6" t="s">
-        <v>2170</v>
+        <v>2169</v>
       </c>
       <c r="G71" s="6"/>
       <c r="I71" s="6" t="s">
-        <v>2163</v>
+        <v>2162</v>
       </c>
       <c r="K71" s="6" t="s">
-        <v>2142</v>
+        <v>2141</v>
       </c>
       <c r="M71" s="6" t="s">
-        <v>2215</v>
+        <v>2214</v>
       </c>
     </row>
     <row r="72" spans="1:13">
       <c r="A72" s="6" t="s">
-        <v>2139</v>
+        <v>2138</v>
       </c>
       <c r="B72" t="s">
         <v>208</v>
       </c>
       <c r="D72" s="6" t="s">
-        <v>2178</v>
+        <v>2177</v>
       </c>
       <c r="F72" s="6" t="s">
-        <v>2171</v>
+        <v>2170</v>
       </c>
       <c r="G72" s="6"/>
       <c r="I72" s="6" t="s">
-        <v>2164</v>
+        <v>2163</v>
       </c>
       <c r="K72" s="6" t="s">
-        <v>2143</v>
+        <v>2142</v>
       </c>
       <c r="M72" s="6" t="s">
-        <v>2216</v>
+        <v>2215</v>
       </c>
     </row>
     <row r="73" spans="1:13">
       <c r="A73" s="6" t="s">
-        <v>2140</v>
+        <v>2139</v>
       </c>
       <c r="B73" t="s">
         <v>644</v>
       </c>
       <c r="D73" s="6" t="s">
-        <v>2179</v>
+        <v>2178</v>
       </c>
       <c r="F73" s="6" t="s">
-        <v>2172</v>
+        <v>2171</v>
       </c>
       <c r="G73" s="6"/>
       <c r="I73" s="6" t="s">
-        <v>2165</v>
+        <v>2164</v>
       </c>
       <c r="K73" s="6" t="s">
-        <v>2144</v>
+        <v>2143</v>
       </c>
       <c r="M73" s="6" t="s">
-        <v>2217</v>
+        <v>2216</v>
       </c>
     </row>
     <row r="74" spans="1:13">
       <c r="A74" s="6" t="s">
-        <v>2141</v>
+        <v>2140</v>
       </c>
       <c r="B74" t="s">
         <v>645</v>
       </c>
       <c r="D74" s="6" t="s">
-        <v>2180</v>
+        <v>2179</v>
       </c>
       <c r="F74" s="6" t="s">
-        <v>2173</v>
+        <v>2172</v>
       </c>
       <c r="G74" s="6"/>
       <c r="I74" s="6" t="s">
-        <v>2166</v>
+        <v>2165</v>
       </c>
       <c r="K74" s="6" t="s">
-        <v>2145</v>
+        <v>2144</v>
       </c>
       <c r="M74" s="6" t="s">
-        <v>2218</v>
+        <v>2217</v>
       </c>
     </row>
     <row r="76" spans="1:13">
       <c r="A76" s="6" t="s">
-        <v>2151</v>
+        <v>2150</v>
       </c>
       <c r="B76" t="s">
-        <v>1989</v>
+        <v>1988</v>
       </c>
       <c r="D76" s="6" t="s">
-        <v>2181</v>
+        <v>2180</v>
       </c>
       <c r="F76" s="6" t="s">
-        <v>2174</v>
+        <v>2173</v>
       </c>
       <c r="G76" s="6"/>
       <c r="I76" s="6" t="s">
-        <v>2167</v>
+        <v>2166</v>
       </c>
       <c r="K76" s="6" t="s">
-        <v>2152</v>
+        <v>2151</v>
       </c>
       <c r="M76" s="6" t="s">
-        <v>2219</v>
+        <v>2218</v>
       </c>
     </row>
   </sheetData>
@@ -13803,10 +13800,10 @@
   <dimension ref="A1:BE165"/>
   <sheetViews>
     <sheetView zoomScale="125" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="AM17" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="AH2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A33" sqref="A33:XFD33"/>
+      <selection pane="bottomRight" activeCell="AV7" sqref="AV7:AV8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -14247,6 +14244,15 @@
       </c>
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
+      <c r="L7" s="6" t="s">
+        <v>431</v>
+      </c>
+      <c r="AD7" s="6" t="s">
+        <v>1013</v>
+      </c>
+      <c r="AV7" s="6" t="s">
+        <v>1013</v>
+      </c>
     </row>
     <row r="8" spans="1:57">
       <c r="A8" t="s">
@@ -14261,6 +14267,15 @@
       </c>
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
+      <c r="L8" s="6" t="s">
+        <v>1013</v>
+      </c>
+      <c r="AD8" s="6" t="s">
+        <v>431</v>
+      </c>
+      <c r="AV8" s="6" t="s">
+        <v>431</v>
+      </c>
     </row>
     <row r="9" spans="1:57">
       <c r="A9" t="s">
@@ -17948,11 +17963,11 @@
   </sheetPr>
   <dimension ref="A1:CW103"/>
   <sheetViews>
-    <sheetView zoomScale="176" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C10" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="176" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="M2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="BR34" sqref="BR34"/>
+      <selection pane="bottomRight" activeCell="S7" sqref="S7:S8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -17986,7 +18001,7 @@
         <v>1534</v>
       </c>
       <c r="D1" t="s">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="E1" t="s">
         <v>1537</v>
@@ -18034,250 +18049,250 @@
         <v>1617</v>
       </c>
       <c r="T1" t="s">
-        <v>1621</v>
+        <v>1620</v>
       </c>
       <c r="U1" t="s">
-        <v>1627</v>
+        <v>1626</v>
       </c>
       <c r="V1" t="s">
-        <v>1630</v>
+        <v>1629</v>
       </c>
       <c r="W1" t="s">
-        <v>1632</v>
+        <v>1631</v>
       </c>
       <c r="X1" t="s">
-        <v>1644</v>
+        <v>1643</v>
       </c>
       <c r="Y1" t="s">
-        <v>1647</v>
+        <v>1646</v>
       </c>
       <c r="Z1" t="s">
-        <v>1650</v>
+        <v>1649</v>
       </c>
       <c r="AA1" s="23" t="s">
+        <v>1652</v>
+      </c>
+      <c r="AB1" t="s">
         <v>1653</v>
       </c>
-      <c r="AB1" t="s">
-        <v>1654</v>
-      </c>
       <c r="AC1" t="s">
+        <v>1657</v>
+      </c>
+      <c r="AD1" t="s">
         <v>1658</v>
       </c>
-      <c r="AD1" t="s">
-        <v>1659</v>
-      </c>
       <c r="AE1" t="s">
-        <v>1666</v>
+        <v>1665</v>
       </c>
       <c r="AF1" t="s">
-        <v>1670</v>
+        <v>1669</v>
       </c>
       <c r="AG1" t="s">
-        <v>1677</v>
+        <v>1676</v>
       </c>
       <c r="AH1" t="s">
-        <v>1683</v>
+        <v>1682</v>
       </c>
       <c r="AI1" t="s">
+        <v>1690</v>
+      </c>
+      <c r="AJ1" s="23" t="s">
         <v>1691</v>
       </c>
-      <c r="AJ1" s="23" t="s">
+      <c r="AK1" t="s">
         <v>1692</v>
       </c>
-      <c r="AK1" t="s">
-        <v>1693</v>
-      </c>
       <c r="AL1" t="s">
-        <v>1696</v>
+        <v>1695</v>
       </c>
       <c r="AM1" t="s">
-        <v>1698</v>
+        <v>1697</v>
       </c>
       <c r="AN1" t="s">
-        <v>1702</v>
+        <v>1701</v>
       </c>
       <c r="AO1" t="s">
-        <v>1710</v>
+        <v>1709</v>
       </c>
       <c r="AP1" t="s">
-        <v>1713</v>
+        <v>1712</v>
       </c>
       <c r="AQ1" t="s">
-        <v>1717</v>
+        <v>1716</v>
       </c>
       <c r="AR1" t="s">
-        <v>1720</v>
+        <v>1719</v>
       </c>
       <c r="AS1" s="23" t="s">
+        <v>1730</v>
+      </c>
+      <c r="AT1" t="s">
         <v>1731</v>
       </c>
-      <c r="AT1" t="s">
-        <v>1732</v>
-      </c>
       <c r="AU1" s="6" t="s">
+        <v>1794</v>
+      </c>
+      <c r="AV1" t="s">
+        <v>1734</v>
+      </c>
+      <c r="AW1" s="5" t="s">
+        <v>1736</v>
+      </c>
+      <c r="AX1" t="s">
+        <v>1748</v>
+      </c>
+      <c r="AY1" t="s">
+        <v>1755</v>
+      </c>
+      <c r="AZ1" t="s">
+        <v>1762</v>
+      </c>
+      <c r="BA1" t="s">
+        <v>1770</v>
+      </c>
+      <c r="BB1" t="s">
+        <v>1776</v>
+      </c>
+      <c r="BC1" t="s">
+        <v>1778</v>
+      </c>
+      <c r="BD1" t="s">
+        <v>1782</v>
+      </c>
+      <c r="BE1" s="23" t="s">
+        <v>1786</v>
+      </c>
+      <c r="BF1" t="s">
+        <v>1787</v>
+      </c>
+      <c r="BG1" t="s">
         <v>1795</v>
       </c>
-      <c r="AV1" t="s">
-        <v>1735</v>
-      </c>
-      <c r="AW1" s="5" t="s">
-        <v>1737</v>
-      </c>
-      <c r="AX1" t="s">
-        <v>1749</v>
-      </c>
-      <c r="AY1" t="s">
-        <v>1756</v>
-      </c>
-      <c r="AZ1" t="s">
-        <v>1763</v>
-      </c>
-      <c r="BA1" t="s">
-        <v>1771</v>
-      </c>
-      <c r="BB1" t="s">
-        <v>1777</v>
-      </c>
-      <c r="BC1" t="s">
-        <v>1779</v>
-      </c>
-      <c r="BD1" t="s">
-        <v>1783</v>
-      </c>
-      <c r="BE1" s="23" t="s">
-        <v>1787</v>
-      </c>
-      <c r="BF1" t="s">
-        <v>1788</v>
-      </c>
-      <c r="BG1" t="s">
-        <v>1796</v>
-      </c>
       <c r="BH1" t="s">
-        <v>1800</v>
+        <v>1799</v>
       </c>
       <c r="BI1" t="s">
-        <v>1805</v>
+        <v>1804</v>
       </c>
       <c r="BJ1" t="s">
-        <v>1807</v>
+        <v>1806</v>
       </c>
       <c r="BK1" t="s">
-        <v>1809</v>
+        <v>1808</v>
       </c>
       <c r="BL1" s="6" t="s">
-        <v>1815</v>
+        <v>1814</v>
       </c>
       <c r="BM1" t="s">
-        <v>1819</v>
+        <v>1818</v>
       </c>
       <c r="BN1" t="s">
-        <v>1821</v>
+        <v>1820</v>
       </c>
       <c r="BO1" s="23" t="s">
+        <v>1829</v>
+      </c>
+      <c r="BP1" t="s">
         <v>1830</v>
       </c>
-      <c r="BP1" t="s">
-        <v>1831</v>
-      </c>
       <c r="BQ1" t="s">
-        <v>1837</v>
+        <v>1836</v>
       </c>
       <c r="BR1" t="s">
-        <v>1839</v>
+        <v>1838</v>
       </c>
       <c r="BS1" t="s">
-        <v>1844</v>
+        <v>1843</v>
       </c>
       <c r="BT1" t="s">
-        <v>1851</v>
+        <v>1850</v>
       </c>
       <c r="BU1" t="s">
-        <v>1853</v>
+        <v>1852</v>
       </c>
       <c r="BV1" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="BW1" t="s">
-        <v>1860</v>
+        <v>1859</v>
       </c>
       <c r="BX1" t="s">
-        <v>1866</v>
+        <v>1865</v>
       </c>
       <c r="BY1" t="s">
-        <v>1873</v>
+        <v>1872</v>
       </c>
       <c r="BZ1" t="s">
-        <v>1877</v>
+        <v>1876</v>
       </c>
       <c r="CA1" s="23" t="s">
+        <v>1879</v>
+      </c>
+      <c r="CB1" t="s">
         <v>1880</v>
       </c>
-      <c r="CB1" t="s">
-        <v>1881</v>
-      </c>
       <c r="CC1" t="s">
-        <v>1886</v>
+        <v>1885</v>
       </c>
       <c r="CD1" t="s">
-        <v>1891</v>
+        <v>1890</v>
       </c>
       <c r="CE1" t="s">
-        <v>1893</v>
+        <v>1892</v>
       </c>
       <c r="CF1" t="s">
-        <v>1899</v>
+        <v>1898</v>
       </c>
       <c r="CG1" t="s">
-        <v>1906</v>
+        <v>1905</v>
       </c>
       <c r="CH1" t="s">
-        <v>1908</v>
+        <v>1907</v>
       </c>
       <c r="CI1" t="s">
-        <v>1912</v>
+        <v>1911</v>
       </c>
       <c r="CJ1" t="s">
-        <v>1917</v>
+        <v>1916</v>
       </c>
       <c r="CK1" t="s">
-        <v>1923</v>
+        <v>1922</v>
       </c>
       <c r="CL1" t="s">
-        <v>1926</v>
+        <v>1925</v>
       </c>
       <c r="CM1" s="23" t="s">
+        <v>1931</v>
+      </c>
+      <c r="CN1" t="s">
         <v>1932</v>
       </c>
-      <c r="CN1" t="s">
-        <v>1933</v>
-      </c>
       <c r="CO1" t="s">
-        <v>1938</v>
+        <v>1937</v>
       </c>
       <c r="CP1" t="s">
-        <v>1940</v>
+        <v>1939</v>
       </c>
       <c r="CQ1" t="s">
-        <v>1946</v>
+        <v>1945</v>
       </c>
       <c r="CR1" t="s">
-        <v>1953</v>
+        <v>1952</v>
       </c>
       <c r="CS1" t="s">
-        <v>1955</v>
+        <v>1954</v>
       </c>
       <c r="CT1" t="s">
-        <v>1957</v>
+        <v>1956</v>
       </c>
       <c r="CU1" t="s">
-        <v>1961</v>
+        <v>1960</v>
       </c>
       <c r="CV1" t="s">
-        <v>1967</v>
+        <v>1966</v>
       </c>
       <c r="CW1" t="s">
-        <v>1970</v>
+        <v>1969</v>
       </c>
     </row>
     <row r="2" spans="1:101">
@@ -18412,7 +18427,7 @@
         <v>1535</v>
       </c>
       <c r="AT3" t="s">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="AU3" t="s">
         <v>1535</v>
@@ -18445,7 +18460,7 @@
         <v>1535</v>
       </c>
       <c r="BF3" t="s">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="BG3" t="s">
         <v>1535</v>
@@ -18472,7 +18487,7 @@
         <v>1535</v>
       </c>
       <c r="BP3" t="s">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="BQ3" t="s">
         <v>1535</v>
@@ -18505,7 +18520,7 @@
         <v>1535</v>
       </c>
       <c r="CB3" t="s">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="CC3" t="s">
         <v>1535</v>
@@ -18592,25 +18607,25 @@
         <v>1610</v>
       </c>
       <c r="AB5" s="6" t="s">
-        <v>1655</v>
+        <v>1654</v>
       </c>
       <c r="AK5" t="s">
-        <v>1694</v>
+        <v>1693</v>
       </c>
       <c r="AT5" t="s">
-        <v>1733</v>
+        <v>1732</v>
       </c>
       <c r="BF5" t="s">
-        <v>1790</v>
+        <v>1789</v>
       </c>
       <c r="BP5" t="s">
-        <v>1832</v>
+        <v>1831</v>
       </c>
       <c r="CB5" t="s">
-        <v>1884</v>
+        <v>1883</v>
       </c>
       <c r="CN5" t="s">
-        <v>1934</v>
+        <v>1933</v>
       </c>
     </row>
     <row r="6" spans="1:101">
@@ -18628,25 +18643,25 @@
         <v>1618</v>
       </c>
       <c r="AC6" t="s">
-        <v>1657</v>
+        <v>1656</v>
       </c>
       <c r="AL6" t="s">
-        <v>1697</v>
+        <v>1696</v>
       </c>
       <c r="AV6" t="s">
-        <v>1736</v>
+        <v>1735</v>
       </c>
       <c r="BG6" t="s">
-        <v>1799</v>
+        <v>1798</v>
       </c>
       <c r="BQ6" s="6" t="s">
-        <v>1838</v>
+        <v>1837</v>
       </c>
       <c r="CD6" t="s">
-        <v>1892</v>
+        <v>1891</v>
       </c>
       <c r="CO6" s="6" t="s">
-        <v>1939</v>
+        <v>1938</v>
       </c>
     </row>
     <row r="7" spans="1:101">
@@ -18660,9 +18675,6 @@
       <c r="F7" t="s">
         <v>1540</v>
       </c>
-      <c r="S7" t="s">
-        <v>151</v>
-      </c>
     </row>
     <row r="8" spans="1:101">
       <c r="A8" s="18" t="s">
@@ -18675,9 +18687,6 @@
       <c r="F8" t="s">
         <v>1541</v>
       </c>
-      <c r="S8" t="s">
-        <v>1620</v>
-      </c>
     </row>
     <row r="9" spans="1:101">
       <c r="A9" s="18" t="s">
@@ -18724,28 +18733,28 @@
         <v>height</v>
       </c>
       <c r="W13" t="s">
-        <v>1633</v>
+        <v>1632</v>
       </c>
       <c r="AE13" t="s">
-        <v>1667</v>
+        <v>1666</v>
       </c>
       <c r="AM13" t="s">
-        <v>1699</v>
+        <v>1698</v>
       </c>
       <c r="AW13" t="s">
-        <v>1738</v>
+        <v>1737</v>
       </c>
       <c r="BH13" s="6" t="s">
-        <v>1801</v>
+        <v>1800</v>
       </c>
       <c r="BR13" s="6" t="s">
-        <v>1840</v>
+        <v>1839</v>
       </c>
       <c r="CE13" s="6" t="s">
-        <v>1894</v>
+        <v>1893</v>
       </c>
       <c r="CP13" s="6" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="14" spans="1:101">
@@ -18757,28 +18766,28 @@
         <v>weight</v>
       </c>
       <c r="W14" t="s">
-        <v>1634</v>
+        <v>1633</v>
       </c>
       <c r="AE14" t="s">
-        <v>1668</v>
+        <v>1667</v>
       </c>
       <c r="AM14" t="s">
-        <v>1700</v>
+        <v>1699</v>
       </c>
       <c r="AW14" s="6" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="BH14" s="6" t="s">
-        <v>1802</v>
+        <v>1801</v>
       </c>
       <c r="BR14" s="6" t="s">
-        <v>1841</v>
+        <v>1840</v>
       </c>
       <c r="CE14" s="6" t="s">
-        <v>1895</v>
+        <v>1894</v>
       </c>
       <c r="CP14" s="6" t="s">
-        <v>1942</v>
+        <v>1941</v>
       </c>
     </row>
     <row r="15" spans="1:101">
@@ -18793,28 +18802,28 @@
         <v>1570</v>
       </c>
       <c r="W15" t="s">
-        <v>1635</v>
+        <v>1634</v>
       </c>
       <c r="AE15" t="s">
-        <v>1669</v>
+        <v>1668</v>
       </c>
       <c r="AM15" t="s">
-        <v>1701</v>
+        <v>1700</v>
       </c>
       <c r="AW15" s="6" t="s">
-        <v>1741</v>
+        <v>1740</v>
       </c>
       <c r="BH15" s="6" t="s">
-        <v>1803</v>
+        <v>1802</v>
       </c>
       <c r="BR15" s="6" t="s">
-        <v>1842</v>
+        <v>1841</v>
       </c>
       <c r="CE15" s="6" t="s">
-        <v>1896</v>
+        <v>1895</v>
       </c>
       <c r="CP15" s="6" t="s">
-        <v>1943</v>
+        <v>1942</v>
       </c>
     </row>
     <row r="16" spans="1:101">
@@ -18844,31 +18853,31 @@
         <v>wc</v>
       </c>
       <c r="J18" t="s">
-        <v>1643</v>
+        <v>1642</v>
       </c>
       <c r="W18" s="6" t="s">
-        <v>1642</v>
+        <v>1641</v>
       </c>
       <c r="AE18" t="s">
-        <v>1746</v>
+        <v>1745</v>
       </c>
       <c r="AM18" t="s">
-        <v>1709</v>
+        <v>1708</v>
       </c>
       <c r="AW18" s="6" t="s">
-        <v>1740</v>
+        <v>1739</v>
       </c>
       <c r="BH18" s="6" t="s">
-        <v>1804</v>
+        <v>1803</v>
       </c>
       <c r="BR18" s="6" t="s">
-        <v>1843</v>
+        <v>1842</v>
       </c>
       <c r="CE18" s="6" t="s">
-        <v>1897</v>
+        <v>1896</v>
       </c>
       <c r="CP18" s="6" t="s">
-        <v>1944</v>
+        <v>1943</v>
       </c>
     </row>
     <row r="19" spans="1:100">
@@ -18880,13 +18889,13 @@
         <v>hba1c</v>
       </c>
       <c r="BT19" s="6" t="s">
-        <v>1852</v>
+        <v>1851</v>
       </c>
       <c r="CG19" s="6" t="s">
-        <v>1907</v>
+        <v>1906</v>
       </c>
       <c r="CR19" s="6" t="s">
-        <v>1954</v>
+        <v>1953</v>
       </c>
     </row>
     <row r="20" spans="1:100">
@@ -18898,19 +18907,19 @@
         <v>insulinf</v>
       </c>
       <c r="AZ20" s="6" t="s">
-        <v>1764</v>
+        <v>1763</v>
       </c>
       <c r="BI20" s="6" t="s">
-        <v>1806</v>
+        <v>1805</v>
       </c>
       <c r="BU20" s="6" t="s">
-        <v>1854</v>
+        <v>1853</v>
       </c>
       <c r="CH20" s="6" t="s">
-        <v>1909</v>
+        <v>1908</v>
       </c>
       <c r="CS20" s="6" t="s">
-        <v>1956</v>
+        <v>1955</v>
       </c>
     </row>
     <row r="21" spans="1:100">
@@ -18931,19 +18940,19 @@
         <v>glucosef</v>
       </c>
       <c r="AY22" s="6" t="s">
-        <v>1757</v>
+        <v>1756</v>
       </c>
       <c r="BJ22" s="6" t="s">
-        <v>1808</v>
+        <v>1807</v>
       </c>
       <c r="BV22" s="6" t="s">
-        <v>1858</v>
+        <v>1857</v>
       </c>
       <c r="CI22" s="6" t="s">
-        <v>1913</v>
+        <v>1912</v>
       </c>
       <c r="CT22" s="6" t="s">
-        <v>1958</v>
+        <v>1957</v>
       </c>
     </row>
     <row r="23" spans="1:100">
@@ -18964,16 +18973,16 @@
         <v>glucose2h</v>
       </c>
       <c r="AY24" s="6" t="s">
-        <v>1758</v>
+        <v>1757</v>
       </c>
       <c r="BV24" s="6" t="s">
-        <v>1859</v>
+        <v>1858</v>
       </c>
       <c r="CI24" s="6" t="s">
-        <v>1914</v>
+        <v>1913</v>
       </c>
       <c r="CT24" s="6" t="s">
-        <v>1959</v>
+        <v>1958</v>
       </c>
     </row>
     <row r="25" spans="1:100">
@@ -19007,25 +19016,25 @@
       </c>
       <c r="P27" s="6"/>
       <c r="AG27" s="6" t="s">
-        <v>1678</v>
+        <v>1677</v>
       </c>
       <c r="AR27" t="s">
-        <v>1721</v>
+        <v>1720</v>
       </c>
       <c r="BA27" s="6" t="s">
-        <v>1772</v>
+        <v>1771</v>
       </c>
       <c r="BK27" s="6" t="s">
-        <v>1810</v>
+        <v>1809</v>
       </c>
       <c r="BW27" s="6" t="s">
-        <v>1861</v>
+        <v>1860</v>
       </c>
       <c r="CJ27" s="6" t="s">
-        <v>1918</v>
+        <v>1917</v>
       </c>
       <c r="CU27" s="6" t="s">
-        <v>1962</v>
+        <v>1961</v>
       </c>
     </row>
     <row r="28" spans="1:100">
@@ -19041,25 +19050,25 @@
       </c>
       <c r="P28" s="6"/>
       <c r="AG28" s="6" t="s">
-        <v>1679</v>
+        <v>1678</v>
       </c>
       <c r="AR28" s="6" t="s">
-        <v>1724</v>
+        <v>1723</v>
       </c>
       <c r="BA28" s="6" t="s">
-        <v>1773</v>
+        <v>1772</v>
       </c>
       <c r="BK28" s="6" t="s">
-        <v>1812</v>
+        <v>1811</v>
       </c>
       <c r="BW28" s="6" t="s">
-        <v>1862</v>
+        <v>1861</v>
       </c>
       <c r="CJ28" s="6" t="s">
-        <v>1920</v>
+        <v>1919</v>
       </c>
       <c r="CU28" s="6" t="s">
-        <v>1963</v>
+        <v>1962</v>
       </c>
     </row>
     <row r="29" spans="1:100">
@@ -19075,25 +19084,25 @@
       </c>
       <c r="P29" s="6"/>
       <c r="AG29" s="6" t="s">
-        <v>1680</v>
+        <v>1679</v>
       </c>
       <c r="AR29" s="6" t="s">
-        <v>1723</v>
+        <v>1722</v>
       </c>
       <c r="BA29" s="6" t="s">
-        <v>1774</v>
+        <v>1773</v>
       </c>
       <c r="BK29" s="6" t="s">
-        <v>1811</v>
+        <v>1810</v>
       </c>
       <c r="BW29" s="6" t="s">
-        <v>1863</v>
+        <v>1862</v>
       </c>
       <c r="CJ29" s="6" t="s">
-        <v>1921</v>
+        <v>1920</v>
       </c>
       <c r="CU29" s="6" t="s">
-        <v>1964</v>
+        <v>1963</v>
       </c>
     </row>
     <row r="30" spans="1:100">
@@ -19105,25 +19114,25 @@
         <v>vldlc</v>
       </c>
       <c r="AG30" s="6" t="s">
-        <v>1681</v>
+        <v>1680</v>
       </c>
       <c r="AR30" s="6" t="s">
-        <v>1722</v>
+        <v>1721</v>
       </c>
       <c r="BA30" s="6" t="s">
-        <v>1775</v>
+        <v>1774</v>
       </c>
       <c r="BK30" s="6" t="s">
-        <v>1813</v>
+        <v>1812</v>
       </c>
       <c r="BW30" s="6" t="s">
-        <v>1864</v>
+        <v>1863</v>
       </c>
       <c r="CJ30" s="6" t="s">
-        <v>1919</v>
+        <v>1918</v>
       </c>
       <c r="CU30" s="6" t="s">
-        <v>1965</v>
+        <v>1964</v>
       </c>
     </row>
     <row r="31" spans="1:100">
@@ -19139,25 +19148,25 @@
       </c>
       <c r="P31" s="6"/>
       <c r="AG31" s="6" t="s">
-        <v>1682</v>
+        <v>1681</v>
       </c>
       <c r="AR31" s="6" t="s">
-        <v>1725</v>
+        <v>1724</v>
       </c>
       <c r="BA31" s="6" t="s">
-        <v>1776</v>
+        <v>1775</v>
       </c>
       <c r="BK31" s="6" t="s">
-        <v>1814</v>
+        <v>1813</v>
       </c>
       <c r="BW31" s="6" t="s">
-        <v>1865</v>
+        <v>1864</v>
       </c>
       <c r="CJ31" s="6" t="s">
-        <v>1922</v>
+        <v>1921</v>
       </c>
       <c r="CU31" s="6" t="s">
-        <v>1966</v>
+        <v>1965</v>
       </c>
     </row>
     <row r="32" spans="1:100">
@@ -19169,19 +19178,19 @@
         <v>serumcreatinine</v>
       </c>
       <c r="BB32" s="6" t="s">
-        <v>1778</v>
+        <v>1777</v>
       </c>
       <c r="BM32" s="6" t="s">
-        <v>1820</v>
+        <v>1819</v>
       </c>
       <c r="BX32" s="6" t="s">
-        <v>1867</v>
+        <v>1866</v>
       </c>
       <c r="CK32" s="6" t="s">
-        <v>1924</v>
+        <v>1923</v>
       </c>
       <c r="CV32" s="6" t="s">
-        <v>1968</v>
+        <v>1967</v>
       </c>
     </row>
     <row r="33" spans="1:101">
@@ -19193,19 +19202,19 @@
         <v>urinealbumin</v>
       </c>
       <c r="BC33" s="6" t="s">
-        <v>1781</v>
+        <v>1780</v>
       </c>
       <c r="BL33" s="6" t="s">
-        <v>1817</v>
+        <v>1816</v>
       </c>
       <c r="BY33" s="6" t="s">
-        <v>1874</v>
+        <v>1873</v>
       </c>
       <c r="CL33" s="6" t="s">
-        <v>1927</v>
+        <v>1926</v>
       </c>
       <c r="CW33" s="6" t="s">
-        <v>1972</v>
+        <v>1971</v>
       </c>
     </row>
     <row r="34" spans="1:101">
@@ -19217,19 +19226,19 @@
         <v>urinecreatinine</v>
       </c>
       <c r="BC34" s="6" t="s">
-        <v>1780</v>
+        <v>1779</v>
       </c>
       <c r="BL34" s="6" t="s">
-        <v>1816</v>
+        <v>1815</v>
       </c>
       <c r="BY34" s="6" t="s">
-        <v>1875</v>
+        <v>1874</v>
       </c>
       <c r="CL34" s="6" t="s">
-        <v>1928</v>
+        <v>1927</v>
       </c>
       <c r="CW34" s="6" t="s">
-        <v>1971</v>
+        <v>1970</v>
       </c>
     </row>
     <row r="35" spans="1:101">
@@ -19241,19 +19250,19 @@
         <v>uacr</v>
       </c>
       <c r="BC35" s="6" t="s">
-        <v>1782</v>
+        <v>1781</v>
       </c>
       <c r="BL35" s="6" t="s">
-        <v>1818</v>
+        <v>1817</v>
       </c>
       <c r="BY35" s="6" t="s">
-        <v>1876</v>
+        <v>1875</v>
       </c>
       <c r="CL35" s="6" t="s">
-        <v>1929</v>
+        <v>1928</v>
       </c>
       <c r="CW35" s="6" t="s">
-        <v>1973</v>
+        <v>1972</v>
       </c>
     </row>
     <row r="36" spans="1:101">
@@ -19265,13 +19274,13 @@
         <v>egfr</v>
       </c>
       <c r="BX36" s="6" t="s">
-        <v>1868</v>
+        <v>1867</v>
       </c>
       <c r="CK36" s="6" t="s">
-        <v>1925</v>
+        <v>1924</v>
       </c>
       <c r="CV36" s="6" t="s">
-        <v>1969</v>
+        <v>1968</v>
       </c>
     </row>
     <row r="37" spans="1:101">
@@ -19302,7 +19311,7 @@
         <v>1543</v>
       </c>
       <c r="B41" t="s">
-        <v>1976</v>
+        <v>1975</v>
       </c>
       <c r="F41" t="s">
         <v>1542</v>
@@ -19313,7 +19322,7 @@
         <v>1544</v>
       </c>
       <c r="B42" t="s">
-        <v>1977</v>
+        <v>1976</v>
       </c>
       <c r="E42" t="s">
         <v>625</v>
@@ -19324,7 +19333,7 @@
         <v>1545</v>
       </c>
       <c r="B43" t="s">
-        <v>1978</v>
+        <v>1977</v>
       </c>
       <c r="E43" t="s">
         <v>151</v>
@@ -19335,7 +19344,7 @@
         <v>1546</v>
       </c>
       <c r="B44" t="s">
-        <v>1979</v>
+        <v>1978</v>
       </c>
       <c r="F44" t="s">
         <v>1547</v>
@@ -19346,7 +19355,7 @@
         <v>1619</v>
       </c>
       <c r="B45" t="s">
-        <v>1980</v>
+        <v>1979</v>
       </c>
       <c r="S45" s="5" t="s">
         <v>1538</v>
@@ -19378,7 +19387,7 @@
         <v>1548</v>
       </c>
       <c r="B46" t="s">
-        <v>1981</v>
+        <v>1980</v>
       </c>
       <c r="F46" t="s">
         <v>1549</v>
@@ -19389,7 +19398,7 @@
         <v>1551</v>
       </c>
       <c r="B47" t="s">
-        <v>1982</v>
+        <v>1981</v>
       </c>
       <c r="G47" t="s">
         <v>1552</v>
@@ -19397,24 +19406,24 @@
     </row>
     <row r="48" spans="1:101">
       <c r="A48" t="s">
+        <v>1621</v>
+      </c>
+      <c r="B48" t="s">
+        <v>1982</v>
+      </c>
+      <c r="T48" t="s">
         <v>1622</v>
-      </c>
-      <c r="B48" t="s">
-        <v>1983</v>
-      </c>
-      <c r="T48" t="s">
-        <v>1623</v>
       </c>
     </row>
     <row r="49" spans="1:94">
       <c r="A49" t="s">
+        <v>1623</v>
+      </c>
+      <c r="B49" t="s">
+        <v>1983</v>
+      </c>
+      <c r="T49" t="s">
         <v>1624</v>
-      </c>
-      <c r="B49" t="s">
-        <v>1984</v>
-      </c>
-      <c r="T49" t="s">
-        <v>1625</v>
       </c>
     </row>
     <row r="50" spans="1:94">
@@ -19422,13 +19431,13 @@
         <v>1553</v>
       </c>
       <c r="B50" t="s">
-        <v>1985</v>
+        <v>1984</v>
       </c>
       <c r="G50" t="s">
         <v>1554</v>
       </c>
       <c r="T50" t="s">
-        <v>1626</v>
+        <v>1625</v>
       </c>
     </row>
     <row r="51" spans="1:94">
@@ -19436,24 +19445,24 @@
         <v>1556</v>
       </c>
       <c r="B51" t="s">
-        <v>1986</v>
+        <v>1985</v>
       </c>
       <c r="H51" t="s">
         <v>1557</v>
       </c>
       <c r="V51" t="s">
-        <v>1631</v>
+        <v>1630</v>
       </c>
     </row>
     <row r="52" spans="1:94">
       <c r="A52" t="s">
+        <v>1627</v>
+      </c>
+      <c r="B52" t="s">
+        <v>1986</v>
+      </c>
+      <c r="U52" t="s">
         <v>1628</v>
-      </c>
-      <c r="B52" t="s">
-        <v>1987</v>
-      </c>
-      <c r="U52" t="s">
-        <v>1629</v>
       </c>
     </row>
     <row r="53" spans="1:94">
@@ -19461,7 +19470,7 @@
         <v>1607</v>
       </c>
       <c r="B53" t="s">
-        <v>1988</v>
+        <v>1987</v>
       </c>
       <c r="E53" t="s">
         <v>1606</v>
@@ -19469,33 +19478,33 @@
     </row>
     <row r="54" spans="1:94">
       <c r="A54" s="6" t="s">
+        <v>1741</v>
+      </c>
+      <c r="B54" t="s">
+        <v>1988</v>
+      </c>
+      <c r="J54" t="s">
         <v>1742</v>
       </c>
-      <c r="B54" t="s">
-        <v>1989</v>
-      </c>
-      <c r="J54" t="s">
+      <c r="W54" t="s">
         <v>1743</v>
       </c>
-      <c r="W54" t="s">
+      <c r="AE54" t="s">
         <v>1744</v>
       </c>
-      <c r="AE54" t="s">
-        <v>1745</v>
-      </c>
       <c r="AM54" s="6" t="s">
+        <v>1746</v>
+      </c>
+      <c r="AW54" s="6" t="s">
         <v>1747</v>
-      </c>
-      <c r="AW54" s="6" t="s">
-        <v>1748</v>
       </c>
       <c r="BH54" s="25"/>
       <c r="BR54" s="26"/>
       <c r="CE54" s="6" t="s">
-        <v>1898</v>
+        <v>1897</v>
       </c>
       <c r="CP54" s="6" t="s">
-        <v>1945</v>
+        <v>1944</v>
       </c>
     </row>
     <row r="56" spans="1:94">
@@ -19503,7 +19512,7 @@
         <v>1560</v>
       </c>
       <c r="B56" t="s">
-        <v>1990</v>
+        <v>1989</v>
       </c>
       <c r="D56" t="s">
         <v>1559</v>
@@ -19520,76 +19529,76 @@
         <v>1398</v>
       </c>
       <c r="P57" t="s">
-        <v>1664</v>
+        <v>1663</v>
       </c>
       <c r="R57" s="6"/>
       <c r="X57" s="5" t="s">
-        <v>1665</v>
+        <v>1664</v>
       </c>
       <c r="AB57" t="s">
-        <v>1656</v>
+        <v>1655</v>
       </c>
       <c r="AK57" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
       <c r="AT57" t="s">
-        <v>1734</v>
+        <v>1733</v>
       </c>
       <c r="BF57" s="6" t="s">
-        <v>1789</v>
+        <v>1788</v>
       </c>
       <c r="BP57" t="s">
-        <v>1833</v>
+        <v>1832</v>
       </c>
       <c r="CB57" t="s">
-        <v>1882</v>
+        <v>1881</v>
       </c>
       <c r="CN57" t="s">
-        <v>1936</v>
+        <v>1935</v>
       </c>
     </row>
     <row r="58" spans="1:94">
       <c r="A58" s="6" t="s">
-        <v>1797</v>
+        <v>1796</v>
       </c>
       <c r="B58" t="s">
-        <v>1991</v>
+        <v>1990</v>
       </c>
       <c r="R58" s="6"/>
       <c r="X58" s="5"/>
       <c r="BF58" s="6"/>
       <c r="BG58" s="6" t="s">
-        <v>1798</v>
+        <v>1797</v>
       </c>
       <c r="BP58" t="s">
-        <v>1834</v>
+        <v>1833</v>
       </c>
       <c r="CB58" t="s">
-        <v>1885</v>
+        <v>1884</v>
       </c>
       <c r="CN58" t="s">
-        <v>1935</v>
+        <v>1934</v>
       </c>
     </row>
     <row r="59" spans="1:94">
       <c r="A59" s="6" t="s">
-        <v>1835</v>
+        <v>1834</v>
       </c>
       <c r="B59" t="s">
-        <v>1992</v>
+        <v>1991</v>
       </c>
       <c r="R59" s="6"/>
       <c r="X59" s="5"/>
       <c r="BF59" s="6"/>
       <c r="BG59" s="6"/>
       <c r="BP59" t="s">
-        <v>1836</v>
+        <v>1835</v>
       </c>
       <c r="CB59" t="s">
-        <v>1883</v>
+        <v>1882</v>
       </c>
       <c r="CN59" t="s">
-        <v>1937</v>
+        <v>1936</v>
       </c>
     </row>
     <row r="60" spans="1:94">
@@ -19597,19 +19606,19 @@
         <v>1561</v>
       </c>
       <c r="B60" t="s">
-        <v>1995</v>
+        <v>1994</v>
       </c>
       <c r="I60" t="s">
         <v>1562</v>
       </c>
       <c r="AD60" s="6" t="s">
-        <v>1660</v>
+        <v>1659</v>
       </c>
       <c r="AU60" s="6" t="s">
-        <v>1791</v>
+        <v>1790</v>
       </c>
       <c r="CC60" s="6" t="s">
-        <v>1887</v>
+        <v>1886</v>
       </c>
     </row>
     <row r="61" spans="1:94">
@@ -19617,19 +19626,19 @@
         <v>1563</v>
       </c>
       <c r="B61" t="s">
-        <v>1996</v>
+        <v>1995</v>
       </c>
       <c r="I61" t="s">
         <v>1564</v>
       </c>
       <c r="AD61" s="6" t="s">
-        <v>1661</v>
+        <v>1660</v>
       </c>
       <c r="AU61" s="6" t="s">
-        <v>1792</v>
+        <v>1791</v>
       </c>
       <c r="CC61" s="6" t="s">
-        <v>1888</v>
+        <v>1887</v>
       </c>
     </row>
     <row r="62" spans="1:94">
@@ -19637,19 +19646,19 @@
         <v>1565</v>
       </c>
       <c r="B62" t="s">
-        <v>1994</v>
+        <v>1993</v>
       </c>
       <c r="I62" t="s">
         <v>1566</v>
       </c>
       <c r="AD62" s="6" t="s">
-        <v>1662</v>
+        <v>1661</v>
       </c>
       <c r="AU62" s="6" t="s">
-        <v>1793</v>
+        <v>1792</v>
       </c>
       <c r="CC62" s="6" t="s">
-        <v>1889</v>
+        <v>1888</v>
       </c>
     </row>
     <row r="63" spans="1:94">
@@ -19657,19 +19666,19 @@
         <v>1567</v>
       </c>
       <c r="B63" t="s">
-        <v>1993</v>
+        <v>1992</v>
       </c>
       <c r="I63" t="s">
         <v>1568</v>
       </c>
       <c r="AD63" s="6" t="s">
-        <v>1663</v>
+        <v>1662</v>
       </c>
       <c r="AU63" s="6" t="s">
-        <v>1794</v>
+        <v>1793</v>
       </c>
       <c r="CC63" s="6" t="s">
-        <v>1890</v>
+        <v>1889</v>
       </c>
     </row>
     <row r="65" spans="1:95">
@@ -19683,28 +19692,28 @@
         <v>1574</v>
       </c>
       <c r="U65" s="6" t="s">
-        <v>1636</v>
+        <v>1635</v>
       </c>
       <c r="AF65" s="6" t="s">
-        <v>1671</v>
+        <v>1670</v>
       </c>
       <c r="AN65" s="6" t="s">
-        <v>1703</v>
+        <v>1702</v>
       </c>
       <c r="AX65" s="6" t="s">
-        <v>1750</v>
+        <v>1749</v>
       </c>
       <c r="BN65" s="6" t="s">
-        <v>1822</v>
+        <v>1821</v>
       </c>
       <c r="BS65" s="6" t="s">
-        <v>1845</v>
+        <v>1844</v>
       </c>
       <c r="CF65" s="6" t="s">
-        <v>1900</v>
+        <v>1899</v>
       </c>
       <c r="CQ65" s="6" t="s">
-        <v>1947</v>
+        <v>1946</v>
       </c>
     </row>
     <row r="66" spans="1:95">
@@ -19718,28 +19727,28 @@
         <v>1575</v>
       </c>
       <c r="U66" s="6" t="s">
-        <v>1637</v>
+        <v>1636</v>
       </c>
       <c r="AF66" s="6" t="s">
-        <v>1672</v>
+        <v>1671</v>
       </c>
       <c r="AN66" s="6" t="s">
-        <v>1704</v>
+        <v>1703</v>
       </c>
       <c r="AX66" s="6" t="s">
-        <v>1751</v>
+        <v>1750</v>
       </c>
       <c r="BN66" s="6" t="s">
-        <v>1823</v>
+        <v>1822</v>
       </c>
       <c r="BS66" s="6" t="s">
-        <v>1846</v>
+        <v>1845</v>
       </c>
       <c r="CF66" s="6" t="s">
-        <v>1901</v>
+        <v>1900</v>
       </c>
       <c r="CQ66" s="6" t="s">
-        <v>1948</v>
+        <v>1947</v>
       </c>
     </row>
     <row r="67" spans="1:95">
@@ -19753,28 +19762,28 @@
         <v>1578</v>
       </c>
       <c r="U67" s="6" t="s">
-        <v>1638</v>
+        <v>1637</v>
       </c>
       <c r="AF67" s="6" t="s">
-        <v>1673</v>
+        <v>1672</v>
       </c>
       <c r="AN67" s="6" t="s">
-        <v>1705</v>
+        <v>1704</v>
       </c>
       <c r="AX67" s="6" t="s">
-        <v>1752</v>
+        <v>1751</v>
       </c>
       <c r="BN67" s="6" t="s">
-        <v>1824</v>
+        <v>1823</v>
       </c>
       <c r="BS67" s="6" t="s">
-        <v>1847</v>
+        <v>1846</v>
       </c>
       <c r="CF67" s="6" t="s">
-        <v>1902</v>
+        <v>1901</v>
       </c>
       <c r="CQ67" s="6" t="s">
-        <v>1949</v>
+        <v>1948</v>
       </c>
     </row>
     <row r="68" spans="1:95">
@@ -19788,28 +19797,28 @@
         <v>1579</v>
       </c>
       <c r="U68" s="6" t="s">
-        <v>1639</v>
+        <v>1638</v>
       </c>
       <c r="AF68" s="6" t="s">
-        <v>1674</v>
+        <v>1673</v>
       </c>
       <c r="AN68" s="6" t="s">
-        <v>1706</v>
+        <v>1705</v>
       </c>
       <c r="AX68" s="6" t="s">
-        <v>1753</v>
+        <v>1752</v>
       </c>
       <c r="BN68" s="6" t="s">
-        <v>1825</v>
+        <v>1824</v>
       </c>
       <c r="BS68" s="6" t="s">
-        <v>1848</v>
+        <v>1847</v>
       </c>
       <c r="CF68" s="6" t="s">
-        <v>1903</v>
+        <v>1902</v>
       </c>
       <c r="CQ68" s="6" t="s">
-        <v>1950</v>
+        <v>1949</v>
       </c>
     </row>
     <row r="69" spans="1:95">
@@ -19823,28 +19832,28 @@
         <v>1582</v>
       </c>
       <c r="U69" s="6" t="s">
-        <v>1640</v>
+        <v>1639</v>
       </c>
       <c r="AF69" s="6" t="s">
-        <v>1675</v>
+        <v>1674</v>
       </c>
       <c r="AN69" s="6" t="s">
-        <v>1707</v>
+        <v>1706</v>
       </c>
       <c r="AX69" s="6" t="s">
-        <v>1754</v>
+        <v>1753</v>
       </c>
       <c r="BN69" s="6" t="s">
-        <v>1826</v>
+        <v>1825</v>
       </c>
       <c r="BS69" s="6" t="s">
-        <v>1849</v>
+        <v>1848</v>
       </c>
       <c r="CF69" s="6" t="s">
-        <v>1904</v>
+        <v>1903</v>
       </c>
       <c r="CQ69" s="6" t="s">
-        <v>1951</v>
+        <v>1950</v>
       </c>
     </row>
     <row r="70" spans="1:95">
@@ -19858,28 +19867,28 @@
         <v>1583</v>
       </c>
       <c r="U70" s="6" t="s">
-        <v>1641</v>
+        <v>1640</v>
       </c>
       <c r="AF70" s="6" t="s">
-        <v>1676</v>
+        <v>1675</v>
       </c>
       <c r="AN70" s="6" t="s">
-        <v>1708</v>
+        <v>1707</v>
       </c>
       <c r="AX70" s="6" t="s">
-        <v>1755</v>
+        <v>1754</v>
       </c>
       <c r="BN70" s="6" t="s">
-        <v>1827</v>
+        <v>1826</v>
       </c>
       <c r="BS70" s="6" t="s">
-        <v>1850</v>
+        <v>1849</v>
       </c>
       <c r="CF70" s="6" t="s">
-        <v>1905</v>
+        <v>1904</v>
       </c>
       <c r="CQ70" s="6" t="s">
-        <v>1952</v>
+        <v>1951</v>
       </c>
     </row>
     <row r="74" spans="1:95">
@@ -19893,65 +19902,65 @@
         <v>1585</v>
       </c>
       <c r="AO74" t="s">
-        <v>1711</v>
+        <v>1710</v>
       </c>
     </row>
     <row r="75" spans="1:95">
       <c r="A75" s="6" t="s">
-        <v>1765</v>
+        <v>1764</v>
       </c>
       <c r="B75" t="s">
-        <v>1997</v>
+        <v>1996</v>
       </c>
       <c r="AZ75" s="6" t="s">
-        <v>1768</v>
+        <v>1767</v>
       </c>
     </row>
     <row r="76" spans="1:95">
       <c r="A76" s="6" t="s">
-        <v>1766</v>
+        <v>1765</v>
       </c>
       <c r="B76" t="s">
-        <v>1998</v>
+        <v>1997</v>
       </c>
       <c r="AZ76" s="6" t="s">
-        <v>1769</v>
+        <v>1768</v>
       </c>
     </row>
     <row r="77" spans="1:95">
       <c r="A77" s="6" t="s">
-        <v>1767</v>
+        <v>1766</v>
       </c>
       <c r="B77" t="s">
-        <v>1999</v>
+        <v>1998</v>
       </c>
       <c r="AZ77" s="6" t="s">
-        <v>1770</v>
+        <v>1769</v>
       </c>
     </row>
     <row r="78" spans="1:95">
       <c r="A78" s="6" t="s">
-        <v>1855</v>
+        <v>1854</v>
       </c>
       <c r="B78" t="s">
-        <v>2000</v>
+        <v>1999</v>
       </c>
       <c r="AZ78" s="6"/>
       <c r="BU78" s="6" t="s">
-        <v>1856</v>
+        <v>1855</v>
       </c>
     </row>
     <row r="79" spans="1:95">
       <c r="A79" s="6" t="s">
-        <v>1910</v>
+        <v>1909</v>
       </c>
       <c r="B79" t="s">
-        <v>2001</v>
+        <v>2000</v>
       </c>
       <c r="AZ79" s="6"/>
       <c r="BU79" s="6"/>
       <c r="CH79" s="6" t="s">
-        <v>1911</v>
+        <v>1910</v>
       </c>
     </row>
     <row r="80" spans="1:95">
@@ -19959,27 +19968,27 @@
         <v>1589</v>
       </c>
       <c r="B80" t="s">
-        <v>2002</v>
+        <v>2001</v>
       </c>
       <c r="M80" t="s">
         <v>1588</v>
       </c>
       <c r="AP80" t="s">
-        <v>1712</v>
+        <v>1711</v>
       </c>
     </row>
     <row r="81" spans="1:98">
       <c r="A81" s="6" t="s">
-        <v>1715</v>
+        <v>1714</v>
       </c>
       <c r="B81" t="s">
         <v>1528</v>
       </c>
       <c r="M81" t="s">
-        <v>1716</v>
+        <v>1715</v>
       </c>
       <c r="AP81" s="6" t="s">
-        <v>1714</v>
+        <v>1713</v>
       </c>
     </row>
     <row r="82" spans="1:98">
@@ -19987,7 +19996,7 @@
         <v>1591</v>
       </c>
       <c r="B82" t="s">
-        <v>2003</v>
+        <v>2002</v>
       </c>
       <c r="N82" s="6" t="s">
         <v>1592</v>
@@ -19995,51 +20004,51 @@
     </row>
     <row r="83" spans="1:98">
       <c r="A83" s="6" t="s">
+        <v>1717</v>
+      </c>
+      <c r="B83" t="s">
+        <v>2003</v>
+      </c>
+      <c r="AQ83" s="6" t="s">
         <v>1718</v>
-      </c>
-      <c r="B83" t="s">
-        <v>2004</v>
-      </c>
-      <c r="AQ83" s="6" t="s">
-        <v>1719</v>
       </c>
     </row>
     <row r="84" spans="1:98">
       <c r="A84" s="6" t="s">
-        <v>1759</v>
+        <v>1758</v>
       </c>
       <c r="B84" t="s">
-        <v>2005</v>
+        <v>2004</v>
       </c>
       <c r="AQ84" s="6"/>
       <c r="AY84" s="6" t="s">
-        <v>1761</v>
+        <v>1760</v>
       </c>
     </row>
     <row r="85" spans="1:98">
       <c r="A85" s="6" t="s">
-        <v>1760</v>
+        <v>1759</v>
       </c>
       <c r="B85" t="s">
-        <v>2006</v>
+        <v>2005</v>
       </c>
       <c r="AQ85" s="6"/>
       <c r="AY85" s="6" t="s">
-        <v>1762</v>
+        <v>1761</v>
       </c>
     </row>
     <row r="86" spans="1:98">
       <c r="A86" s="6" t="s">
+        <v>1914</v>
+      </c>
+      <c r="B86" t="s">
+        <v>2006</v>
+      </c>
+      <c r="CI86" s="6" t="s">
         <v>1915</v>
       </c>
-      <c r="B86" t="s">
-        <v>2007</v>
-      </c>
-      <c r="CI86" s="6" t="s">
-        <v>1916</v>
-      </c>
       <c r="CT86" s="6" t="s">
-        <v>1960</v>
+        <v>1959</v>
       </c>
     </row>
     <row r="89" spans="1:98">
@@ -20066,10 +20075,10 @@
       </c>
       <c r="P90" s="6"/>
       <c r="AI90" s="6" t="s">
-        <v>1690</v>
+        <v>1689</v>
       </c>
       <c r="BD90" t="s">
-        <v>1784</v>
+        <v>1783</v>
       </c>
     </row>
     <row r="91" spans="1:98">
@@ -20077,7 +20086,7 @@
         <v>1602</v>
       </c>
       <c r="B91" t="s">
-        <v>2008</v>
+        <v>2007</v>
       </c>
       <c r="N91" s="6" t="s">
         <v>1603</v>
@@ -20088,7 +20097,7 @@
         <v>1604</v>
       </c>
       <c r="B92" t="s">
-        <v>2009</v>
+        <v>2008</v>
       </c>
       <c r="N92" s="6" t="s">
         <v>1605</v>
@@ -20096,57 +20105,57 @@
     </row>
     <row r="93" spans="1:98">
       <c r="A93" s="6" t="s">
-        <v>1684</v>
+        <v>1683</v>
       </c>
       <c r="B93" t="s">
-        <v>2010</v>
+        <v>2009</v>
       </c>
       <c r="AH93" s="6" t="s">
-        <v>1687</v>
+        <v>1686</v>
       </c>
     </row>
     <row r="94" spans="1:98">
       <c r="A94" s="6" t="s">
-        <v>1685</v>
+        <v>1684</v>
       </c>
       <c r="B94" t="s">
-        <v>2011</v>
+        <v>2010</v>
       </c>
       <c r="AH94" s="6" t="s">
-        <v>1688</v>
+        <v>1687</v>
       </c>
     </row>
     <row r="95" spans="1:98">
       <c r="A95" s="6" t="s">
-        <v>1686</v>
+        <v>1685</v>
       </c>
       <c r="B95" t="s">
-        <v>2012</v>
+        <v>2011</v>
       </c>
       <c r="AH95" s="6" t="s">
-        <v>1689</v>
+        <v>1688</v>
       </c>
     </row>
     <row r="96" spans="1:98">
       <c r="A96" s="6" t="s">
-        <v>1869</v>
+        <v>1868</v>
       </c>
       <c r="B96" t="s">
-        <v>2013</v>
+        <v>2012</v>
       </c>
       <c r="BX96" s="6" t="s">
-        <v>1871</v>
+        <v>1870</v>
       </c>
     </row>
     <row r="97" spans="1:92">
       <c r="A97" s="6" t="s">
-        <v>1870</v>
+        <v>1869</v>
       </c>
       <c r="B97" t="s">
-        <v>2014</v>
+        <v>2013</v>
       </c>
       <c r="BX97" s="6" t="s">
-        <v>1872</v>
+        <v>1871</v>
       </c>
     </row>
     <row r="99" spans="1:92">
@@ -20154,13 +20163,13 @@
         <v>1613</v>
       </c>
       <c r="B99" t="s">
-        <v>2015</v>
+        <v>2014</v>
       </c>
       <c r="P99" s="6" t="s">
         <v>1614</v>
       </c>
       <c r="X99" t="s">
-        <v>1645</v>
+        <v>1644</v>
       </c>
     </row>
     <row r="100" spans="1:92">
@@ -20168,85 +20177,85 @@
         <v>1615</v>
       </c>
       <c r="B100" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="P100" s="6" t="s">
         <v>1616</v>
       </c>
       <c r="X100" t="s">
-        <v>1646</v>
+        <v>1645</v>
       </c>
     </row>
     <row r="101" spans="1:92">
       <c r="A101" s="6" t="s">
+        <v>1647</v>
+      </c>
+      <c r="B101" t="s">
+        <v>2016</v>
+      </c>
+      <c r="Y101" s="6" t="s">
         <v>1648</v>
-      </c>
-      <c r="B101" t="s">
-        <v>2017</v>
-      </c>
-      <c r="Y101" s="6" t="s">
-        <v>1649</v>
       </c>
     </row>
     <row r="102" spans="1:92">
       <c r="A102" s="6" t="s">
+        <v>1650</v>
+      </c>
+      <c r="B102" t="s">
+        <v>2017</v>
+      </c>
+      <c r="Z102" s="6" t="s">
         <v>1651</v>
       </c>
-      <c r="B102" t="s">
-        <v>2018</v>
-      </c>
-      <c r="Z102" s="6" t="s">
-        <v>1652</v>
-      </c>
       <c r="AB102" t="s">
-        <v>1730</v>
+        <v>1729</v>
       </c>
       <c r="AK102" t="s">
-        <v>1726</v>
+        <v>1725</v>
       </c>
       <c r="AT102" t="s">
-        <v>1785</v>
+        <v>1784</v>
       </c>
       <c r="BF102" t="s">
-        <v>1828</v>
+        <v>1827</v>
       </c>
       <c r="BZ102" s="6" t="s">
-        <v>1878</v>
+        <v>1877</v>
       </c>
       <c r="CB102" t="s">
-        <v>1931</v>
+        <v>1930</v>
       </c>
       <c r="CN102" t="s">
-        <v>1975</v>
+        <v>1974</v>
       </c>
     </row>
     <row r="103" spans="1:92">
       <c r="A103" s="6" t="s">
+        <v>1726</v>
+      </c>
+      <c r="B103" t="s">
+        <v>2018</v>
+      </c>
+      <c r="AB103" t="s">
+        <v>1728</v>
+      </c>
+      <c r="AK103" t="s">
         <v>1727</v>
       </c>
-      <c r="B103" t="s">
-        <v>2019</v>
-      </c>
-      <c r="AB103" t="s">
-        <v>1729</v>
-      </c>
-      <c r="AK103" t="s">
-        <v>1728</v>
-      </c>
       <c r="AT103" t="s">
-        <v>1786</v>
+        <v>1785</v>
       </c>
       <c r="BF103" t="s">
-        <v>1829</v>
+        <v>1828</v>
       </c>
       <c r="BZ103" s="6" t="s">
-        <v>1879</v>
+        <v>1878</v>
       </c>
       <c r="CB103" t="s">
-        <v>1930</v>
+        <v>1929</v>
       </c>
       <c r="CN103" t="s">
-        <v>1974</v>
+        <v>1973</v>
       </c>
     </row>
   </sheetData>
@@ -20258,7 +20267,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{824997C4-ECFA-43DC-9501-1C6C5C097BCA}">
   <dimension ref="A1:U91"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+    <sheetView zoomScale="150" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C18" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -20815,7 +20824,7 @@
         <v>totalc</v>
       </c>
       <c r="E27" t="s">
-        <v>2249</v>
+        <v>2248</v>
       </c>
       <c r="L27" s="27"/>
       <c r="M27" s="27"/>
@@ -20897,7 +20906,7 @@
         <v>urinealbumin</v>
       </c>
       <c r="E33" t="s">
-        <v>2247</v>
+        <v>2246</v>
       </c>
     </row>
     <row r="34" spans="1:8">
@@ -20909,7 +20918,7 @@
         <v>urinecreatinine</v>
       </c>
       <c r="E34" t="s">
-        <v>2248</v>
+        <v>2247</v>
       </c>
     </row>
     <row r="35" spans="1:8">

</xml_diff>

<commit_message>
updated codes for cohen and elbow plots
</commit_message>
<xml_diff>
--- a/data/Phenotypes Variable List.xlsx
+++ b/data/Phenotypes Variable List.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10609"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="2222" documentId="13_ncr:1_{0AF53CB1-23E0-45A0-9003-9470A819876D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A5552DD7-E038-CF43-B4AF-58FD49FFAD91}"/>
+  <xr:revisionPtr revIDLastSave="2228" documentId="13_ncr:1_{0AF53CB1-23E0-45A0-9003-9470A819876D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ABD8E7B9-FB9B-1040-9816-7538BFA481F6}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17680" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17680" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Harmonized" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <sheet name="SEARCH" sheetId="9" r:id="rId11"/>
     <sheet name="TODAY" sheetId="10" r:id="rId12"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -7612,10 +7612,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -13799,11 +13795,11 @@
   </sheetPr>
   <dimension ref="A1:BE165"/>
   <sheetViews>
-    <sheetView zoomScale="125" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="AH2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="AT2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AV7" sqref="AV7:AV8"/>
+      <selection pane="bottomRight" activeCell="AV7" sqref="AV7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -14248,10 +14244,10 @@
         <v>431</v>
       </c>
       <c r="AD7" s="6" t="s">
-        <v>1013</v>
+        <v>431</v>
       </c>
       <c r="AV7" s="6" t="s">
-        <v>1013</v>
+        <v>431</v>
       </c>
     </row>
     <row r="8" spans="1:57">
@@ -14271,10 +14267,10 @@
         <v>1013</v>
       </c>
       <c r="AD8" s="6" t="s">
-        <v>431</v>
+        <v>1013</v>
       </c>
       <c r="AV8" s="6" t="s">
-        <v>431</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="9" spans="1:57">
@@ -17963,7 +17959,7 @@
   </sheetPr>
   <dimension ref="A1:CW103"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="176" workbookViewId="0">
+    <sheetView zoomScale="176" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="M2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>

</xml_diff>

<commit_message>
added medication for lipid
availble for now for ARIC, CARDIA and MESA
</commit_message>
<xml_diff>
--- a/data/Phenotypes Variable List.xlsx
+++ b/data/Phenotypes Variable List.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10811"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{737B7464-E1EB-4A48-967A-E9EF54A23B52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{620F84E1-9118-8B44-892D-83D017977405}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{737B7464-E1EB-4A48-967A-E9EF54A23B52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{894381F3-8508-5640-A8B7-DEF723E69685}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17760" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -8213,7 +8213,7 @@
   </sheetPr>
   <dimension ref="A1:M76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="156" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="156" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="A51" sqref="A51:XFD51"/>
     </sheetView>
@@ -13802,10 +13802,10 @@
   <dimension ref="A1:BE165"/>
   <sheetViews>
     <sheetView zoomScale="125" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="AL27" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C90" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A47" sqref="A47:XFD47"/>
+      <selection pane="bottomRight" activeCell="E101" sqref="E101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -17966,10 +17966,10 @@
   <dimension ref="A1:CW103"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="BY43" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="G76" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="CB57" sqref="CB57"/>
+      <selection pane="bottomRight" activeCell="B102" sqref="B102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -20270,10 +20270,10 @@
   <dimension ref="A1:U92"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C66" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F92" sqref="F92"/>
+      <selection pane="bottomRight" activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -21561,11 +21561,11 @@
   <dimension ref="A1:V88"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C67" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C10" activePane="bottomRight" state="frozen"/>
       <selection activeCell="E30" sqref="E30"/>
       <selection pane="topRight" activeCell="E30" sqref="E30"/>
       <selection pane="bottomLeft" activeCell="E30" sqref="E30"/>
-      <selection pane="bottomRight" activeCell="F88" sqref="F88"/>
+      <selection pane="bottomRight" activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -22747,10 +22747,10 @@
   <dimension ref="A1:X47"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C26" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D34" sqref="D34:H34"/>
+      <selection pane="bottomRight" activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Corrected 'RACEGRP' and 'GENDER' mapping for visit 5 and visit 6
</commit_message>
<xml_diff>
--- a/data/Phenotypes Variable List.xlsx
+++ b/data/Phenotypes Variable List.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{737B7464-E1EB-4A48-967A-E9EF54A23B52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{894381F3-8508-5640-A8B7-DEF723E69685}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCA6DE1B-8F2C-445A-B7D6-ACB5F687D830}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17760" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Harmonized" sheetId="2" r:id="rId1"/>
@@ -7887,11 +7887,11 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.36328125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" customWidth="1"/>
-    <col min="3" max="3" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -8213,25 +8213,25 @@
   </sheetPr>
   <dimension ref="A1:M76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="156" workbookViewId="0">
+    <sheetView topLeftCell="A44" zoomScale="119" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="A51" sqref="A51:XFD51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
     <col min="2" max="2" width="20" customWidth="1"/>
-    <col min="3" max="3" width="2.33203125" style="23" customWidth="1"/>
-    <col min="4" max="4" width="21.1640625" customWidth="1"/>
-    <col min="5" max="5" width="2.1640625" style="23" customWidth="1"/>
-    <col min="6" max="7" width="18.1640625" customWidth="1"/>
-    <col min="8" max="8" width="1.83203125" style="23" customWidth="1"/>
+    <col min="3" max="3" width="2.36328125" style="23" customWidth="1"/>
+    <col min="4" max="4" width="21.1796875" customWidth="1"/>
+    <col min="5" max="5" width="2.1796875" style="23" customWidth="1"/>
+    <col min="6" max="7" width="18.1796875" customWidth="1"/>
+    <col min="8" max="8" width="1.81640625" style="23" customWidth="1"/>
     <col min="9" max="9" width="18" customWidth="1"/>
-    <col min="10" max="10" width="2.1640625" style="23" customWidth="1"/>
-    <col min="11" max="11" width="17.6640625" customWidth="1"/>
-    <col min="12" max="12" width="2.33203125" style="23" customWidth="1"/>
-    <col min="13" max="13" width="21.83203125" customWidth="1"/>
+    <col min="10" max="10" width="2.1796875" style="23" customWidth="1"/>
+    <col min="11" max="11" width="17.6328125" customWidth="1"/>
+    <col min="12" max="12" width="2.36328125" style="23" customWidth="1"/>
+    <col min="13" max="13" width="21.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
@@ -9396,11 +9396,11 @@
       <selection pane="bottomRight" activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="69.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.1640625" customWidth="1"/>
-    <col min="3" max="3" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="69.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.1796875" customWidth="1"/>
+    <col min="3" max="3" width="18.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -11267,7 +11267,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="150" spans="1:4" ht="32">
+    <row r="150" spans="1:4" ht="29">
       <c r="A150" s="5" t="s">
         <v>913</v>
       </c>
@@ -11278,7 +11278,7 @@
         <v>932</v>
       </c>
     </row>
-    <row r="151" spans="1:4" ht="48">
+    <row r="151" spans="1:4" ht="43.5">
       <c r="A151" s="5" t="s">
         <v>914</v>
       </c>
@@ -11289,7 +11289,7 @@
         <v>933</v>
       </c>
     </row>
-    <row r="152" spans="1:4" ht="32">
+    <row r="152" spans="1:4" ht="29">
       <c r="A152" s="5" t="s">
         <v>915</v>
       </c>
@@ -11300,7 +11300,7 @@
         <v>934</v>
       </c>
     </row>
-    <row r="153" spans="1:4" ht="32">
+    <row r="153" spans="1:4" ht="29">
       <c r="A153" s="5" t="s">
         <v>916</v>
       </c>
@@ -11311,7 +11311,7 @@
         <v>935</v>
       </c>
     </row>
-    <row r="154" spans="1:4" ht="32">
+    <row r="154" spans="1:4" ht="29">
       <c r="A154" s="5" t="s">
         <v>917</v>
       </c>
@@ -11322,7 +11322,7 @@
         <v>936</v>
       </c>
     </row>
-    <row r="155" spans="1:4" ht="32">
+    <row r="155" spans="1:4" ht="29">
       <c r="A155" s="5" t="s">
         <v>888</v>
       </c>
@@ -11355,7 +11355,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="158" spans="1:4" ht="32">
+    <row r="158" spans="1:4" ht="29">
       <c r="A158" s="5" t="s">
         <v>897</v>
       </c>
@@ -11476,12 +11476,12 @@
       <selection pane="bottomRight" activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="98.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.5" customWidth="1"/>
-    <col min="5" max="5" width="14.5" customWidth="1"/>
+    <col min="1" max="1" width="98.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.453125" customWidth="1"/>
+    <col min="5" max="5" width="14.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -13019,13 +13019,13 @@
       <selection pane="bottomRight" activeCell="G43" sqref="G43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="26.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="7" width="14.5" customWidth="1"/>
+    <col min="1" max="1" width="26.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="7" width="14.453125" customWidth="1"/>
     <col min="8" max="8" width="13" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21">
@@ -13801,34 +13801,34 @@
   </sheetPr>
   <dimension ref="A1:BE165"/>
   <sheetViews>
-    <sheetView zoomScale="125" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C90" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="BE2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E101" sqref="E101"/>
+      <selection pane="bottomRight" activeCell="BN8" sqref="BN8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="22.83203125" customWidth="1"/>
+    <col min="1" max="1" width="22.81640625" customWidth="1"/>
     <col min="2" max="2" width="15" customWidth="1"/>
-    <col min="3" max="3" width="2.5" style="8" customWidth="1"/>
+    <col min="3" max="3" width="2.453125" style="8" customWidth="1"/>
     <col min="4" max="4" width="9" customWidth="1"/>
-    <col min="5" max="6" width="9.83203125" customWidth="1"/>
+    <col min="5" max="6" width="9.81640625" customWidth="1"/>
     <col min="7" max="7" width="8" customWidth="1"/>
-    <col min="11" max="11" width="2.33203125" style="8" customWidth="1"/>
-    <col min="12" max="12" width="11.1640625" customWidth="1"/>
-    <col min="18" max="18" width="7.1640625" customWidth="1"/>
-    <col min="19" max="19" width="2.83203125" style="8" customWidth="1"/>
-    <col min="21" max="21" width="10.83203125" customWidth="1"/>
-    <col min="22" max="22" width="9.6640625" customWidth="1"/>
+    <col min="11" max="11" width="2.36328125" style="8" customWidth="1"/>
+    <col min="12" max="12" width="11.1796875" customWidth="1"/>
+    <col min="18" max="18" width="7.1796875" customWidth="1"/>
+    <col min="19" max="19" width="2.81640625" style="8" customWidth="1"/>
+    <col min="21" max="21" width="10.81640625" customWidth="1"/>
+    <col min="22" max="22" width="9.6328125" customWidth="1"/>
     <col min="29" max="29" width="3" style="8" customWidth="1"/>
-    <col min="38" max="38" width="2.5" style="8" customWidth="1"/>
-    <col min="39" max="39" width="11.5" customWidth="1"/>
-    <col min="40" max="40" width="12.83203125" customWidth="1"/>
-    <col min="47" max="47" width="2.83203125" style="8" customWidth="1"/>
-    <col min="48" max="48" width="10.83203125" customWidth="1"/>
-    <col min="57" max="57" width="15.1640625" customWidth="1"/>
+    <col min="38" max="38" width="2.453125" style="8" customWidth="1"/>
+    <col min="39" max="39" width="11.453125" customWidth="1"/>
+    <col min="40" max="40" width="12.81640625" customWidth="1"/>
+    <col min="47" max="47" width="2.81640625" style="8" customWidth="1"/>
+    <col min="48" max="48" width="10.81640625" customWidth="1"/>
+    <col min="57" max="57" width="15.1796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:57">
@@ -14250,10 +14250,10 @@
         <v>431</v>
       </c>
       <c r="AD7" s="6" t="s">
-        <v>1005</v>
+        <v>431</v>
       </c>
       <c r="AV7" s="6" t="s">
-        <v>1005</v>
+        <v>431</v>
       </c>
     </row>
     <row r="8" spans="1:57">
@@ -14273,10 +14273,10 @@
         <v>1005</v>
       </c>
       <c r="AD8" s="6" t="s">
-        <v>431</v>
+        <v>1005</v>
       </c>
       <c r="AV8" s="6" t="s">
-        <v>431</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="9" spans="1:57">
@@ -14669,7 +14669,7 @@
         <v>1382</v>
       </c>
     </row>
-    <row r="32" spans="1:53" ht="16">
+    <row r="32" spans="1:53">
       <c r="A32" t="s">
         <v>24</v>
       </c>
@@ -14790,7 +14790,7 @@
         <v>1204</v>
       </c>
     </row>
-    <row r="46" spans="1:56" ht="16">
+    <row r="46" spans="1:56">
       <c r="A46" s="6" t="s">
         <v>1205</v>
       </c>
@@ -17081,9 +17081,9 @@
       <selection pane="topRight" activeCell="D67" sqref="D67"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="22.83203125" style="18" customWidth="1"/>
+    <col min="1" max="1" width="22.81640625" style="18" customWidth="1"/>
     <col min="2" max="2" width="15" customWidth="1"/>
     <col min="3" max="3" width="11" customWidth="1"/>
   </cols>
@@ -17972,27 +17972,27 @@
       <selection pane="bottomRight" activeCell="B102" sqref="B102"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="16.6640625" customWidth="1"/>
-    <col min="2" max="2" width="15.1640625" customWidth="1"/>
+    <col min="1" max="1" width="16.6328125" customWidth="1"/>
+    <col min="2" max="2" width="15.1796875" customWidth="1"/>
     <col min="3" max="3" width="3" style="23" customWidth="1"/>
-    <col min="6" max="6" width="10.5" customWidth="1"/>
-    <col min="7" max="7" width="9.83203125" customWidth="1"/>
-    <col min="8" max="8" width="10.1640625" customWidth="1"/>
-    <col min="17" max="17" width="2.83203125" style="23" customWidth="1"/>
-    <col min="18" max="18" width="9.33203125" customWidth="1"/>
-    <col min="27" max="27" width="2.1640625" style="23" customWidth="1"/>
-    <col min="28" max="28" width="9.83203125" customWidth="1"/>
-    <col min="36" max="36" width="2.6640625" style="23" customWidth="1"/>
-    <col min="45" max="45" width="3.1640625" style="23" customWidth="1"/>
+    <col min="6" max="6" width="10.453125" customWidth="1"/>
+    <col min="7" max="7" width="9.81640625" customWidth="1"/>
+    <col min="8" max="8" width="10.1796875" customWidth="1"/>
+    <col min="17" max="17" width="2.81640625" style="23" customWidth="1"/>
+    <col min="18" max="18" width="9.36328125" customWidth="1"/>
+    <col min="27" max="27" width="2.1796875" style="23" customWidth="1"/>
+    <col min="28" max="28" width="9.81640625" customWidth="1"/>
+    <col min="36" max="36" width="2.6328125" style="23" customWidth="1"/>
+    <col min="45" max="45" width="3.1796875" style="23" customWidth="1"/>
     <col min="57" max="57" width="3" style="23" customWidth="1"/>
-    <col min="67" max="67" width="2.6640625" style="23" customWidth="1"/>
+    <col min="67" max="67" width="2.6328125" style="23" customWidth="1"/>
     <col min="79" max="79" width="3" style="23" customWidth="1"/>
-    <col min="91" max="91" width="3.1640625" style="23" customWidth="1"/>
+    <col min="91" max="91" width="3.1796875" style="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:101" ht="16">
+    <row r="1" spans="1:101">
       <c r="A1" s="18" t="s">
         <v>124</v>
       </c>
@@ -19308,7 +19308,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="41" spans="1:101" ht="16">
+    <row r="41" spans="1:101">
       <c r="A41" s="24" t="s">
         <v>1535</v>
       </c>
@@ -19352,7 +19352,7 @@
         <v>1539</v>
       </c>
     </row>
-    <row r="45" spans="1:101" ht="16">
+    <row r="45" spans="1:101" ht="29">
       <c r="A45" t="s">
         <v>1611</v>
       </c>
@@ -19523,7 +19523,7 @@
         <v>1603</v>
       </c>
     </row>
-    <row r="57" spans="1:94" ht="16">
+    <row r="57" spans="1:94">
       <c r="A57" t="s">
         <v>385</v>
       </c>
@@ -20276,11 +20276,11 @@
       <selection pane="bottomRight" activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="26.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="14.5" customWidth="1"/>
+    <col min="1" max="1" width="26.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="14.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21">
@@ -21568,11 +21568,11 @@
       <selection pane="bottomRight" activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="26.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="14.5" customWidth="1"/>
+    <col min="1" max="1" width="26.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="14.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22">
@@ -22753,9 +22753,9 @@
       <selection pane="bottomRight" activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.36328125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -23551,12 +23551,12 @@
       <selection pane="bottomRight" activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="23.33203125" customWidth="1"/>
-    <col min="2" max="2" width="13.83203125" customWidth="1"/>
-    <col min="3" max="3" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.36328125" customWidth="1"/>
+    <col min="2" max="2" width="13.81640625" customWidth="1"/>
+    <col min="3" max="3" width="22.36328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20">

</xml_diff>